<commit_message>
Update automatico via Actualizar 06-09-2020 20-20-16
</commit_message>
<xml_diff>
--- a/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
+++ b/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID CL/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID CL/IndicadoresEconomicos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{96CF5CFE-59E2-49C5-A076-2B24390C2C1E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{80F393C9-2C1B-4224-A06A-82C852B96E95}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:1_{96CF5CFE-59E2-49C5-A076-2B24390C2C1E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{EF98311F-A37E-473F-A3FF-48B0EFF17CA2}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DOLAR_OBS_ADO" sheetId="1" r:id="rId1"/>
@@ -939,14 +939,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B528"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A503" workbookViewId="0">
-      <selection activeCell="B482" sqref="B482"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.88671875" customWidth="1"/>
-    <col min="2" max="2" width="15.5546875" customWidth="1"/>
+    <col min="1" max="1" width="11.5546875" customWidth="1"/>
+    <col min="2" max="2" width="15.88671875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -5174,5 +5174,6 @@
     <mergeCell ref="A1:B1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update automatico via Actualizar 07-11-2020 17-08-08
</commit_message>
<xml_diff>
--- a/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
+++ b/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/944d5b9328a00097/Proyectos/Data intelligence/Covid-19/Chile/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="10" documentId="114_{4E138255-E71E-4AEB-A9EF-82D3D6322094}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{AD956519-9444-461A-A298-61C12564A60D}"/>
+  <xr:revisionPtr revIDLastSave="11" documentId="114_{4E138255-E71E-4AEB-A9EF-82D3D6322094}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{351AD669-100F-462C-BE77-5AB794EE41E1}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5784" yWindow="0" windowWidth="17220" windowHeight="12960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DOLAR_OBS_ADO" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$559</definedName>
+    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$562</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="5">
   <si>
     <t>Tipos de cambio (pesos por dólar)</t>
   </si>
@@ -927,10 +927,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B559"/>
+  <dimension ref="A1:B562"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A542" workbookViewId="0">
-      <selection activeCell="B563" sqref="B563"/>
+      <selection activeCell="B565" sqref="B565"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5407,6 +5407,30 @@
         <v>781.74</v>
       </c>
     </row>
+    <row r="560" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A560" s="2">
+        <v>44023</v>
+      </c>
+      <c r="B560" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="561" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A561" s="2">
+        <v>44024</v>
+      </c>
+      <c r="B561" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="562" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A562" s="2">
+        <v>44025</v>
+      </c>
+      <c r="B562" s="3">
+        <v>790.82</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:B1"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 07-14-2020 17-05-09
</commit_message>
<xml_diff>
--- a/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
+++ b/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/944d5b9328a00097/Proyectos/Data intelligence/Covid-19/Chile/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="11" documentId="114_{4E138255-E71E-4AEB-A9EF-82D3D6322094}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{351AD669-100F-462C-BE77-5AB794EE41E1}"/>
+  <xr:revisionPtr revIDLastSave="12" documentId="114_{4E138255-E71E-4AEB-A9EF-82D3D6322094}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{F65BF3F7-8F0E-40F6-918B-3E80C1464272}"/>
   <bookViews>
-    <workbookView xWindow="5784" yWindow="0" windowWidth="17220" windowHeight="12960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5832" yWindow="0" windowWidth="17184" windowHeight="12960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DOLAR_OBS_ADO" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$562</definedName>
+    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$563</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
@@ -927,10 +927,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B562"/>
+  <dimension ref="A1:B563"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A542" workbookViewId="0">
-      <selection activeCell="B565" sqref="B565"/>
+      <selection activeCell="B566" sqref="B566"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5431,6 +5431,14 @@
         <v>790.82</v>
       </c>
     </row>
+    <row r="563" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A563" s="2">
+        <v>44026</v>
+      </c>
+      <c r="B563" s="3">
+        <v>788.22</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:B1"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 07-15-2020 17-05-52
</commit_message>
<xml_diff>
--- a/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
+++ b/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/944d5b9328a00097/Proyectos/Data intelligence/Covid-19/Chile/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="12" documentId="114_{4E138255-E71E-4AEB-A9EF-82D3D6322094}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{F65BF3F7-8F0E-40F6-918B-3E80C1464272}"/>
+  <xr:revisionPtr revIDLastSave="13" documentId="114_{4E138255-E71E-4AEB-A9EF-82D3D6322094}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{A7D020E8-15FE-4CB1-87CF-BC2CB80BE699}"/>
   <bookViews>
-    <workbookView xWindow="5832" yWindow="0" windowWidth="17184" windowHeight="12960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8568" yWindow="696" windowWidth="15144" windowHeight="12960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DOLAR_OBS_ADO" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$563</definedName>
+    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$564</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
@@ -927,7 +927,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B563"/>
+  <dimension ref="A1:B564"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A542" workbookViewId="0">
       <selection activeCell="B566" sqref="B566"/>
@@ -5439,6 +5439,14 @@
         <v>788.22</v>
       </c>
     </row>
+    <row r="564" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A564" s="2">
+        <v>44027</v>
+      </c>
+      <c r="B564" s="3">
+        <v>787.87</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:B1"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 07-17-2020 02-26-40
</commit_message>
<xml_diff>
--- a/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
+++ b/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/944d5b9328a00097/Proyectos/Data intelligence/Covid-19/Chile/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="13" documentId="114_{4E138255-E71E-4AEB-A9EF-82D3D6322094}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{A7D020E8-15FE-4CB1-87CF-BC2CB80BE699}"/>
+  <xr:revisionPtr revIDLastSave="14" documentId="114_{4E138255-E71E-4AEB-A9EF-82D3D6322094}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{E9FF7E26-29D1-4A48-B688-AB78C4EC9AE9}"/>
   <bookViews>
-    <workbookView xWindow="8568" yWindow="696" windowWidth="15144" windowHeight="12960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6468" yWindow="0" windowWidth="16524" windowHeight="12960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DOLAR_OBS_ADO" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$564</definedName>
+    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$566</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="5">
   <si>
     <t>Tipos de cambio (pesos por dólar)</t>
   </si>
@@ -927,10 +927,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B564"/>
+  <dimension ref="A1:B566"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A542" workbookViewId="0">
-      <selection activeCell="B566" sqref="B566"/>
+      <selection activeCell="B568" sqref="B568"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5447,6 +5447,22 @@
         <v>787.87</v>
       </c>
     </row>
+    <row r="565" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A565" s="2">
+        <v>44028</v>
+      </c>
+      <c r="B565" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="566" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A566" s="2">
+        <v>44029</v>
+      </c>
+      <c r="B566" s="3">
+        <v>787.5</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:B1"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 07-18-2020 17-05-16
</commit_message>
<xml_diff>
--- a/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
+++ b/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/944d5b9328a00097/Proyectos/Data intelligence/Covid-19/Chile/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="14" documentId="114_{4E138255-E71E-4AEB-A9EF-82D3D6322094}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{E9FF7E26-29D1-4A48-B688-AB78C4EC9AE9}"/>
+  <xr:revisionPtr revIDLastSave="15" documentId="114_{4E138255-E71E-4AEB-A9EF-82D3D6322094}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{CC476FA1-CA32-471F-AAF3-5C4BF72DCBF8}"/>
   <bookViews>
-    <workbookView xWindow="6468" yWindow="0" windowWidth="16524" windowHeight="12960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6516" yWindow="0" windowWidth="16524" windowHeight="12960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DOLAR_OBS_ADO" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$566</definedName>
+    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$569</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="5">
   <si>
     <t>Tipos de cambio (pesos por dólar)</t>
   </si>
@@ -927,10 +927,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B566"/>
+  <dimension ref="A1:B569"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A542" workbookViewId="0">
-      <selection activeCell="B568" sqref="B568"/>
+    <sheetView tabSelected="1" topLeftCell="A556" workbookViewId="0">
+      <selection activeCell="B570" sqref="B570"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5463,6 +5463,30 @@
         <v>787.5</v>
       </c>
     </row>
+    <row r="567" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A567" s="2">
+        <v>44030</v>
+      </c>
+      <c r="B567" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="568" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A568" s="2">
+        <v>44031</v>
+      </c>
+      <c r="B568" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="569" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A569" s="2">
+        <v>44032</v>
+      </c>
+      <c r="B569" s="3">
+        <v>787.26</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:B1"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 07-21-2020 17-10-15
</commit_message>
<xml_diff>
--- a/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
+++ b/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/944d5b9328a00097/Proyectos/Data intelligence/Covid-19/Chile/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="15" documentId="114_{4E138255-E71E-4AEB-A9EF-82D3D6322094}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{CC476FA1-CA32-471F-AAF3-5C4BF72DCBF8}"/>
+  <xr:revisionPtr revIDLastSave="16" documentId="114_{4E138255-E71E-4AEB-A9EF-82D3D6322094}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{28FE27B5-01CA-4E7F-BF46-A5E635094EDD}"/>
   <bookViews>
-    <workbookView xWindow="6516" yWindow="0" windowWidth="16524" windowHeight="12960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DOLAR_OBS_ADO" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$569</definedName>
+    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$570</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
@@ -927,10 +927,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B569"/>
+  <dimension ref="A1:B570"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A556" workbookViewId="0">
-      <selection activeCell="B570" sqref="B570"/>
+      <selection activeCell="B572" sqref="B572"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5487,6 +5487,14 @@
         <v>787.26</v>
       </c>
     </row>
+    <row r="570" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A570" s="2">
+        <v>44033</v>
+      </c>
+      <c r="B570" s="3">
+        <v>786.04</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:B1"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 07-22-2020 17-04-46
</commit_message>
<xml_diff>
--- a/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
+++ b/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/944d5b9328a00097/Proyectos/Data intelligence/Covid-19/Chile/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="16" documentId="114_{4E138255-E71E-4AEB-A9EF-82D3D6322094}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{28FE27B5-01CA-4E7F-BF46-A5E635094EDD}"/>
+  <xr:revisionPtr revIDLastSave="17" documentId="114_{4E138255-E71E-4AEB-A9EF-82D3D6322094}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{F324C252-22ED-4FC7-B725-4DB888146147}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="DOLAR_OBS_ADO" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$570</definedName>
+    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$571</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
@@ -927,10 +927,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B570"/>
+  <dimension ref="A1:B571"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A556" workbookViewId="0">
-      <selection activeCell="B572" sqref="B572"/>
+      <selection activeCell="B573" sqref="B573"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5495,6 +5495,14 @@
         <v>786.04</v>
       </c>
     </row>
+    <row r="571" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A571" s="2">
+        <v>44034</v>
+      </c>
+      <c r="B571" s="3">
+        <v>777.66</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:B1"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 07-23-2020 17-13-09
</commit_message>
<xml_diff>
--- a/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
+++ b/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/944d5b9328a00097/Proyectos/Data intelligence/Covid-19/Chile/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="17" documentId="114_{4E138255-E71E-4AEB-A9EF-82D3D6322094}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{F324C252-22ED-4FC7-B725-4DB888146147}"/>
+  <xr:revisionPtr revIDLastSave="18" documentId="114_{4E138255-E71E-4AEB-A9EF-82D3D6322094}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{CDCD7E0C-84C1-4EA6-93E6-EAAD30F22A20}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2304" yWindow="0" windowWidth="11544" windowHeight="12960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DOLAR_OBS_ADO" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$571</definedName>
+    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$572</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
@@ -927,10 +927,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B571"/>
+  <dimension ref="A1:B572"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A556" workbookViewId="0">
-      <selection activeCell="B573" sqref="B573"/>
+      <selection activeCell="B574" sqref="B574"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5503,6 +5503,14 @@
         <v>777.66</v>
       </c>
     </row>
+    <row r="572" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A572" s="2">
+        <v>44035</v>
+      </c>
+      <c r="B572" s="3">
+        <v>769.06</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:B1"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 07-24-2020 17-13-39
</commit_message>
<xml_diff>
--- a/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
+++ b/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/944d5b9328a00097/Proyectos/Data intelligence/Covid-19/Chile/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="18" documentId="114_{4E138255-E71E-4AEB-A9EF-82D3D6322094}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{CDCD7E0C-84C1-4EA6-93E6-EAAD30F22A20}"/>
+  <xr:revisionPtr revIDLastSave="19" documentId="114_{4E138255-E71E-4AEB-A9EF-82D3D6322094}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{A3D92239-A52D-4583-9EFC-B26122B5EEA0}"/>
   <bookViews>
-    <workbookView xWindow="2304" yWindow="0" windowWidth="11544" windowHeight="12960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DOLAR_OBS_ADO" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$572</definedName>
+    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$573</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
@@ -927,10 +927,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B572"/>
+  <dimension ref="A1:B573"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A556" workbookViewId="0">
-      <selection activeCell="B574" sqref="B574"/>
+      <selection activeCell="B576" sqref="B576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5511,6 +5511,14 @@
         <v>769.06</v>
       </c>
     </row>
+    <row r="573" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A573" s="2">
+        <v>44036</v>
+      </c>
+      <c r="B573" s="3">
+        <v>767.17</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:B1"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 07-25-2020 17-07-49
</commit_message>
<xml_diff>
--- a/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
+++ b/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/944d5b9328a00097/Proyectos/Data intelligence/Covid-19/Chile/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\reyes.rodriguezucv@gmail.com\OneDrive\Proyectos\Data intelligence\Covid-19\Chile\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="19" documentId="114_{4E138255-E71E-4AEB-A9EF-82D3D6322094}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{A3D92239-A52D-4583-9EFC-B26122B5EEA0}"/>
+  <xr:revisionPtr revIDLastSave="20" documentId="114_{4E138255-E71E-4AEB-A9EF-82D3D6322094}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{17B8D2D8-7173-41CF-9ED5-6D34144DD675}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10128" yWindow="1248" windowWidth="12912" windowHeight="9420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DOLAR_OBS_ADO" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$573</definedName>
+    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$576</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="5">
   <si>
     <t>Tipos de cambio (pesos por dólar)</t>
   </si>
@@ -927,10 +927,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B573"/>
+  <dimension ref="A1:B576"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A556" workbookViewId="0">
-      <selection activeCell="B576" sqref="B576"/>
+      <selection activeCell="A579" sqref="A579"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5519,6 +5519,30 @@
         <v>767.17</v>
       </c>
     </row>
+    <row r="574" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A574" s="2">
+        <v>44037</v>
+      </c>
+      <c r="B574" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="575" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A575" s="2">
+        <v>44038</v>
+      </c>
+      <c r="B575" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="576" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A576" s="2">
+        <v>44039</v>
+      </c>
+      <c r="B576" s="3">
+        <v>768.63</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:B1"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 07-28-2020 17-03-55
</commit_message>
<xml_diff>
--- a/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
+++ b/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\reyes.rodriguezucv@gmail.com\OneDrive\Proyectos\Data intelligence\Covid-19\Chile\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="20" documentId="114_{4E138255-E71E-4AEB-A9EF-82D3D6322094}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{17B8D2D8-7173-41CF-9ED5-6D34144DD675}"/>
+  <xr:revisionPtr revIDLastSave="21" documentId="114_{4E138255-E71E-4AEB-A9EF-82D3D6322094}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{2779362E-588B-4835-9B27-9D0AB18A01E1}"/>
   <bookViews>
-    <workbookView xWindow="10128" yWindow="1248" windowWidth="12912" windowHeight="9420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DOLAR_OBS_ADO" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$576</definedName>
+    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$577</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
@@ -927,10 +927,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B576"/>
+  <dimension ref="A1:B577"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A556" workbookViewId="0">
-      <selection activeCell="A579" sqref="A579"/>
+    <sheetView tabSelected="1" topLeftCell="A569" workbookViewId="0">
+      <selection activeCell="B581" sqref="B581"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5543,6 +5543,14 @@
         <v>768.63</v>
       </c>
     </row>
+    <row r="577" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A577" s="2">
+        <v>44040</v>
+      </c>
+      <c r="B577" s="3">
+        <v>768.81</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:B1"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 07-29-2020 17-12-18
</commit_message>
<xml_diff>
--- a/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
+++ b/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\reyes.rodriguezucv@gmail.com\OneDrive\Proyectos\Data intelligence\Covid-19\Chile\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="21" documentId="114_{4E138255-E71E-4AEB-A9EF-82D3D6322094}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{2779362E-588B-4835-9B27-9D0AB18A01E1}"/>
+  <xr:revisionPtr revIDLastSave="22" documentId="114_{4E138255-E71E-4AEB-A9EF-82D3D6322094}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{C011FB4A-0AC4-4DEC-9725-9B812A1BABDD}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="DOLAR_OBS_ADO" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$577</definedName>
+    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$578</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
@@ -927,10 +927,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B577"/>
+  <dimension ref="A1:B578"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A569" workbookViewId="0">
-      <selection activeCell="B581" sqref="B581"/>
+      <selection activeCell="B582" sqref="B582"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5551,6 +5551,14 @@
         <v>768.81</v>
       </c>
     </row>
+    <row r="578" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A578" s="2">
+        <v>44041</v>
+      </c>
+      <c r="B578" s="3">
+        <v>767.82</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:B1"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 07-30-2020 17-07-18
</commit_message>
<xml_diff>
--- a/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
+++ b/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\reyes.rodriguezucv@gmail.com\OneDrive\Proyectos\Data intelligence\Covid-19\Chile\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="22" documentId="114_{4E138255-E71E-4AEB-A9EF-82D3D6322094}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{C011FB4A-0AC4-4DEC-9725-9B812A1BABDD}"/>
+  <xr:revisionPtr revIDLastSave="23" documentId="114_{4E138255-E71E-4AEB-A9EF-82D3D6322094}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{747492B5-E655-4430-9EED-86B912026419}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="DOLAR_OBS_ADO" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$578</definedName>
+    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$579</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
@@ -927,10 +927,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B578"/>
+  <dimension ref="A1:B579"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A569" workbookViewId="0">
-      <selection activeCell="B582" sqref="B582"/>
+      <selection activeCell="B581" sqref="B581"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5559,6 +5559,14 @@
         <v>767.82</v>
       </c>
     </row>
+    <row r="579" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A579" s="2">
+        <v>44042</v>
+      </c>
+      <c r="B579" s="3">
+        <v>759.18</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:B1"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 07-31-2020 17-06-08
</commit_message>
<xml_diff>
--- a/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
+++ b/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\reyes.rodriguezucv@gmail.com\OneDrive\Proyectos\Data intelligence\Covid-19\Chile\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="23" documentId="114_{4E138255-E71E-4AEB-A9EF-82D3D6322094}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{747492B5-E655-4430-9EED-86B912026419}"/>
+  <xr:revisionPtr revIDLastSave="24" documentId="114_{4E138255-E71E-4AEB-A9EF-82D3D6322094}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{56C442FD-F082-46BA-B5DC-BF6D3DA2667B}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="DOLAR_OBS_ADO" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$579</definedName>
+    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$580</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
@@ -927,10 +927,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B579"/>
+  <dimension ref="A1:B580"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A569" workbookViewId="0">
-      <selection activeCell="B581" sqref="B581"/>
+      <selection activeCell="B583" sqref="B583"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5567,6 +5567,14 @@
         <v>759.18</v>
       </c>
     </row>
+    <row r="580" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A580" s="2">
+        <v>44043</v>
+      </c>
+      <c r="B580" s="3">
+        <v>754.45</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:B1"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 08-01-2020 17-08-12
</commit_message>
<xml_diff>
--- a/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
+++ b/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\reyes.rodriguezucv@gmail.com\OneDrive\Proyectos\Data intelligence\Covid-19\Chile\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="24" documentId="114_{4E138255-E71E-4AEB-A9EF-82D3D6322094}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{56C442FD-F082-46BA-B5DC-BF6D3DA2667B}"/>
+  <xr:revisionPtr revIDLastSave="25" documentId="114_{4E138255-E71E-4AEB-A9EF-82D3D6322094}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{9120E324-4FEC-48FA-9EA2-90DE4F7CA2E3}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8736" yWindow="0" windowWidth="14268" windowHeight="12960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DOLAR_OBS_ADO" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$580</definedName>
+    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$583</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="5">
   <si>
     <t>Tipos de cambio (pesos por dólar)</t>
   </si>
@@ -927,10 +927,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B580"/>
+  <dimension ref="A1:B583"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A569" workbookViewId="0">
-      <selection activeCell="B583" sqref="B583"/>
+      <selection activeCell="B586" sqref="B586"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5575,6 +5575,30 @@
         <v>754.45</v>
       </c>
     </row>
+    <row r="581" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A581" s="2">
+        <v>44044</v>
+      </c>
+      <c r="B581" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="582" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A582" s="2">
+        <v>44045</v>
+      </c>
+      <c r="B582" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="583" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A583" s="2">
+        <v>44046</v>
+      </c>
+      <c r="B583" s="3">
+        <v>757.06</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:B1"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 08-04-2020 17-07-46
</commit_message>
<xml_diff>
--- a/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
+++ b/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\reyes.rodriguezucv@gmail.com\OneDrive\Proyectos\Data intelligence\Covid-19\Chile\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="25" documentId="114_{4E138255-E71E-4AEB-A9EF-82D3D6322094}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{9120E324-4FEC-48FA-9EA2-90DE4F7CA2E3}"/>
+  <xr:revisionPtr revIDLastSave="26" documentId="114_{4E138255-E71E-4AEB-A9EF-82D3D6322094}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{AA8612E1-CB67-494D-B501-684A090792BC}"/>
   <bookViews>
-    <workbookView xWindow="8736" yWindow="0" windowWidth="14268" windowHeight="12960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6840" yWindow="2640" windowWidth="15852" windowHeight="9420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DOLAR_OBS_ADO" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$583</definedName>
+    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$584</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
@@ -927,7 +927,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B583"/>
+  <dimension ref="A1:B584"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A569" workbookViewId="0">
       <selection activeCell="B586" sqref="B586"/>
@@ -5599,6 +5599,14 @@
         <v>757.06</v>
       </c>
     </row>
+    <row r="584" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A584" s="2">
+        <v>44047</v>
+      </c>
+      <c r="B584" s="3">
+        <v>761.34</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:B1"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 08-05-2020 17-04-11
</commit_message>
<xml_diff>
--- a/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
+++ b/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\reyes.rodriguezucv@gmail.com\OneDrive\Proyectos\Data intelligence\Covid-19\Chile\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="26" documentId="114_{4E138255-E71E-4AEB-A9EF-82D3D6322094}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{AA8612E1-CB67-494D-B501-684A090792BC}"/>
+  <xr:revisionPtr revIDLastSave="27" documentId="114_{4E138255-E71E-4AEB-A9EF-82D3D6322094}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{E3F900AA-0917-461A-812F-443EA7CE1B8E}"/>
   <bookViews>
-    <workbookView xWindow="6840" yWindow="2640" windowWidth="15852" windowHeight="9420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DOLAR_OBS_ADO" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$584</definedName>
+    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$585</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
@@ -927,10 +927,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B584"/>
+  <dimension ref="A1:B585"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A569" workbookViewId="0">
-      <selection activeCell="B586" sqref="B586"/>
+      <selection activeCell="B587" sqref="B587"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5607,6 +5607,14 @@
         <v>761.34</v>
       </c>
     </row>
+    <row r="585" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A585" s="2">
+        <v>44048</v>
+      </c>
+      <c r="B585" s="3">
+        <v>767.98</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:B1"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 08-06-2020 17-10-02
</commit_message>
<xml_diff>
--- a/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
+++ b/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\reyes.rodriguezucv@gmail.com\OneDrive\Proyectos\Data intelligence\Covid-19\Chile\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="27" documentId="114_{4E138255-E71E-4AEB-A9EF-82D3D6322094}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{E3F900AA-0917-461A-812F-443EA7CE1B8E}"/>
+  <xr:revisionPtr revIDLastSave="28" documentId="114_{4E138255-E71E-4AEB-A9EF-82D3D6322094}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{E80AFB61-3CC7-4CE1-B20F-B061D8146CEA}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1392" yWindow="2964" windowWidth="14436" windowHeight="9420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DOLAR_OBS_ADO" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$585</definedName>
+    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$586</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
@@ -927,10 +927,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B585"/>
+  <dimension ref="A1:B586"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A569" workbookViewId="0">
-      <selection activeCell="B587" sqref="B587"/>
+    <sheetView tabSelected="1" topLeftCell="A578" workbookViewId="0">
+      <selection activeCell="B588" sqref="B588"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5615,6 +5615,14 @@
         <v>767.98</v>
       </c>
     </row>
+    <row r="586" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A586" s="2">
+        <v>44049</v>
+      </c>
+      <c r="B586" s="3">
+        <v>774.82</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:B1"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 08-07-2020 17-08-55
</commit_message>
<xml_diff>
--- a/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
+++ b/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\reyes.rodriguezucv@gmail.com\OneDrive\Proyectos\Data intelligence\Covid-19\Chile\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="28" documentId="114_{4E138255-E71E-4AEB-A9EF-82D3D6322094}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{E80AFB61-3CC7-4CE1-B20F-B061D8146CEA}"/>
+  <xr:revisionPtr revIDLastSave="29" documentId="114_{4E138255-E71E-4AEB-A9EF-82D3D6322094}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{BF0E699B-0629-402A-9D76-D12622E37B82}"/>
   <bookViews>
-    <workbookView xWindow="1392" yWindow="2964" windowWidth="14436" windowHeight="9420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DOLAR_OBS_ADO" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$586</definedName>
+    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$587</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
@@ -927,10 +927,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B586"/>
+  <dimension ref="A1:B587"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A578" workbookViewId="0">
-      <selection activeCell="B588" sqref="B588"/>
+      <selection activeCell="B589" sqref="B589"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5623,6 +5623,14 @@
         <v>774.82</v>
       </c>
     </row>
+    <row r="587" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A587" s="2">
+        <v>44050</v>
+      </c>
+      <c r="B587" s="3">
+        <v>777.18</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:B1"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 08-08-2020 17-12-02
</commit_message>
<xml_diff>
--- a/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
+++ b/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\reyes.rodriguezucv@gmail.com\OneDrive\Proyectos\Data intelligence\Covid-19\Chile\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="29" documentId="114_{4E138255-E71E-4AEB-A9EF-82D3D6322094}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{BF0E699B-0629-402A-9D76-D12622E37B82}"/>
+  <xr:revisionPtr revIDLastSave="30" documentId="114_{4E138255-E71E-4AEB-A9EF-82D3D6322094}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{D76B761E-FFB2-4299-A78F-9A09E76EFFCC}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="DOLAR_OBS_ADO" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$587</definedName>
+    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$590</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="5">
   <si>
     <t>Tipos de cambio (pesos por dólar)</t>
   </si>
@@ -927,10 +927,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B587"/>
+  <dimension ref="A1:B590"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A578" workbookViewId="0">
-      <selection activeCell="B589" sqref="B589"/>
+      <selection activeCell="B593" sqref="B593"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5631,6 +5631,30 @@
         <v>777.18</v>
       </c>
     </row>
+    <row r="588" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A588" s="2">
+        <v>44051</v>
+      </c>
+      <c r="B588" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="589" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A589" s="2">
+        <v>44052</v>
+      </c>
+      <c r="B589" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="590" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A590" s="2">
+        <v>44053</v>
+      </c>
+      <c r="B590" s="3">
+        <v>784.28</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:B1"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 08-11-2020 17-09-41
</commit_message>
<xml_diff>
--- a/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
+++ b/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\reyes.rodriguezucv@gmail.com\OneDrive\Proyectos\Data intelligence\Covid-19\Chile\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="30" documentId="114_{4E138255-E71E-4AEB-A9EF-82D3D6322094}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{D76B761E-FFB2-4299-A78F-9A09E76EFFCC}"/>
+  <xr:revisionPtr revIDLastSave="31" documentId="114_{4E138255-E71E-4AEB-A9EF-82D3D6322094}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{EE15A79F-493C-4D0F-B891-3BF46920E5D0}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="DOLAR_OBS_ADO" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$590</definedName>
+    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$591</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
@@ -927,10 +927,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B590"/>
+  <dimension ref="A1:B591"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A578" workbookViewId="0">
-      <selection activeCell="B593" sqref="B593"/>
+      <selection activeCell="B595" sqref="B595"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5655,6 +5655,14 @@
         <v>784.28</v>
       </c>
     </row>
+    <row r="591" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A591" s="2">
+        <v>44054</v>
+      </c>
+      <c r="B591" s="3">
+        <v>796.58</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:B1"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 08-12-2020 17-10-30
</commit_message>
<xml_diff>
--- a/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
+++ b/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\reyes.rodriguezucv@gmail.com\OneDrive\Proyectos\Data intelligence\Covid-19\Chile\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="31" documentId="114_{4E138255-E71E-4AEB-A9EF-82D3D6322094}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{EE15A79F-493C-4D0F-B891-3BF46920E5D0}"/>
+  <xr:revisionPtr revIDLastSave="32" documentId="114_{4E138255-E71E-4AEB-A9EF-82D3D6322094}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{6174338D-1136-41E4-B130-05494DC1FFBC}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="DOLAR_OBS_ADO" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$591</definedName>
+    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$592</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
@@ -927,10 +927,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B591"/>
+  <dimension ref="A1:B592"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A578" workbookViewId="0">
-      <selection activeCell="B595" sqref="B595"/>
+      <selection activeCell="B592" sqref="B592"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5663,6 +5663,14 @@
         <v>796.58</v>
       </c>
     </row>
+    <row r="592" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A592" s="2">
+        <v>44055</v>
+      </c>
+      <c r="B592" s="3">
+        <v>793.61</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:B1"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 08-13-2020 17-04-36
</commit_message>
<xml_diff>
--- a/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
+++ b/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\reyes.rodriguezucv@gmail.com\OneDrive\Proyectos\Data intelligence\Covid-19\Chile\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="32" documentId="114_{4E138255-E71E-4AEB-A9EF-82D3D6322094}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{6174338D-1136-41E4-B130-05494DC1FFBC}"/>
+  <xr:revisionPtr revIDLastSave="33" documentId="114_{4E138255-E71E-4AEB-A9EF-82D3D6322094}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{A52185C3-9096-4051-A7CE-2C4191DABEC3}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="DOLAR_OBS_ADO" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$592</definedName>
+    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$593</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
@@ -927,10 +927,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B592"/>
+  <dimension ref="A1:B593"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A578" workbookViewId="0">
-      <selection activeCell="B592" sqref="B592"/>
+      <selection activeCell="B596" sqref="B596"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5671,6 +5671,14 @@
         <v>793.61</v>
       </c>
     </row>
+    <row r="593" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A593" s="2">
+        <v>44056</v>
+      </c>
+      <c r="B593" s="3">
+        <v>792.69</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:B1"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 08-14-2020 17-11-42
</commit_message>
<xml_diff>
--- a/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
+++ b/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\reyes.rodriguezucv@gmail.com\OneDrive\Proyectos\Data intelligence\Covid-19\Chile\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="33" documentId="114_{4E138255-E71E-4AEB-A9EF-82D3D6322094}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{A52185C3-9096-4051-A7CE-2C4191DABEC3}"/>
+  <xr:revisionPtr revIDLastSave="34" documentId="114_{4E138255-E71E-4AEB-A9EF-82D3D6322094}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{3B89A267-34E0-4226-A4FB-ED433D75CF2A}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="DOLAR_OBS_ADO" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$593</definedName>
+    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$594</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
@@ -927,7 +927,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B593"/>
+  <dimension ref="A1:B594"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A578" workbookViewId="0">
       <selection activeCell="B596" sqref="B596"/>
@@ -5679,6 +5679,14 @@
         <v>792.69</v>
       </c>
     </row>
+    <row r="594" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A594" s="2">
+        <v>44057</v>
+      </c>
+      <c r="B594" s="3">
+        <v>793.32</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:B1"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 08-15-2020 17-08-49
</commit_message>
<xml_diff>
--- a/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
+++ b/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\reyes.rodriguezucv@gmail.com\OneDrive\Proyectos\Data intelligence\Covid-19\Chile\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="34" documentId="114_{4E138255-E71E-4AEB-A9EF-82D3D6322094}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{3B89A267-34E0-4226-A4FB-ED433D75CF2A}"/>
+  <xr:revisionPtr revIDLastSave="36" documentId="114_{4E138255-E71E-4AEB-A9EF-82D3D6322094}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{4BA17ED6-103C-4661-9ABA-45D8D57BCA20}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="DOLAR_OBS_ADO" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$594</definedName>
+    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$597</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="5">
   <si>
     <t>Tipos de cambio (pesos por dólar)</t>
   </si>
@@ -927,10 +927,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B594"/>
+  <dimension ref="A1:B597"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A578" workbookViewId="0">
-      <selection activeCell="B596" sqref="B596"/>
+      <selection activeCell="B599" sqref="B599"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5687,6 +5687,30 @@
         <v>793.32</v>
       </c>
     </row>
+    <row r="595" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A595" s="2">
+        <v>44058</v>
+      </c>
+      <c r="B595" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="596" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A596" s="2">
+        <v>44059</v>
+      </c>
+      <c r="B596" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="597" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A597" s="2">
+        <v>44060</v>
+      </c>
+      <c r="B597" s="3">
+        <v>796.73</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:B1"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 08-18-2020 21-14-36
</commit_message>
<xml_diff>
--- a/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
+++ b/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\reyes.rodriguezucv@gmail.com\OneDrive\Proyectos\Data intelligence\Covid-19\Chile\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="36" documentId="114_{4E138255-E71E-4AEB-A9EF-82D3D6322094}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{4BA17ED6-103C-4661-9ABA-45D8D57BCA20}"/>
+  <xr:revisionPtr revIDLastSave="37" documentId="114_{4E138255-E71E-4AEB-A9EF-82D3D6322094}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{7518DCBC-50DE-40D2-9561-592363CC13D8}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="DOLAR_OBS_ADO" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$597</definedName>
+    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$598</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
@@ -927,10 +927,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B597"/>
+  <dimension ref="A1:B598"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A578" workbookViewId="0">
-      <selection activeCell="B599" sqref="B599"/>
+    <sheetView tabSelected="1" topLeftCell="A587" workbookViewId="0">
+      <selection activeCell="B601" sqref="B601"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5711,6 +5711,14 @@
         <v>796.73</v>
       </c>
     </row>
+    <row r="598" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A598" s="2">
+        <v>44061</v>
+      </c>
+      <c r="B598" s="3">
+        <v>803.4</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:B1"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 08-19-2020 17-11-37
</commit_message>
<xml_diff>
--- a/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
+++ b/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\reyes.rodriguezucv@gmail.com\OneDrive\Proyectos\Data intelligence\Covid-19\Chile\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="37" documentId="114_{4E138255-E71E-4AEB-A9EF-82D3D6322094}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{7518DCBC-50DE-40D2-9561-592363CC13D8}"/>
+  <xr:revisionPtr revIDLastSave="39" documentId="114_{4E138255-E71E-4AEB-A9EF-82D3D6322094}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{FD2550FF-BB65-4964-8B7B-AF17DBC69C88}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2304" yWindow="0" windowWidth="14904" windowHeight="12960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DOLAR_OBS_ADO" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$598</definedName>
+    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$599</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
@@ -927,10 +927,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B598"/>
+  <dimension ref="A1:B599"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A587" workbookViewId="0">
-      <selection activeCell="B601" sqref="B601"/>
+      <selection activeCell="C602" sqref="C602"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5719,6 +5719,14 @@
         <v>803.4</v>
       </c>
     </row>
+    <row r="599" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A599" s="2">
+        <v>44062</v>
+      </c>
+      <c r="B599" s="3">
+        <v>796.23</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:B1"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 08-20-2020 17-11-50
</commit_message>
<xml_diff>
--- a/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
+++ b/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\reyes.rodriguezucv@gmail.com\OneDrive\Proyectos\Data intelligence\Covid-19\Chile\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="39" documentId="114_{4E138255-E71E-4AEB-A9EF-82D3D6322094}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{FD2550FF-BB65-4964-8B7B-AF17DBC69C88}"/>
+  <xr:revisionPtr revIDLastSave="40" documentId="114_{4E138255-E71E-4AEB-A9EF-82D3D6322094}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{49806599-DDF3-45D7-B846-0D68E5C3CFE3}"/>
   <bookViews>
-    <workbookView xWindow="2304" yWindow="0" windowWidth="14904" windowHeight="12960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DOLAR_OBS_ADO" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$599</definedName>
+    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$600</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
@@ -927,10 +927,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B599"/>
+  <dimension ref="A1:B600"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A587" workbookViewId="0">
-      <selection activeCell="C602" sqref="C602"/>
+      <selection activeCell="B602" sqref="B602"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5727,6 +5727,14 @@
         <v>796.23</v>
       </c>
     </row>
+    <row r="600" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A600" s="2">
+        <v>44063</v>
+      </c>
+      <c r="B600" s="3">
+        <v>784.25</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:B1"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 08-21-2020 17-12-17
</commit_message>
<xml_diff>
--- a/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
+++ b/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\reyes.rodriguezucv@gmail.com\OneDrive\Proyectos\Data intelligence\Covid-19\Chile\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="40" documentId="114_{4E138255-E71E-4AEB-A9EF-82D3D6322094}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{49806599-DDF3-45D7-B846-0D68E5C3CFE3}"/>
+  <xr:revisionPtr revIDLastSave="41" documentId="114_{4E138255-E71E-4AEB-A9EF-82D3D6322094}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{67A2DAAD-F4FA-4F60-BFCF-27937355945B}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="DOLAR_OBS_ADO" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$600</definedName>
+    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$601</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
@@ -927,10 +927,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B600"/>
+  <dimension ref="A1:B601"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A587" workbookViewId="0">
-      <selection activeCell="B602" sqref="B602"/>
+      <selection activeCell="B603" sqref="B603"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5735,6 +5735,14 @@
         <v>784.25</v>
       </c>
     </row>
+    <row r="601" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A601" s="2">
+        <v>44064</v>
+      </c>
+      <c r="B601" s="3">
+        <v>785.84</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:B1"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 08-22-2020 17-08-33
</commit_message>
<xml_diff>
--- a/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
+++ b/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\reyes.rodriguezucv@gmail.com\OneDrive\Proyectos\Data intelligence\Covid-19\Chile\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="41" documentId="114_{4E138255-E71E-4AEB-A9EF-82D3D6322094}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{67A2DAAD-F4FA-4F60-BFCF-27937355945B}"/>
+  <xr:revisionPtr revIDLastSave="42" documentId="114_{4E138255-E71E-4AEB-A9EF-82D3D6322094}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{15EE17CF-30D1-4633-A4E3-B73F94BD980B}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="DOLAR_OBS_ADO" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$601</definedName>
+    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$604</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="5">
   <si>
     <t>Tipos de cambio (pesos por dólar)</t>
   </si>
@@ -927,10 +927,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B601"/>
+  <dimension ref="A1:B604"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A587" workbookViewId="0">
-      <selection activeCell="B603" sqref="B603"/>
+      <selection activeCell="A607" sqref="A607"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5743,6 +5743,30 @@
         <v>785.84</v>
       </c>
     </row>
+    <row r="602" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A602" s="2">
+        <v>44065</v>
+      </c>
+      <c r="B602" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="603" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A603" s="2">
+        <v>44066</v>
+      </c>
+      <c r="B603" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="604" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A604" s="2">
+        <v>44067</v>
+      </c>
+      <c r="B604" s="3">
+        <v>790.88</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:B1"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 08-25-2020 17-09-27
</commit_message>
<xml_diff>
--- a/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
+++ b/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\reyes.rodriguezucv@gmail.com\OneDrive\Proyectos\Data intelligence\Covid-19\Chile\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="42" documentId="114_{4E138255-E71E-4AEB-A9EF-82D3D6322094}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{15EE17CF-30D1-4633-A4E3-B73F94BD980B}"/>
+  <xr:revisionPtr revIDLastSave="43" documentId="114_{4E138255-E71E-4AEB-A9EF-82D3D6322094}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{9E7875ED-0941-4738-89E1-D0FF64DA7312}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11484" yWindow="0" windowWidth="11544" windowHeight="12960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DOLAR_OBS_ADO" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$604</definedName>
+    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$605</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
@@ -927,10 +927,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B604"/>
+  <dimension ref="A1:B605"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A587" workbookViewId="0">
-      <selection activeCell="A607" sqref="A607"/>
+      <selection activeCell="B608" sqref="B608"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5767,6 +5767,14 @@
         <v>790.88</v>
       </c>
     </row>
+    <row r="605" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A605" s="2">
+        <v>44068</v>
+      </c>
+      <c r="B605" s="3">
+        <v>786.17</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:B1"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 08-26-2020 17-12-06
</commit_message>
<xml_diff>
--- a/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
+++ b/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\reyes.rodriguezucv@gmail.com\OneDrive\Proyectos\Data intelligence\Covid-19\Chile\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="43" documentId="114_{4E138255-E71E-4AEB-A9EF-82D3D6322094}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{9E7875ED-0941-4738-89E1-D0FF64DA7312}"/>
+  <xr:revisionPtr revIDLastSave="44" documentId="114_{4E138255-E71E-4AEB-A9EF-82D3D6322094}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{A991C7D5-79D8-48FC-8525-2FDFA4E78412}"/>
   <bookViews>
-    <workbookView xWindow="11484" yWindow="0" windowWidth="11544" windowHeight="12960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DOLAR_OBS_ADO" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$605</definedName>
+    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$606</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
@@ -927,7 +927,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B605"/>
+  <dimension ref="A1:B606"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A587" workbookViewId="0">
       <selection activeCell="B608" sqref="B608"/>
@@ -5775,6 +5775,14 @@
         <v>786.17</v>
       </c>
     </row>
+    <row r="606" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A606" s="2">
+        <v>44069</v>
+      </c>
+      <c r="B606" s="3">
+        <v>784.44</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:B1"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 08-27-2020 17-13-49
</commit_message>
<xml_diff>
--- a/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
+++ b/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\reyes.rodriguezucv@gmail.com\OneDrive\Proyectos\Data intelligence\Covid-19\Chile\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="44" documentId="114_{4E138255-E71E-4AEB-A9EF-82D3D6322094}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{A991C7D5-79D8-48FC-8525-2FDFA4E78412}"/>
+  <xr:revisionPtr revIDLastSave="45" documentId="114_{4E138255-E71E-4AEB-A9EF-82D3D6322094}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{D5171149-78A9-4B20-8DE2-854A7348C4A5}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="DOLAR_OBS_ADO" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$606</definedName>
+    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$607</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
@@ -927,10 +927,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B606"/>
+  <dimension ref="A1:B607"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A587" workbookViewId="0">
-      <selection activeCell="B608" sqref="B608"/>
+      <selection activeCell="B609" sqref="B609"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5783,6 +5783,14 @@
         <v>784.44</v>
       </c>
     </row>
+    <row r="607" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A607" s="2">
+        <v>44070</v>
+      </c>
+      <c r="B607" s="3">
+        <v>786.91</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:B1"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 08-28-2020 17-10-14
</commit_message>
<xml_diff>
--- a/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
+++ b/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\reyes.rodriguezucv@gmail.com\OneDrive\Proyectos\Data intelligence\Covid-19\Chile\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="45" documentId="114_{4E138255-E71E-4AEB-A9EF-82D3D6322094}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{D5171149-78A9-4B20-8DE2-854A7348C4A5}"/>
+  <xr:revisionPtr revIDLastSave="46" documentId="114_{4E138255-E71E-4AEB-A9EF-82D3D6322094}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{3295FE36-4E25-4B0D-AF64-10D8C6EC87CF}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="DOLAR_OBS_ADO" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$607</definedName>
+    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$608</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
@@ -927,10 +927,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B607"/>
+  <dimension ref="A1:B608"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A587" workbookViewId="0">
-      <selection activeCell="B609" sqref="B609"/>
+      <selection activeCell="B610" sqref="B610"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5791,6 +5791,14 @@
         <v>786.91</v>
       </c>
     </row>
+    <row r="608" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A608" s="2">
+        <v>44071</v>
+      </c>
+      <c r="B608" s="3">
+        <v>784.27</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:B1"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 08-29-2020 17-07-52
</commit_message>
<xml_diff>
--- a/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
+++ b/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\reyes.rodriguezucv@gmail.com\OneDrive\Proyectos\Data intelligence\Covid-19\Chile\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="46" documentId="114_{4E138255-E71E-4AEB-A9EF-82D3D6322094}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{3295FE36-4E25-4B0D-AF64-10D8C6EC87CF}"/>
+  <xr:revisionPtr revIDLastSave="47" documentId="114_{4E138255-E71E-4AEB-A9EF-82D3D6322094}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{AD935731-E8BC-437B-99A0-4739175159B7}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="DOLAR_OBS_ADO" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$608</definedName>
+    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$611</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="5">
   <si>
     <t>Tipos de cambio (pesos por dólar)</t>
   </si>
@@ -927,10 +927,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B608"/>
+  <dimension ref="A1:B611"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A587" workbookViewId="0">
-      <selection activeCell="B610" sqref="B610"/>
+    <sheetView tabSelected="1" topLeftCell="A599" workbookViewId="0">
+      <selection activeCell="B615" sqref="B615"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5799,6 +5799,30 @@
         <v>784.27</v>
       </c>
     </row>
+    <row r="609" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A609" s="2">
+        <v>44072</v>
+      </c>
+      <c r="B609" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="610" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A610" s="2">
+        <v>44073</v>
+      </c>
+      <c r="B610" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="611" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A611" s="2">
+        <v>44074</v>
+      </c>
+      <c r="B611" s="3">
+        <v>779.92</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:B1"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 09-01-2020 17-11-50
</commit_message>
<xml_diff>
--- a/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
+++ b/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\reyes.rodriguezucv@gmail.com\OneDrive\Proyectos\Data intelligence\Covid-19\Chile\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="47" documentId="114_{4E138255-E71E-4AEB-A9EF-82D3D6322094}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{AD935731-E8BC-437B-99A0-4739175159B7}"/>
+  <xr:revisionPtr revIDLastSave="48" documentId="114_{4E138255-E71E-4AEB-A9EF-82D3D6322094}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{59187C11-6208-477F-961E-800C3FA6F1CA}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="DOLAR_OBS_ADO" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$611</definedName>
+    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$612</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
@@ -927,10 +927,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B611"/>
+  <dimension ref="A1:B612"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A599" workbookViewId="0">
-      <selection activeCell="B615" sqref="B615"/>
+      <selection activeCell="B617" sqref="B617"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5823,6 +5823,14 @@
         <v>779.92</v>
       </c>
     </row>
+    <row r="612" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A612" s="2">
+        <v>44075</v>
+      </c>
+      <c r="B612" s="3">
+        <v>776.46</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:B1"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 09-01-2020 23-40-00
</commit_message>
<xml_diff>
--- a/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
+++ b/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\reyes.rodriguezucv@gmail.com\OneDrive\Proyectos\Data intelligence\Covid-19\Chile\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="48" documentId="114_{4E138255-E71E-4AEB-A9EF-82D3D6322094}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{59187C11-6208-477F-961E-800C3FA6F1CA}"/>
+  <xr:revisionPtr revIDLastSave="51" documentId="114_{4E138255-E71E-4AEB-A9EF-82D3D6322094}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{C172E11D-12EB-4D94-A154-60B2BE3263F6}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -930,7 +930,7 @@
   <dimension ref="A1:B612"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A599" workbookViewId="0">
-      <selection activeCell="B617" sqref="B617"/>
+      <selection activeCell="B615" sqref="B615"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 09-03-2020 17-04-25
</commit_message>
<xml_diff>
--- a/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
+++ b/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\reyes.rodriguezucv@gmail.com\OneDrive\Proyectos\Data intelligence\Covid-19\Chile\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="51" documentId="114_{4E138255-E71E-4AEB-A9EF-82D3D6322094}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{C172E11D-12EB-4D94-A154-60B2BE3263F6}"/>
+  <xr:revisionPtr revIDLastSave="52" documentId="114_{4E138255-E71E-4AEB-A9EF-82D3D6322094}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{23AD80C7-3E78-4F1D-88B1-00B7122626E3}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="DOLAR_OBS_ADO" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$612</definedName>
+    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$614</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
@@ -927,10 +927,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B612"/>
+  <dimension ref="A1:B614"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A599" workbookViewId="0">
-      <selection activeCell="B615" sqref="B615"/>
+      <selection activeCell="B616" sqref="B616"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5831,6 +5831,22 @@
         <v>776.46</v>
       </c>
     </row>
+    <row r="613" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A613" s="2">
+        <v>44076</v>
+      </c>
+      <c r="B613" s="3">
+        <v>770.59</v>
+      </c>
+    </row>
+    <row r="614" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A614" s="2">
+        <v>44077</v>
+      </c>
+      <c r="B614" s="3">
+        <v>771.45</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:B1"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 09-04-2020 17-11-13
</commit_message>
<xml_diff>
--- a/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
+++ b/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\reyes.rodriguezucv@gmail.com\OneDrive\Proyectos\Data intelligence\Covid-19\Chile\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="52" documentId="114_{4E138255-E71E-4AEB-A9EF-82D3D6322094}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{23AD80C7-3E78-4F1D-88B1-00B7122626E3}"/>
+  <xr:revisionPtr revIDLastSave="57" documentId="114_{4E138255-E71E-4AEB-A9EF-82D3D6322094}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{ACEB13CD-7F66-4D03-AEB5-3F52E6BCA971}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="DOLAR_OBS_ADO" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$614</definedName>
+    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$615</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
@@ -927,10 +927,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B614"/>
+  <dimension ref="A1:B615"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A599" workbookViewId="0">
-      <selection activeCell="B616" sqref="B616"/>
+      <selection activeCell="B618" sqref="B618"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5847,6 +5847,14 @@
         <v>771.45</v>
       </c>
     </row>
+    <row r="615" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A615" s="2">
+        <v>44078</v>
+      </c>
+      <c r="B615" s="3">
+        <v>773.71</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:B1"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 09-05-2020 17-12-07
</commit_message>
<xml_diff>
--- a/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
+++ b/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\reyes.rodriguezucv@gmail.com\OneDrive\Proyectos\Data intelligence\Covid-19\Chile\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="57" documentId="114_{4E138255-E71E-4AEB-A9EF-82D3D6322094}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{ACEB13CD-7F66-4D03-AEB5-3F52E6BCA971}"/>
+  <xr:revisionPtr revIDLastSave="58" documentId="114_{4E138255-E71E-4AEB-A9EF-82D3D6322094}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{CC440E4E-42ED-4D13-B628-1B4C150ADE65}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="DOLAR_OBS_ADO" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$615</definedName>
+    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$618</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="5">
   <si>
     <t>Tipos de cambio (pesos por dólar)</t>
   </si>
@@ -927,10 +927,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B615"/>
+  <dimension ref="A1:B618"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A599" workbookViewId="0">
-      <selection activeCell="B618" sqref="B618"/>
+      <selection activeCell="B615" sqref="B615"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5855,6 +5855,30 @@
         <v>773.71</v>
       </c>
     </row>
+    <row r="616" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A616" s="2">
+        <v>44079</v>
+      </c>
+      <c r="B616" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="617" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A617" s="2">
+        <v>44080</v>
+      </c>
+      <c r="B617" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="618" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A618" s="2">
+        <v>44081</v>
+      </c>
+      <c r="B618" s="3">
+        <v>773.76</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:B1"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 09-08-2020 17-07-45
</commit_message>
<xml_diff>
--- a/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
+++ b/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\reyes.rodriguezucv@gmail.com\OneDrive\Proyectos\Data intelligence\Covid-19\Chile\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="58" documentId="114_{4E138255-E71E-4AEB-A9EF-82D3D6322094}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{CC440E4E-42ED-4D13-B628-1B4C150ADE65}"/>
+  <xr:revisionPtr revIDLastSave="59" documentId="114_{4E138255-E71E-4AEB-A9EF-82D3D6322094}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{23FD4E71-B894-498E-89DB-B24248C07551}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="DOLAR_OBS_ADO" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$618</definedName>
+    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$619</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
@@ -927,10 +927,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B618"/>
+  <dimension ref="A1:B619"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A599" workbookViewId="0">
-      <selection activeCell="B615" sqref="B615"/>
+    <sheetView tabSelected="1" topLeftCell="A608" workbookViewId="0">
+      <selection activeCell="B622" sqref="B622"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5879,6 +5879,14 @@
         <v>773.76</v>
       </c>
     </row>
+    <row r="619" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A619" s="2">
+        <v>44082</v>
+      </c>
+      <c r="B619" s="3">
+        <v>773.24</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:B1"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 09-09-2020 17-09-44
</commit_message>
<xml_diff>
--- a/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
+++ b/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\reyes.rodriguezucv@gmail.com\OneDrive\Proyectos\Data intelligence\Covid-19\Chile\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="59" documentId="114_{4E138255-E71E-4AEB-A9EF-82D3D6322094}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{23FD4E71-B894-498E-89DB-B24248C07551}"/>
+  <xr:revisionPtr revIDLastSave="60" documentId="114_{4E138255-E71E-4AEB-A9EF-82D3D6322094}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{0D4E017A-1ABE-4224-996E-011B4EA49F88}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="DOLAR_OBS_ADO" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$619</definedName>
+    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$620</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
@@ -927,7 +927,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B619"/>
+  <dimension ref="A1:B620"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A608" workbookViewId="0">
       <selection activeCell="B622" sqref="B622"/>
@@ -5887,6 +5887,14 @@
         <v>773.24</v>
       </c>
     </row>
+    <row r="620" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A620" s="2">
+        <v>44083</v>
+      </c>
+      <c r="B620" s="3">
+        <v>776.65</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:B1"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 09-10-2020 17-06-58
</commit_message>
<xml_diff>
--- a/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
+++ b/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\reyes.rodriguezucv@gmail.com\OneDrive\Proyectos\Data intelligence\Covid-19\Chile\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="60" documentId="114_{4E138255-E71E-4AEB-A9EF-82D3D6322094}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{0D4E017A-1ABE-4224-996E-011B4EA49F88}"/>
+  <xr:revisionPtr revIDLastSave="61" documentId="114_{4E138255-E71E-4AEB-A9EF-82D3D6322094}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{FC2223E8-242B-4E73-83D3-DDDF3B1C323A}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="DOLAR_OBS_ADO" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$620</definedName>
+    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$621</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
@@ -927,10 +927,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B620"/>
+  <dimension ref="A1:B621"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A608" workbookViewId="0">
-      <selection activeCell="B622" sqref="B622"/>
+      <selection activeCell="B623" sqref="B623"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5895,6 +5895,14 @@
         <v>776.65</v>
       </c>
     </row>
+    <row r="621" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A621" s="2">
+        <v>44084</v>
+      </c>
+      <c r="B621" s="3">
+        <v>767.87</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:B1"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 09-11-2020 17-05-15
</commit_message>
<xml_diff>
--- a/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
+++ b/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\reyes.rodriguezucv@gmail.com\OneDrive\Proyectos\Data intelligence\Covid-19\Chile\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="61" documentId="114_{4E138255-E71E-4AEB-A9EF-82D3D6322094}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{FC2223E8-242B-4E73-83D3-DDDF3B1C323A}"/>
+  <xr:revisionPtr revIDLastSave="62" documentId="114_{4E138255-E71E-4AEB-A9EF-82D3D6322094}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{D9B9BE50-05EA-4106-BDFB-49FA29893B86}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6936" yWindow="0" windowWidth="16104" windowHeight="12360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DOLAR_OBS_ADO" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$621</definedName>
+    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$622</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
@@ -927,10 +927,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B621"/>
+  <dimension ref="A1:B622"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A608" workbookViewId="0">
-      <selection activeCell="B623" sqref="B623"/>
+      <selection activeCell="B624" sqref="B624"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5903,6 +5903,14 @@
         <v>767.87</v>
       </c>
     </row>
+    <row r="622" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A622" s="2">
+        <v>44085</v>
+      </c>
+      <c r="B622" s="3">
+        <v>764.99</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:B1"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 09-12-2020 17-09-04
</commit_message>
<xml_diff>
--- a/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
+++ b/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\reyes.rodriguezucv@gmail.com\OneDrive\Proyectos\Data intelligence\Covid-19\Chile\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="62" documentId="114_{4E138255-E71E-4AEB-A9EF-82D3D6322094}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{D9B9BE50-05EA-4106-BDFB-49FA29893B86}"/>
+  <xr:revisionPtr revIDLastSave="63" documentId="114_{4E138255-E71E-4AEB-A9EF-82D3D6322094}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{E57204AB-F43E-422A-B153-F7AE3CFF9F07}"/>
   <bookViews>
-    <workbookView xWindow="6936" yWindow="0" windowWidth="16104" windowHeight="12360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DOLAR_OBS_ADO" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$622</definedName>
+    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$625</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="5">
   <si>
     <t>Tipos de cambio (pesos por dólar)</t>
   </si>
@@ -927,10 +927,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B622"/>
+  <dimension ref="A1:B625"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A608" workbookViewId="0">
-      <selection activeCell="B624" sqref="B624"/>
+      <selection activeCell="B627" sqref="B627"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5911,6 +5911,30 @@
         <v>764.99</v>
       </c>
     </row>
+    <row r="623" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A623" s="2">
+        <v>44086</v>
+      </c>
+      <c r="B623" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="624" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A624" s="2">
+        <v>44087</v>
+      </c>
+      <c r="B624" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="625" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A625" s="2">
+        <v>44088</v>
+      </c>
+      <c r="B625" s="3">
+        <v>768.34</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:B1"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 09-15-2020 17-06-31
</commit_message>
<xml_diff>
--- a/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
+++ b/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\reyes.rodriguezucv@gmail.com\OneDrive\Proyectos\Data intelligence\Covid-19\Chile\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="63" documentId="114_{4E138255-E71E-4AEB-A9EF-82D3D6322094}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{E57204AB-F43E-422A-B153-F7AE3CFF9F07}"/>
+  <xr:revisionPtr revIDLastSave="64" documentId="114_{4E138255-E71E-4AEB-A9EF-82D3D6322094}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{C1759809-1181-4A1F-B0D3-C4FCB0A2D885}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="DOLAR_OBS_ADO" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$625</definedName>
+    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$626</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
@@ -927,10 +927,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B625"/>
+  <dimension ref="A1:B626"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A608" workbookViewId="0">
-      <selection activeCell="B627" sqref="B627"/>
+    <sheetView tabSelected="1" topLeftCell="A614" workbookViewId="0">
+      <selection activeCell="B628" sqref="B628"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5935,6 +5935,14 @@
         <v>768.34</v>
       </c>
     </row>
+    <row r="626" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A626" s="2">
+        <v>44089</v>
+      </c>
+      <c r="B626" s="3">
+        <v>767.01</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:B1"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 09-17-2020 17-07-13
</commit_message>
<xml_diff>
--- a/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
+++ b/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/944d5b9328a00097/Proyectos/Data intelligence/Covid-19/Chile/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID CL/IndicadoresEconomicos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="65" documentId="114_{4E138255-E71E-4AEB-A9EF-82D3D6322094}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{4BDB719B-E97E-4E59-AD30-133D54650E5B}"/>
+  <xr:revisionPtr revIDLastSave="66" documentId="114_{4E138255-E71E-4AEB-A9EF-82D3D6322094}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{0BEA353F-C9AC-4DF8-A443-C735088BD9BF}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="DOLAR_OBS_ADO" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$627</definedName>
+    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$628</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
@@ -927,10 +927,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B627"/>
+  <dimension ref="A1:B628"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A614" workbookViewId="0">
-      <selection activeCell="B626" sqref="B626"/>
+      <selection activeCell="D625" sqref="D625"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5951,6 +5951,14 @@
         <v>760.01</v>
       </c>
     </row>
+    <row r="628" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A628" s="2">
+        <v>44091</v>
+      </c>
+      <c r="B628" s="3">
+        <v>761.54</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:B1"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 09-18-2020 17-14-10
</commit_message>
<xml_diff>
--- a/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
+++ b/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID CL/IndicadoresEconomicos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="66" documentId="114_{4E138255-E71E-4AEB-A9EF-82D3D6322094}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{0BEA353F-C9AC-4DF8-A443-C735088BD9BF}"/>
+  <xr:revisionPtr revIDLastSave="67" documentId="114_{4E138255-E71E-4AEB-A9EF-82D3D6322094}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{283AB556-C53C-4F15-9BEF-767A390194F0}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="DOLAR_OBS_ADO" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$628</definedName>
+    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$632</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="5">
   <si>
     <t>Tipos de cambio (pesos por dólar)</t>
   </si>
@@ -927,10 +927,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B628"/>
+  <dimension ref="A1:B632"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A614" workbookViewId="0">
-      <selection activeCell="D625" sqref="D625"/>
+    <sheetView tabSelected="1" topLeftCell="A623" workbookViewId="0">
+      <selection activeCell="B635" sqref="B635"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5959,6 +5959,38 @@
         <v>761.54</v>
       </c>
     </row>
+    <row r="629" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A629" s="2">
+        <v>44092</v>
+      </c>
+      <c r="B629" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="630" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A630" s="2">
+        <v>44093</v>
+      </c>
+      <c r="B630" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="631" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A631" s="2">
+        <v>44094</v>
+      </c>
+      <c r="B631" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="632" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A632" s="2">
+        <v>44095</v>
+      </c>
+      <c r="B632" s="3">
+        <v>764.34</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:B1"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 09-22-2020 17-13-40
</commit_message>
<xml_diff>
--- a/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
+++ b/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID CL/IndicadoresEconomicos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="67" documentId="114_{4E138255-E71E-4AEB-A9EF-82D3D6322094}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{283AB556-C53C-4F15-9BEF-767A390194F0}"/>
+  <xr:revisionPtr revIDLastSave="68" documentId="114_{4E138255-E71E-4AEB-A9EF-82D3D6322094}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{BDC02A4F-BB4B-45E8-BB49-4257F555C3F7}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="DOLAR_OBS_ADO" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$632</definedName>
+    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$633</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
@@ -927,10 +927,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B632"/>
+  <dimension ref="A1:B633"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A623" workbookViewId="0">
-      <selection activeCell="B635" sqref="B635"/>
+      <selection activeCell="B636" sqref="B636"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5991,6 +5991,14 @@
         <v>764.34</v>
       </c>
     </row>
+    <row r="633" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A633" s="2">
+        <v>44096</v>
+      </c>
+      <c r="B633" s="3">
+        <v>772.83</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:B1"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 09-23-2020 17-07-58
</commit_message>
<xml_diff>
--- a/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
+++ b/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID CL/IndicadoresEconomicos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="68" documentId="114_{4E138255-E71E-4AEB-A9EF-82D3D6322094}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{BDC02A4F-BB4B-45E8-BB49-4257F555C3F7}"/>
+  <xr:revisionPtr revIDLastSave="69" documentId="114_{4E138255-E71E-4AEB-A9EF-82D3D6322094}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{8ACA35AA-944B-469D-874D-F3C532A97449}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="DOLAR_OBS_ADO" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$633</definedName>
+    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$634</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
@@ -927,7 +927,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B633"/>
+  <dimension ref="A1:B634"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A623" workbookViewId="0">
       <selection activeCell="B636" sqref="B636"/>
@@ -5999,6 +5999,14 @@
         <v>772.83</v>
       </c>
     </row>
+    <row r="634" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A634" s="2">
+        <v>44097</v>
+      </c>
+      <c r="B634" s="3">
+        <v>773.4</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:B1"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 09-24-2020 17-10-51
</commit_message>
<xml_diff>
--- a/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
+++ b/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID CL/IndicadoresEconomicos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="69" documentId="114_{4E138255-E71E-4AEB-A9EF-82D3D6322094}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{8ACA35AA-944B-469D-874D-F3C532A97449}"/>
+  <xr:revisionPtr revIDLastSave="70" documentId="114_{4E138255-E71E-4AEB-A9EF-82D3D6322094}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{1DF0825B-5A58-4CA9-853C-8A268AFA2C1D}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7395" yWindow="1125" windowWidth="13095" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DOLAR_OBS_ADO" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$634</definedName>
+    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$635</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
@@ -927,10 +927,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B634"/>
+  <dimension ref="A1:B635"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A623" workbookViewId="0">
-      <selection activeCell="B636" sqref="B636"/>
+      <selection activeCell="B637" sqref="B637"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6007,6 +6007,14 @@
         <v>773.4</v>
       </c>
     </row>
+    <row r="635" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A635" s="2">
+        <v>44098</v>
+      </c>
+      <c r="B635" s="3">
+        <v>781.44</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:B1"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 09-25-2020 17-10-21
</commit_message>
<xml_diff>
--- a/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
+++ b/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID CL/IndicadoresEconomicos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="70" documentId="114_{4E138255-E71E-4AEB-A9EF-82D3D6322094}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{1DF0825B-5A58-4CA9-853C-8A268AFA2C1D}"/>
+  <xr:revisionPtr revIDLastSave="71" documentId="114_{4E138255-E71E-4AEB-A9EF-82D3D6322094}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{022A08D4-58D4-4A4D-AB40-D86655FB4DC1}"/>
   <bookViews>
-    <workbookView xWindow="7395" yWindow="1125" windowWidth="13095" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DOLAR_OBS_ADO" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$635</definedName>
+    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$636</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
@@ -927,10 +927,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B635"/>
+  <dimension ref="A1:B636"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A623" workbookViewId="0">
-      <selection activeCell="B637" sqref="B637"/>
+      <selection activeCell="B639" sqref="B639"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6015,6 +6015,14 @@
         <v>781.44</v>
       </c>
     </row>
+    <row r="636" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A636" s="2">
+        <v>44099</v>
+      </c>
+      <c r="B636" s="3">
+        <v>788.02</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:B1"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 09-26-2020 17-11-39
</commit_message>
<xml_diff>
--- a/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
+++ b/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID CL/IndicadoresEconomicos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="71" documentId="114_{4E138255-E71E-4AEB-A9EF-82D3D6322094}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{022A08D4-58D4-4A4D-AB40-D86655FB4DC1}"/>
+  <xr:revisionPtr revIDLastSave="72" documentId="114_{4E138255-E71E-4AEB-A9EF-82D3D6322094}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{C51E312D-5C83-4101-9C89-6E9974EC98B3}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="DOLAR_OBS_ADO" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$636</definedName>
+    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$639</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="5">
   <si>
     <t>Tipos de cambio (pesos por dólar)</t>
   </si>
@@ -927,10 +927,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B636"/>
+  <dimension ref="A1:B639"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A623" workbookViewId="0">
-      <selection activeCell="B639" sqref="B639"/>
+    <sheetView tabSelected="1" topLeftCell="A635" workbookViewId="0">
+      <selection activeCell="B643" sqref="B643"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6023,6 +6023,30 @@
         <v>788.02</v>
       </c>
     </row>
+    <row r="637" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A637" s="2">
+        <v>44100</v>
+      </c>
+      <c r="B637" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="638" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A638" s="2">
+        <v>44101</v>
+      </c>
+      <c r="B638" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="639" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A639" s="2">
+        <v>44102</v>
+      </c>
+      <c r="B639" s="3">
+        <v>787.15</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:B1"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 09-29-2020 17-08-21
</commit_message>
<xml_diff>
--- a/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
+++ b/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID CL/IndicadoresEconomicos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="72" documentId="114_{4E138255-E71E-4AEB-A9EF-82D3D6322094}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{C51E312D-5C83-4101-9C89-6E9974EC98B3}"/>
+  <xr:revisionPtr revIDLastSave="73" documentId="114_{4E138255-E71E-4AEB-A9EF-82D3D6322094}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{36730CA3-7E07-458A-AD94-18326FFB085A}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="DOLAR_OBS_ADO" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$639</definedName>
+    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$640</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
@@ -927,7 +927,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B639"/>
+  <dimension ref="A1:B640"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A635" workbookViewId="0">
       <selection activeCell="B643" sqref="B643"/>
@@ -6047,6 +6047,14 @@
         <v>787.15</v>
       </c>
     </row>
+    <row r="640" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A640" s="2">
+        <v>44103</v>
+      </c>
+      <c r="B640" s="3">
+        <v>784.19</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:B1"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 09-30-2020 17-09-53
</commit_message>
<xml_diff>
--- a/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
+++ b/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID CL/IndicadoresEconomicos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="73" documentId="114_{4E138255-E71E-4AEB-A9EF-82D3D6322094}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{36730CA3-7E07-458A-AD94-18326FFB085A}"/>
+  <xr:revisionPtr revIDLastSave="74" documentId="114_{4E138255-E71E-4AEB-A9EF-82D3D6322094}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{7C6BF6CA-6595-4F83-86C8-DA6D1674E96F}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="DOLAR_OBS_ADO" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$640</definedName>
+    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$641</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
@@ -927,7 +927,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B640"/>
+  <dimension ref="A1:B641"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A635" workbookViewId="0">
       <selection activeCell="B643" sqref="B643"/>
@@ -6055,6 +6055,14 @@
         <v>784.19</v>
       </c>
     </row>
+    <row r="641" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A641" s="2">
+        <v>44104</v>
+      </c>
+      <c r="B641" s="3">
+        <v>784.46</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:B1"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 10-01-2020 17-11-16
</commit_message>
<xml_diff>
--- a/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
+++ b/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID CL/IndicadoresEconomicos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="74" documentId="114_{4E138255-E71E-4AEB-A9EF-82D3D6322094}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{7C6BF6CA-6595-4F83-86C8-DA6D1674E96F}"/>
+  <xr:revisionPtr revIDLastSave="75" documentId="114_{4E138255-E71E-4AEB-A9EF-82D3D6322094}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{71FC8B6A-2A6E-4D0E-9795-02A7DB6A4FD9}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="DOLAR_OBS_ADO" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$641</definedName>
+    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$642</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
@@ -927,10 +927,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B641"/>
+  <dimension ref="A1:B642"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A635" workbookViewId="0">
-      <selection activeCell="B643" sqref="B643"/>
+      <selection activeCell="B641" sqref="B641"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6063,6 +6063,14 @@
         <v>784.46</v>
       </c>
     </row>
+    <row r="642" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A642" s="2">
+        <v>44105</v>
+      </c>
+      <c r="B642" s="3">
+        <v>788.15</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:B1"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 10-02-2020 17-09-03
</commit_message>
<xml_diff>
--- a/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
+++ b/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID CL/IndicadoresEconomicos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="75" documentId="114_{4E138255-E71E-4AEB-A9EF-82D3D6322094}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{71FC8B6A-2A6E-4D0E-9795-02A7DB6A4FD9}"/>
+  <xr:revisionPtr revIDLastSave="76" documentId="114_{4E138255-E71E-4AEB-A9EF-82D3D6322094}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{33D2FA01-0999-4B04-BEB8-85327C5F5CCE}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="DOLAR_OBS_ADO" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$642</definedName>
+    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$643</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
@@ -927,10 +927,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B642"/>
+  <dimension ref="A1:B643"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A635" workbookViewId="0">
-      <selection activeCell="B641" sqref="B641"/>
+    <sheetView tabSelected="1" topLeftCell="A639" workbookViewId="0">
+      <selection activeCell="B646" sqref="B646"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6071,6 +6071,14 @@
         <v>788.15</v>
       </c>
     </row>
+    <row r="643" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A643" s="2">
+        <v>44106</v>
+      </c>
+      <c r="B643" s="3">
+        <v>785.04</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:B1"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 10-03-2020 17-13-06
</commit_message>
<xml_diff>
--- a/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
+++ b/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID CL/IndicadoresEconomicos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="76" documentId="114_{4E138255-E71E-4AEB-A9EF-82D3D6322094}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{33D2FA01-0999-4B04-BEB8-85327C5F5CCE}"/>
+  <xr:revisionPtr revIDLastSave="77" documentId="114_{4E138255-E71E-4AEB-A9EF-82D3D6322094}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{C45EF5C2-4D42-47AF-BF4B-B693E0BB8F48}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="DOLAR_OBS_ADO" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$643</definedName>
+    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$646</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="5">
   <si>
     <t>Tipos de cambio (pesos por dólar)</t>
   </si>
@@ -927,7 +927,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B643"/>
+  <dimension ref="A1:B646"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A639" workbookViewId="0">
       <selection activeCell="B646" sqref="B646"/>
@@ -6079,6 +6079,30 @@
         <v>785.04</v>
       </c>
     </row>
+    <row r="644" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A644" s="2">
+        <v>44107</v>
+      </c>
+      <c r="B644" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="645" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A645" s="2">
+        <v>44108</v>
+      </c>
+      <c r="B645" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="646" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A646" s="2">
+        <v>44109</v>
+      </c>
+      <c r="B646" s="3">
+        <v>790.81</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:B1"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 10-14-2020 17-33-01
</commit_message>
<xml_diff>
--- a/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
+++ b/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID CL/IndicadoresEconomicos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="77" documentId="114_{4E138255-E71E-4AEB-A9EF-82D3D6322094}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{C45EF5C2-4D42-47AF-BF4B-B693E0BB8F48}"/>
+  <xr:revisionPtr revIDLastSave="83" documentId="114_{4E138255-E71E-4AEB-A9EF-82D3D6322094}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{3024AA0B-0C96-4EB9-AFD4-520836306398}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="DOLAR_OBS_ADO" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$646</definedName>
+    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$655</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="5">
   <si>
     <t>Tipos de cambio (pesos por dólar)</t>
   </si>
@@ -927,10 +927,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B646"/>
+  <dimension ref="A1:B655"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A639" workbookViewId="0">
-      <selection activeCell="B646" sqref="B646"/>
+    <sheetView tabSelected="1" topLeftCell="A649" workbookViewId="0">
+      <selection activeCell="B658" sqref="B658"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6103,6 +6103,78 @@
         <v>790.81</v>
       </c>
     </row>
+    <row r="647" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A647" s="2">
+        <v>44110</v>
+      </c>
+      <c r="B647" s="3">
+        <v>794.34</v>
+      </c>
+    </row>
+    <row r="648" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A648" s="2">
+        <v>44111</v>
+      </c>
+      <c r="B648" s="3">
+        <v>797.35</v>
+      </c>
+    </row>
+    <row r="649" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A649" s="2">
+        <v>44112</v>
+      </c>
+      <c r="B649" s="3">
+        <v>795.05</v>
+      </c>
+    </row>
+    <row r="650" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A650" s="2">
+        <v>44113</v>
+      </c>
+      <c r="B650" s="3">
+        <v>797.25</v>
+      </c>
+    </row>
+    <row r="651" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A651" s="2">
+        <v>44114</v>
+      </c>
+      <c r="B651" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="652" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A652" s="2">
+        <v>44115</v>
+      </c>
+      <c r="B652" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="653" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A653" s="2">
+        <v>44116</v>
+      </c>
+      <c r="B653" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="654" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A654" s="2">
+        <v>44117</v>
+      </c>
+      <c r="B654" s="3">
+        <v>796.05</v>
+      </c>
+    </row>
+    <row r="655" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A655" s="2">
+        <v>44118</v>
+      </c>
+      <c r="B655" s="3">
+        <v>797.66</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:B1"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 10-16-2020 19-33-34
</commit_message>
<xml_diff>
--- a/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
+++ b/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID CL/IndicadoresEconomicos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="83" documentId="114_{4E138255-E71E-4AEB-A9EF-82D3D6322094}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{3024AA0B-0C96-4EB9-AFD4-520836306398}"/>
+  <xr:revisionPtr revIDLastSave="85" documentId="114_{4E138255-E71E-4AEB-A9EF-82D3D6322094}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{43456E14-DB13-42C9-9A5B-6F3DF669B8F8}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="DOLAR_OBS_ADO" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$655</definedName>
+    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$657</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
@@ -927,10 +927,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B655"/>
+  <dimension ref="A1:B657"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A649" workbookViewId="0">
-      <selection activeCell="B658" sqref="B658"/>
+      <selection activeCell="B660" sqref="B660"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6175,6 +6175,22 @@
         <v>797.66</v>
       </c>
     </row>
+    <row r="656" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A656" s="2">
+        <v>44119</v>
+      </c>
+      <c r="B656" s="3">
+        <v>798.56</v>
+      </c>
+    </row>
+    <row r="657" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A657" s="2">
+        <v>44120</v>
+      </c>
+      <c r="B657" s="3">
+        <v>801.91</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:B1"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 10-17-2020 17-05-40
</commit_message>
<xml_diff>
--- a/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
+++ b/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID CL/IndicadoresEconomicos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="85" documentId="114_{4E138255-E71E-4AEB-A9EF-82D3D6322094}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{43456E14-DB13-42C9-9A5B-6F3DF669B8F8}"/>
+  <xr:revisionPtr revIDLastSave="86" documentId="114_{4E138255-E71E-4AEB-A9EF-82D3D6322094}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{E6DFE6C9-59A9-4A36-BD42-F3FC183CDA3F}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="DOLAR_OBS_ADO" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$657</definedName>
+    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$660</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="5">
   <si>
     <t>Tipos de cambio (pesos por dólar)</t>
   </si>
@@ -927,10 +927,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B657"/>
+  <dimension ref="A1:B660"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A649" workbookViewId="0">
-      <selection activeCell="B660" sqref="B660"/>
+      <selection activeCell="B662" sqref="B662"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6191,6 +6191,30 @@
         <v>801.91</v>
       </c>
     </row>
+    <row r="658" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A658" s="2">
+        <v>44121</v>
+      </c>
+      <c r="B658" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="659" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A659" s="2">
+        <v>44122</v>
+      </c>
+      <c r="B659" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="660" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A660" s="2">
+        <v>44123</v>
+      </c>
+      <c r="B660" s="3">
+        <v>795.68</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:B1"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 10-20-2020 17-06-25
</commit_message>
<xml_diff>
--- a/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
+++ b/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID CL/IndicadoresEconomicos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="86" documentId="114_{4E138255-E71E-4AEB-A9EF-82D3D6322094}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{E6DFE6C9-59A9-4A36-BD42-F3FC183CDA3F}"/>
+  <xr:revisionPtr revIDLastSave="87" documentId="114_{4E138255-E71E-4AEB-A9EF-82D3D6322094}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{2AFF8357-9964-475E-8E5B-FE2B81087D66}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="DOLAR_OBS_ADO" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$660</definedName>
+    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$661</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
@@ -927,7 +927,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B660"/>
+  <dimension ref="A1:B661"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A649" workbookViewId="0">
       <selection activeCell="B662" sqref="B662"/>
@@ -6215,6 +6215,14 @@
         <v>795.68</v>
       </c>
     </row>
+    <row r="661" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A661" s="2">
+        <v>44124</v>
+      </c>
+      <c r="B661" s="3">
+        <v>788.27</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:B1"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 10-21-2020 17-05-57
</commit_message>
<xml_diff>
--- a/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
+++ b/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID CL/IndicadoresEconomicos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="87" documentId="114_{4E138255-E71E-4AEB-A9EF-82D3D6322094}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{2AFF8357-9964-475E-8E5B-FE2B81087D66}"/>
+  <xr:revisionPtr revIDLastSave="88" documentId="114_{4E138255-E71E-4AEB-A9EF-82D3D6322094}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{53C1217C-3964-4C12-8B76-7DFC6BBCC65F}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="DOLAR_OBS_ADO" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$661</definedName>
+    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$662</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
@@ -927,10 +927,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B661"/>
+  <dimension ref="A1:B662"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A649" workbookViewId="0">
-      <selection activeCell="B662" sqref="B662"/>
+    <sheetView tabSelected="1" topLeftCell="A655" workbookViewId="0">
+      <selection activeCell="B664" sqref="B664"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6223,6 +6223,14 @@
         <v>788.27</v>
       </c>
     </row>
+    <row r="662" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A662" s="2">
+        <v>44125</v>
+      </c>
+      <c r="B662" s="3">
+        <v>786.66</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:B1"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 10-22-2020 17-09-22
</commit_message>
<xml_diff>
--- a/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
+++ b/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID CL/IndicadoresEconomicos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="88" documentId="114_{4E138255-E71E-4AEB-A9EF-82D3D6322094}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{53C1217C-3964-4C12-8B76-7DFC6BBCC65F}"/>
+  <xr:revisionPtr revIDLastSave="89" documentId="114_{4E138255-E71E-4AEB-A9EF-82D3D6322094}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{F8AF192C-1E4D-4572-849E-28751A3C2214}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="DOLAR_OBS_ADO" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$662</definedName>
+    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$663</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
@@ -927,10 +927,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B662"/>
+  <dimension ref="A1:B663"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A655" workbookViewId="0">
-      <selection activeCell="B664" sqref="B664"/>
+      <selection activeCell="B662" sqref="B662"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6231,6 +6231,14 @@
         <v>786.66</v>
       </c>
     </row>
+    <row r="663" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A663" s="2">
+        <v>44126</v>
+      </c>
+      <c r="B663" s="3">
+        <v>784.07</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:B1"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 10-23-2020 17-05-07
</commit_message>
<xml_diff>
--- a/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
+++ b/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID CL/IndicadoresEconomicos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="89" documentId="114_{4E138255-E71E-4AEB-A9EF-82D3D6322094}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{F8AF192C-1E4D-4572-849E-28751A3C2214}"/>
+  <xr:revisionPtr revIDLastSave="90" documentId="114_{4E138255-E71E-4AEB-A9EF-82D3D6322094}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{3F910BEF-684C-4A79-B735-492AA61E80E9}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="DOLAR_OBS_ADO" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$663</definedName>
+    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$664</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
@@ -927,10 +927,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B663"/>
+  <dimension ref="A1:B664"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A655" workbookViewId="0">
-      <selection activeCell="B662" sqref="B662"/>
+      <selection activeCell="B664" sqref="B664"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6239,6 +6239,14 @@
         <v>784.07</v>
       </c>
     </row>
+    <row r="664" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A664" s="2">
+        <v>44127</v>
+      </c>
+      <c r="B664" s="3">
+        <v>781.41</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:B1"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 10-24-2020 17-09-36
</commit_message>
<xml_diff>
--- a/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
+++ b/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID CL/IndicadoresEconomicos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="90" documentId="114_{4E138255-E71E-4AEB-A9EF-82D3D6322094}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{3F910BEF-684C-4A79-B735-492AA61E80E9}"/>
+  <xr:revisionPtr revIDLastSave="92" documentId="114_{4E138255-E71E-4AEB-A9EF-82D3D6322094}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{878B4BB8-4A90-4BDD-B684-B673B7A69A38}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="DOLAR_OBS_ADO" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$664</definedName>
+    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$667</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="5">
   <si>
     <t>Tipos de cambio (pesos por dólar)</t>
   </si>
@@ -927,10 +927,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B664"/>
+  <dimension ref="A1:B667"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A655" workbookViewId="0">
-      <selection activeCell="B664" sqref="B664"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="4" topLeftCell="B665" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
+      <selection pane="bottomRight" activeCell="B667" sqref="B667"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6247,6 +6250,30 @@
         <v>781.41</v>
       </c>
     </row>
+    <row r="665" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A665" s="2">
+        <v>44128</v>
+      </c>
+      <c r="B665" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="666" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A666" s="2">
+        <v>44129</v>
+      </c>
+      <c r="B666" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="667" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A667" s="2">
+        <v>44130</v>
+      </c>
+      <c r="B667" s="3">
+        <v>777.72</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:B1"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 10-27-2020 17-08-40
</commit_message>
<xml_diff>
--- a/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
+++ b/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID CL/IndicadoresEconomicos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="92" documentId="114_{4E138255-E71E-4AEB-A9EF-82D3D6322094}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{878B4BB8-4A90-4BDD-B684-B673B7A69A38}"/>
+  <xr:revisionPtr revIDLastSave="93" documentId="114_{4E138255-E71E-4AEB-A9EF-82D3D6322094}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{DFAFB79E-3371-4946-8ABA-781E2412CF0E}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="16185" windowHeight="10140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DOLAR_OBS_ADO" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$667</definedName>
+    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$668</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
@@ -927,13 +927,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B667"/>
+  <dimension ref="A1:B668"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="4" topLeftCell="B665" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="B667" sqref="B667"/>
+      <selection pane="bottomRight" activeCell="B668" sqref="B668"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6274,6 +6274,14 @@
         <v>777.72</v>
       </c>
     </row>
+    <row r="668" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A668" s="2">
+        <v>44131</v>
+      </c>
+      <c r="B668" s="3">
+        <v>779.57</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:B1"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 10-28-2020 17-14-21
</commit_message>
<xml_diff>
--- a/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
+++ b/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID CL/IndicadoresEconomicos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="93" documentId="114_{4E138255-E71E-4AEB-A9EF-82D3D6322094}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{DFAFB79E-3371-4946-8ABA-781E2412CF0E}"/>
+  <xr:revisionPtr revIDLastSave="94" documentId="114_{4E138255-E71E-4AEB-A9EF-82D3D6322094}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{697528FD-585C-4523-99A9-57C999D18650}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="390" windowWidth="16185" windowHeight="10140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DOLAR_OBS_ADO" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$668</definedName>
+    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$669</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
@@ -927,13 +927,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B668"/>
+  <dimension ref="A1:B669"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="4" topLeftCell="B665" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="B668" sqref="B668"/>
+      <selection pane="bottomRight" activeCell="B669" sqref="B669"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6282,6 +6282,14 @@
         <v>779.57</v>
       </c>
     </row>
+    <row r="669" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A669" s="2">
+        <v>44132</v>
+      </c>
+      <c r="B669" s="3">
+        <v>772.05</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:B1"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 10-29-2020 17-10-27
</commit_message>
<xml_diff>
--- a/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
+++ b/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID CL/IndicadoresEconomicos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="94" documentId="114_{4E138255-E71E-4AEB-A9EF-82D3D6322094}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{697528FD-585C-4523-99A9-57C999D18650}"/>
+  <xr:revisionPtr revIDLastSave="95" documentId="114_{4E138255-E71E-4AEB-A9EF-82D3D6322094}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{ABC83DE1-92E6-42E8-B831-035FF206AE6C}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="DOLAR_OBS_ADO" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$669</definedName>
+    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$670</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
@@ -927,13 +927,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B669"/>
+  <dimension ref="A1:B670"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="4" topLeftCell="B665" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="B669" sqref="B669"/>
+      <selection pane="bottomRight" activeCell="B670" sqref="B670"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6290,6 +6290,14 @@
         <v>772.05</v>
       </c>
     </row>
+    <row r="670" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A670" s="2">
+        <v>44133</v>
+      </c>
+      <c r="B670" s="3">
+        <v>775.56</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:B1"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 10-30-2020 17-05-19
</commit_message>
<xml_diff>
--- a/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
+++ b/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID CL/IndicadoresEconomicos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="95" documentId="114_{4E138255-E71E-4AEB-A9EF-82D3D6322094}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{ABC83DE1-92E6-42E8-B831-035FF206AE6C}"/>
+  <xr:revisionPtr revIDLastSave="96" documentId="114_{4E138255-E71E-4AEB-A9EF-82D3D6322094}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{C225FB2C-41A8-4265-A0EE-59B01DF9F135}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="DOLAR_OBS_ADO" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$670</definedName>
+    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$671</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
@@ -927,13 +927,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B670"/>
+  <dimension ref="A1:B671"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="4" topLeftCell="B665" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="B670" sqref="B670"/>
+      <selection pane="bottomRight" activeCell="B671" sqref="B671"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6298,6 +6298,14 @@
         <v>775.56</v>
       </c>
     </row>
+    <row r="671" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A671" s="2">
+        <v>44134</v>
+      </c>
+      <c r="B671" s="3">
+        <v>770.45</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:B1"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 10-31-2020 17-12-53
</commit_message>
<xml_diff>
--- a/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
+++ b/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID CL/IndicadoresEconomicos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="96" documentId="114_{4E138255-E71E-4AEB-A9EF-82D3D6322094}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{C225FB2C-41A8-4265-A0EE-59B01DF9F135}"/>
+  <xr:revisionPtr revIDLastSave="98" documentId="114_{4E138255-E71E-4AEB-A9EF-82D3D6322094}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{BF662A59-052F-4E03-9047-95F5AEF5DCD0}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="DOLAR_OBS_ADO" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$671</definedName>
+    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$674</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="5">
   <si>
     <t>Tipos de cambio (pesos por dólar)</t>
   </si>
@@ -927,13 +927,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B671"/>
+  <dimension ref="A1:B674"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="4" topLeftCell="B665" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="4" topLeftCell="B659" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="B671" sqref="B671"/>
+      <selection pane="bottomRight" activeCell="B674" sqref="B674"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6306,6 +6306,30 @@
         <v>770.45</v>
       </c>
     </row>
+    <row r="672" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A672" s="2">
+        <v>44135</v>
+      </c>
+      <c r="B672" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="673" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A673" s="2">
+        <v>44136</v>
+      </c>
+      <c r="B673" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="674" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A674" s="2">
+        <v>44137</v>
+      </c>
+      <c r="B674" s="3">
+        <v>771.92</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:B1"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 11-03-2020 17-08-01
</commit_message>
<xml_diff>
--- a/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
+++ b/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID CL/IndicadoresEconomicos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="98" documentId="114_{4E138255-E71E-4AEB-A9EF-82D3D6322094}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{BF662A59-052F-4E03-9047-95F5AEF5DCD0}"/>
+  <xr:revisionPtr revIDLastSave="102" documentId="114_{4E138255-E71E-4AEB-A9EF-82D3D6322094}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{4964F4A2-AD61-472E-ABCD-A1A95BBF5A2C}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -938,8 +938,8 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.5703125" customWidth="1"/>
-    <col min="2" max="2" width="15.5703125" customWidth="1"/>
+    <col min="1" max="1" width="12.7109375" customWidth="1"/>
+    <col min="2" max="2" width="14.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Update automatico via Actualizar 11-04-2020 23-34-59
</commit_message>
<xml_diff>
--- a/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
+++ b/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID CL/IndicadoresEconomicos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="102" documentId="114_{4E138255-E71E-4AEB-A9EF-82D3D6322094}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{4964F4A2-AD61-472E-ABCD-A1A95BBF5A2C}"/>
+  <xr:revisionPtr revIDLastSave="105" documentId="114_{4E138255-E71E-4AEB-A9EF-82D3D6322094}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{6608BE5E-D8D9-417A-8A31-3A79CAE595DE}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="DOLAR_OBS_ADO" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$674</definedName>
+    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$677</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
@@ -927,19 +927,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B674"/>
+  <dimension ref="A1:B677"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="4" topLeftCell="B659" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="4" topLeftCell="B662" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="B674" sqref="B674"/>
+      <selection pane="bottomRight" activeCell="B677" sqref="B677"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.7109375" customWidth="1"/>
-    <col min="2" max="2" width="14.42578125" customWidth="1"/>
+    <col min="1" max="1" width="11.5703125" customWidth="1"/>
+    <col min="2" max="2" width="15.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -6328,6 +6328,30 @@
       </c>
       <c r="B674" s="3">
         <v>771.92</v>
+      </c>
+    </row>
+    <row r="675" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A675" s="2">
+        <v>44138</v>
+      </c>
+      <c r="B675" s="3">
+        <v>769.17</v>
+      </c>
+    </row>
+    <row r="676" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A676" s="2">
+        <v>44139</v>
+      </c>
+      <c r="B676" s="3">
+        <v>758.53</v>
+      </c>
+    </row>
+    <row r="677" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A677" s="2">
+        <v>44140</v>
+      </c>
+      <c r="B677" s="3">
+        <v>757.16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update automatico via Actualizar 11-06-2020 20-41-25
</commit_message>
<xml_diff>
--- a/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
+++ b/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID CL/IndicadoresEconomicos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="105" documentId="114_{4E138255-E71E-4AEB-A9EF-82D3D6322094}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{6608BE5E-D8D9-417A-8A31-3A79CAE595DE}"/>
+  <xr:revisionPtr revIDLastSave="106" documentId="114_{4E138255-E71E-4AEB-A9EF-82D3D6322094}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{2059CF24-B5C7-4AD0-9F94-878A550394FE}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="DOLAR_OBS_ADO" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$677</definedName>
+    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$678</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
@@ -927,13 +927,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B677"/>
+  <dimension ref="A1:B678"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="4" topLeftCell="B662" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="4" topLeftCell="B671" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="B677" sqref="B677"/>
+      <selection pane="bottomRight" activeCell="B678" sqref="B678"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6354,6 +6354,14 @@
         <v>757.16</v>
       </c>
     </row>
+    <row r="678" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A678" s="2">
+        <v>44141</v>
+      </c>
+      <c r="B678" s="3">
+        <v>752.01</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:B1"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 11-07-2020 17-13-44
</commit_message>
<xml_diff>
--- a/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
+++ b/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID CL/IndicadoresEconomicos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="106" documentId="114_{4E138255-E71E-4AEB-A9EF-82D3D6322094}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{2059CF24-B5C7-4AD0-9F94-878A550394FE}"/>
+  <xr:revisionPtr revIDLastSave="108" documentId="114_{4E138255-E71E-4AEB-A9EF-82D3D6322094}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{B896F2F0-116D-474A-97C0-F12B35DF1B78}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="DOLAR_OBS_ADO" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$678</definedName>
+    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$681</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="5">
   <si>
     <t>Tipos de cambio (pesos por dólar)</t>
   </si>
@@ -927,13 +927,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B678"/>
+  <dimension ref="A1:B681"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="4" topLeftCell="B671" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="B678" sqref="B678"/>
+      <selection pane="bottomRight" activeCell="B681" sqref="B681"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6362,6 +6362,30 @@
         <v>752.01</v>
       </c>
     </row>
+    <row r="679" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A679" s="2">
+        <v>44142</v>
+      </c>
+      <c r="B679" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="680" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A680" s="2">
+        <v>44143</v>
+      </c>
+      <c r="B680" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="681" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A681" s="2">
+        <v>44144</v>
+      </c>
+      <c r="B681" s="3">
+        <v>759.25</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:B1"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 11-12-2020 17-06-29
</commit_message>
<xml_diff>
--- a/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
+++ b/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID CL/IndicadoresEconomicos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="108" documentId="114_{4E138255-E71E-4AEB-A9EF-82D3D6322094}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{B896F2F0-116D-474A-97C0-F12B35DF1B78}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="14_{F2753A6D-642C-43B1-9D50-7716AF012233}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{EB69DD7D-6DC7-40C7-A6EB-3567AAC68B32}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="DOLAR_OBS_ADO" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$681</definedName>
+    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$683</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
@@ -927,13 +927,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B681"/>
+  <dimension ref="A1:B683"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="4" topLeftCell="B671" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="B681" sqref="B681"/>
+      <selection pane="bottomRight" activeCell="B683" sqref="B683"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6386,6 +6386,22 @@
         <v>759.25</v>
       </c>
     </row>
+    <row r="682" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A682" s="2">
+        <v>44145</v>
+      </c>
+      <c r="B682" s="3">
+        <v>753.75</v>
+      </c>
+    </row>
+    <row r="683" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A683" s="2">
+        <v>44146</v>
+      </c>
+      <c r="B683" s="3">
+        <v>760.9</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:B1"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 02-04-2021 19-31-20
</commit_message>
<xml_diff>
--- a/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
+++ b/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID CL/IndicadoresEconomicos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="14_{F2753A6D-642C-43B1-9D50-7716AF012233}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{EB69DD7D-6DC7-40C7-A6EB-3567AAC68B32}"/>
+  <xr:revisionPtr revIDLastSave="125" documentId="13_ncr:1_{C8B25996-B8C9-45E8-BF5F-0058EDDB5306}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{B2D90656-DD48-4ECD-BB23-8C8D4EDECED3}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,9 +16,21 @@
     <sheet name="DOLAR_OBS_ADO" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$683</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">DOLAR_OBS_ADO!$A$3:$B$762</definedName>
+    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$762</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -35,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="5">
   <si>
     <t>Tipos de cambio (pesos por dólar)</t>
   </si>
@@ -56,7 +68,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -202,6 +214,21 @@
       <b/>
       <sz val="10"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -504,7 +531,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="42">
+  <cellStyleXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -547,6 +574,14 @@
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -569,7 +604,7 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="42">
+  <cellStyles count="50">
     <cellStyle name="20% - Énfasis1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Énfasis2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Énfasis3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -583,11 +618,17 @@
     <cellStyle name="40% - Énfasis5" xfId="36" builtinId="47" customBuiltin="1"/>
     <cellStyle name="40% - Énfasis6" xfId="40" builtinId="51" customBuiltin="1"/>
     <cellStyle name="60% - Énfasis1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Énfasis1 2" xfId="42" xr:uid="{4385A8D2-651C-4773-80CB-11F47798F1CE}"/>
     <cellStyle name="60% - Énfasis2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Énfasis2 2" xfId="43" xr:uid="{054221C2-13B6-4754-B0B6-C32A4E8A95AD}"/>
     <cellStyle name="60% - Énfasis3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Énfasis3 2" xfId="44" xr:uid="{BB28A6FF-22BE-46E4-B116-00518D401B6E}"/>
     <cellStyle name="60% - Énfasis4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Énfasis4 2" xfId="45" xr:uid="{D1C02AD5-7A4A-4764-935B-FAB4D7D87EE9}"/>
     <cellStyle name="60% - Énfasis5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Énfasis5 2" xfId="46" xr:uid="{9F6E8D91-7C00-42FF-8A7D-91C893DA4AB8}"/>
     <cellStyle name="60% - Énfasis6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="60% - Énfasis6 2" xfId="47" xr:uid="{1DF80BA0-24DE-4DA9-8EE2-A15003600F7C}"/>
     <cellStyle name="Bueno" xfId="6" builtinId="26" customBuiltin="1"/>
     <cellStyle name="Cálculo" xfId="11" builtinId="22" customBuiltin="1"/>
     <cellStyle name="Celda de comprobación" xfId="13" builtinId="23" customBuiltin="1"/>
@@ -603,6 +644,7 @@
     <cellStyle name="Entrada" xfId="9" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Incorrecto" xfId="7" builtinId="27" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
+    <cellStyle name="Neutral 2" xfId="48" xr:uid="{96B4E413-929F-4319-B3D6-5D1EF8AD0E76}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Notas" xfId="15" builtinId="10" customBuiltin="1"/>
     <cellStyle name="Salida" xfId="10" builtinId="21" customBuiltin="1"/>
@@ -611,6 +653,7 @@
     <cellStyle name="Título" xfId="1" builtinId="15" customBuiltin="1"/>
     <cellStyle name="Título 2" xfId="3" builtinId="17" customBuiltin="1"/>
     <cellStyle name="Título 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Título 4" xfId="49" xr:uid="{072D0298-5CC9-445D-BF36-9D06198D96B3}"/>
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -927,19 +970,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B683"/>
+  <dimension ref="A1:B762"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="4" topLeftCell="B671" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="4" topLeftCell="B761" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="B683" sqref="B683"/>
+      <selection pane="bottomRight" activeCell="B762" sqref="B762"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.5703125" customWidth="1"/>
-    <col min="2" max="2" width="15.5703125" customWidth="1"/>
+    <col min="1" max="1" width="12.7109375" customWidth="1"/>
+    <col min="2" max="2" width="14.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -6400,6 +6443,638 @@
       </c>
       <c r="B683" s="3">
         <v>760.9</v>
+      </c>
+    </row>
+    <row r="684" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A684" s="2">
+        <v>44147</v>
+      </c>
+      <c r="B684" s="3">
+        <v>757.42</v>
+      </c>
+    </row>
+    <row r="685" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A685" s="2">
+        <v>44148</v>
+      </c>
+      <c r="B685" s="3">
+        <v>757.43</v>
+      </c>
+    </row>
+    <row r="686" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A686" s="2">
+        <v>44149</v>
+      </c>
+      <c r="B686" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="687" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A687" s="2">
+        <v>44150</v>
+      </c>
+      <c r="B687" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="688" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A688" s="2">
+        <v>44151</v>
+      </c>
+      <c r="B688" s="3">
+        <v>766.7</v>
+      </c>
+    </row>
+    <row r="689" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A689" s="2">
+        <v>44152</v>
+      </c>
+      <c r="B689" s="3">
+        <v>767.86</v>
+      </c>
+    </row>
+    <row r="690" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A690" s="2">
+        <v>44153</v>
+      </c>
+      <c r="B690" s="3">
+        <v>767.05</v>
+      </c>
+    </row>
+    <row r="691" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A691" s="2">
+        <v>44154</v>
+      </c>
+      <c r="B691" s="3">
+        <v>758.1</v>
+      </c>
+    </row>
+    <row r="692" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A692" s="2">
+        <v>44155</v>
+      </c>
+      <c r="B692" s="3">
+        <v>758.62</v>
+      </c>
+    </row>
+    <row r="693" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A693" s="2">
+        <v>44156</v>
+      </c>
+      <c r="B693" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="694" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A694" s="2">
+        <v>44157</v>
+      </c>
+      <c r="B694" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="695" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A695" s="2">
+        <v>44158</v>
+      </c>
+      <c r="B695" s="3">
+        <v>761.55</v>
+      </c>
+    </row>
+    <row r="696" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A696" s="2">
+        <v>44159</v>
+      </c>
+      <c r="B696" s="3">
+        <v>765.96</v>
+      </c>
+    </row>
+    <row r="697" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A697" s="2">
+        <v>44160</v>
+      </c>
+      <c r="B697" s="3">
+        <v>772.83</v>
+      </c>
+    </row>
+    <row r="698" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A698" s="2">
+        <v>44161</v>
+      </c>
+      <c r="B698" s="3">
+        <v>771.68</v>
+      </c>
+    </row>
+    <row r="699" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A699" s="2">
+        <v>44162</v>
+      </c>
+      <c r="B699" s="3">
+        <v>766</v>
+      </c>
+    </row>
+    <row r="700" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A700" s="2">
+        <v>44163</v>
+      </c>
+      <c r="B700" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="701" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A701" s="2">
+        <v>44164</v>
+      </c>
+      <c r="B701" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="702" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A702" s="2">
+        <v>44165</v>
+      </c>
+      <c r="B702" s="3">
+        <v>766.69</v>
+      </c>
+    </row>
+    <row r="703" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A703" s="2">
+        <v>44166</v>
+      </c>
+      <c r="B703" s="3">
+        <v>767.29</v>
+      </c>
+    </row>
+    <row r="704" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A704" s="2">
+        <v>44167</v>
+      </c>
+      <c r="B704" s="3">
+        <v>760.16</v>
+      </c>
+    </row>
+    <row r="705" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A705" s="2">
+        <v>44168</v>
+      </c>
+      <c r="B705" s="3">
+        <v>755.34</v>
+      </c>
+    </row>
+    <row r="706" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A706" s="2">
+        <v>44169</v>
+      </c>
+      <c r="B706" s="3">
+        <v>752.03</v>
+      </c>
+    </row>
+    <row r="707" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A707" s="2">
+        <v>44170</v>
+      </c>
+      <c r="B707" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="708" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A708" s="2">
+        <v>44171</v>
+      </c>
+      <c r="B708" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="709" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A709" s="2">
+        <v>44172</v>
+      </c>
+      <c r="B709" s="3">
+        <v>747.61</v>
+      </c>
+    </row>
+    <row r="710" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A710" s="2">
+        <v>44173</v>
+      </c>
+      <c r="B710" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="711" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A711" s="2">
+        <v>44174</v>
+      </c>
+      <c r="B711" s="3">
+        <v>744.82</v>
+      </c>
+    </row>
+    <row r="712" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A712" s="2">
+        <v>44175</v>
+      </c>
+      <c r="B712" s="3">
+        <v>739.45</v>
+      </c>
+    </row>
+    <row r="713" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A713" s="2">
+        <v>44176</v>
+      </c>
+      <c r="B713" s="3">
+        <v>738.17</v>
+      </c>
+    </row>
+    <row r="714" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A714" s="2">
+        <v>44177</v>
+      </c>
+      <c r="B714" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="715" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A715" s="2">
+        <v>44178</v>
+      </c>
+      <c r="B715" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="716" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A716" s="2">
+        <v>44179</v>
+      </c>
+      <c r="B716" s="3">
+        <v>733.55</v>
+      </c>
+    </row>
+    <row r="717" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A717" s="2">
+        <v>44180</v>
+      </c>
+      <c r="B717" s="3">
+        <v>731.58</v>
+      </c>
+    </row>
+    <row r="718" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A718" s="2">
+        <v>44181</v>
+      </c>
+      <c r="B718" s="3">
+        <v>734.23</v>
+      </c>
+    </row>
+    <row r="719" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A719" s="2">
+        <v>44182</v>
+      </c>
+      <c r="B719" s="3">
+        <v>735.09</v>
+      </c>
+    </row>
+    <row r="720" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A720" s="2">
+        <v>44183</v>
+      </c>
+      <c r="B720" s="3">
+        <v>723.44</v>
+      </c>
+    </row>
+    <row r="721" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A721" s="2">
+        <v>44184</v>
+      </c>
+      <c r="B721" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="722" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A722" s="2">
+        <v>44185</v>
+      </c>
+      <c r="B722" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="723" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A723" s="2">
+        <v>44186</v>
+      </c>
+      <c r="B723" s="3">
+        <v>723.85</v>
+      </c>
+    </row>
+    <row r="724" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A724" s="2">
+        <v>44187</v>
+      </c>
+      <c r="B724" s="3">
+        <v>730.7</v>
+      </c>
+    </row>
+    <row r="725" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A725" s="2">
+        <v>44188</v>
+      </c>
+      <c r="B725" s="3">
+        <v>728.96</v>
+      </c>
+    </row>
+    <row r="726" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A726" s="2">
+        <v>44189</v>
+      </c>
+      <c r="B726" s="3">
+        <v>716.25</v>
+      </c>
+    </row>
+    <row r="727" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A727" s="2">
+        <v>44190</v>
+      </c>
+      <c r="B727" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="728" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A728" s="2">
+        <v>44191</v>
+      </c>
+      <c r="B728" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="729" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A729" s="2">
+        <v>44192</v>
+      </c>
+      <c r="B729" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="730" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A730" s="2">
+        <v>44193</v>
+      </c>
+      <c r="B730" s="3">
+        <v>710.26</v>
+      </c>
+    </row>
+    <row r="731" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A731" s="2">
+        <v>44194</v>
+      </c>
+      <c r="B731" s="3">
+        <v>710.64</v>
+      </c>
+    </row>
+    <row r="732" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A732" s="2">
+        <v>44195</v>
+      </c>
+      <c r="B732" s="3">
+        <v>711.24</v>
+      </c>
+    </row>
+    <row r="733" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A733" s="2">
+        <v>44196</v>
+      </c>
+      <c r="B733" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="734" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A734" s="2">
+        <v>44197</v>
+      </c>
+      <c r="B734" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="735" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A735" s="2">
+        <v>44198</v>
+      </c>
+      <c r="B735" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="736" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A736" s="2">
+        <v>44199</v>
+      </c>
+      <c r="B736" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="737" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A737" s="2">
+        <v>44200</v>
+      </c>
+      <c r="B737" s="3">
+        <v>710.95</v>
+      </c>
+    </row>
+    <row r="738" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A738" s="2">
+        <v>44201</v>
+      </c>
+      <c r="B738" s="3">
+        <v>702.93</v>
+      </c>
+    </row>
+    <row r="739" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A739" s="2">
+        <v>44202</v>
+      </c>
+      <c r="B739" s="3">
+        <v>702.29</v>
+      </c>
+    </row>
+    <row r="740" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A740" s="2">
+        <v>44203</v>
+      </c>
+      <c r="B740" s="3">
+        <v>696.18</v>
+      </c>
+    </row>
+    <row r="741" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A741" s="2">
+        <v>44204</v>
+      </c>
+      <c r="B741" s="3">
+        <v>709.99</v>
+      </c>
+    </row>
+    <row r="742" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A742" s="2">
+        <v>44205</v>
+      </c>
+      <c r="B742" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="743" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A743" s="2">
+        <v>44206</v>
+      </c>
+      <c r="B743" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="744" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A744" s="2">
+        <v>44207</v>
+      </c>
+      <c r="B744" s="3">
+        <v>713.28</v>
+      </c>
+    </row>
+    <row r="745" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A745" s="2">
+        <v>44208</v>
+      </c>
+      <c r="B745" s="3">
+        <v>718.89</v>
+      </c>
+    </row>
+    <row r="746" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A746" s="2">
+        <v>44209</v>
+      </c>
+      <c r="B746" s="3">
+        <v>725.24</v>
+      </c>
+    </row>
+    <row r="747" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A747" s="2">
+        <v>44210</v>
+      </c>
+      <c r="B747" s="3">
+        <v>739.72</v>
+      </c>
+    </row>
+    <row r="748" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A748" s="2">
+        <v>44211</v>
+      </c>
+      <c r="B748" s="3">
+        <v>735.35</v>
+      </c>
+    </row>
+    <row r="749" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A749" s="2">
+        <v>44212</v>
+      </c>
+      <c r="B749" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="750" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A750" s="2">
+        <v>44213</v>
+      </c>
+      <c r="B750" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="751" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A751" s="2">
+        <v>44214</v>
+      </c>
+      <c r="B751" s="3">
+        <v>735.06</v>
+      </c>
+    </row>
+    <row r="752" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A752" s="2">
+        <v>44215</v>
+      </c>
+      <c r="B752" s="3">
+        <v>736.11</v>
+      </c>
+    </row>
+    <row r="753" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A753" s="2">
+        <v>44216</v>
+      </c>
+      <c r="B753" s="3">
+        <v>733.73</v>
+      </c>
+    </row>
+    <row r="754" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A754" s="2">
+        <v>44217</v>
+      </c>
+      <c r="B754" s="3">
+        <v>730.38</v>
+      </c>
+    </row>
+    <row r="755" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A755" s="2">
+        <v>44218</v>
+      </c>
+      <c r="B755" s="3">
+        <v>715.56</v>
+      </c>
+    </row>
+    <row r="756" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A756" s="2">
+        <v>44219</v>
+      </c>
+      <c r="B756" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="757" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A757" s="2">
+        <v>44220</v>
+      </c>
+      <c r="B757" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="758" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A758" s="2">
+        <v>44221</v>
+      </c>
+      <c r="B758" s="3">
+        <v>724.26</v>
+      </c>
+    </row>
+    <row r="759" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A759" s="2">
+        <v>44222</v>
+      </c>
+      <c r="B759" s="3">
+        <v>731.92</v>
+      </c>
+    </row>
+    <row r="760" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A760" s="2">
+        <v>44223</v>
+      </c>
+      <c r="B760" s="3">
+        <v>731</v>
+      </c>
+    </row>
+    <row r="761" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A761" s="2">
+        <v>44224</v>
+      </c>
+      <c r="B761" s="3">
+        <v>736.88</v>
+      </c>
+    </row>
+    <row r="762" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A762" s="2">
+        <v>44225</v>
+      </c>
+      <c r="B762" s="3">
+        <v>741.4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update automatico via Actualizar 02-05-2021 17-12-47
</commit_message>
<xml_diff>
--- a/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
+++ b/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID CL/IndicadoresEconomicos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="125" documentId="13_ncr:1_{C8B25996-B8C9-45E8-BF5F-0058EDDB5306}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{B2D90656-DD48-4ECD-BB23-8C8D4EDECED3}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="14_{F2753A6D-642C-43B1-9D50-7716AF012233}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{EB69DD7D-6DC7-40C7-A6EB-3567AAC68B32}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,21 +16,9 @@
     <sheet name="DOLAR_OBS_ADO" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">DOLAR_OBS_ADO!$A$3:$B$762</definedName>
-    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$762</definedName>
+    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$683</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -47,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="5">
   <si>
     <t>Tipos de cambio (pesos por dólar)</t>
   </si>
@@ -68,7 +56,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="22" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -214,21 +202,6 @@
       <b/>
       <sz val="10"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri Light"/>
-      <family val="2"/>
-      <scheme val="major"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -531,7 +504,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="50">
+  <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -574,14 +547,6 @@
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -604,7 +569,7 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="50">
+  <cellStyles count="42">
     <cellStyle name="20% - Énfasis1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Énfasis2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Énfasis3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -618,17 +583,11 @@
     <cellStyle name="40% - Énfasis5" xfId="36" builtinId="47" customBuiltin="1"/>
     <cellStyle name="40% - Énfasis6" xfId="40" builtinId="51" customBuiltin="1"/>
     <cellStyle name="60% - Énfasis1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% - Énfasis1 2" xfId="42" xr:uid="{4385A8D2-651C-4773-80CB-11F47798F1CE}"/>
     <cellStyle name="60% - Énfasis2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% - Énfasis2 2" xfId="43" xr:uid="{054221C2-13B6-4754-B0B6-C32A4E8A95AD}"/>
     <cellStyle name="60% - Énfasis3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% - Énfasis3 2" xfId="44" xr:uid="{BB28A6FF-22BE-46E4-B116-00518D401B6E}"/>
     <cellStyle name="60% - Énfasis4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% - Énfasis4 2" xfId="45" xr:uid="{D1C02AD5-7A4A-4764-935B-FAB4D7D87EE9}"/>
     <cellStyle name="60% - Énfasis5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% - Énfasis5 2" xfId="46" xr:uid="{9F6E8D91-7C00-42FF-8A7D-91C893DA4AB8}"/>
     <cellStyle name="60% - Énfasis6" xfId="41" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="60% - Énfasis6 2" xfId="47" xr:uid="{1DF80BA0-24DE-4DA9-8EE2-A15003600F7C}"/>
     <cellStyle name="Bueno" xfId="6" builtinId="26" customBuiltin="1"/>
     <cellStyle name="Cálculo" xfId="11" builtinId="22" customBuiltin="1"/>
     <cellStyle name="Celda de comprobación" xfId="13" builtinId="23" customBuiltin="1"/>
@@ -644,7 +603,6 @@
     <cellStyle name="Entrada" xfId="9" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Incorrecto" xfId="7" builtinId="27" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
-    <cellStyle name="Neutral 2" xfId="48" xr:uid="{96B4E413-929F-4319-B3D6-5D1EF8AD0E76}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Notas" xfId="15" builtinId="10" customBuiltin="1"/>
     <cellStyle name="Salida" xfId="10" builtinId="21" customBuiltin="1"/>
@@ -653,7 +611,6 @@
     <cellStyle name="Título" xfId="1" builtinId="15" customBuiltin="1"/>
     <cellStyle name="Título 2" xfId="3" builtinId="17" customBuiltin="1"/>
     <cellStyle name="Título 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Título 4" xfId="49" xr:uid="{072D0298-5CC9-445D-BF36-9D06198D96B3}"/>
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -970,19 +927,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B762"/>
+  <dimension ref="A1:B683"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="4" topLeftCell="B761" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="4" topLeftCell="B671" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="B762" sqref="B762"/>
+      <selection pane="bottomRight" activeCell="B683" sqref="B683"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.7109375" customWidth="1"/>
-    <col min="2" max="2" width="14.42578125" customWidth="1"/>
+    <col min="1" max="1" width="11.5703125" customWidth="1"/>
+    <col min="2" max="2" width="15.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -6443,638 +6400,6 @@
       </c>
       <c r="B683" s="3">
         <v>760.9</v>
-      </c>
-    </row>
-    <row r="684" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A684" s="2">
-        <v>44147</v>
-      </c>
-      <c r="B684" s="3">
-        <v>757.42</v>
-      </c>
-    </row>
-    <row r="685" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A685" s="2">
-        <v>44148</v>
-      </c>
-      <c r="B685" s="3">
-        <v>757.43</v>
-      </c>
-    </row>
-    <row r="686" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A686" s="2">
-        <v>44149</v>
-      </c>
-      <c r="B686" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="687" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A687" s="2">
-        <v>44150</v>
-      </c>
-      <c r="B687" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="688" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A688" s="2">
-        <v>44151</v>
-      </c>
-      <c r="B688" s="3">
-        <v>766.7</v>
-      </c>
-    </row>
-    <row r="689" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A689" s="2">
-        <v>44152</v>
-      </c>
-      <c r="B689" s="3">
-        <v>767.86</v>
-      </c>
-    </row>
-    <row r="690" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A690" s="2">
-        <v>44153</v>
-      </c>
-      <c r="B690" s="3">
-        <v>767.05</v>
-      </c>
-    </row>
-    <row r="691" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A691" s="2">
-        <v>44154</v>
-      </c>
-      <c r="B691" s="3">
-        <v>758.1</v>
-      </c>
-    </row>
-    <row r="692" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A692" s="2">
-        <v>44155</v>
-      </c>
-      <c r="B692" s="3">
-        <v>758.62</v>
-      </c>
-    </row>
-    <row r="693" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A693" s="2">
-        <v>44156</v>
-      </c>
-      <c r="B693" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="694" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A694" s="2">
-        <v>44157</v>
-      </c>
-      <c r="B694" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="695" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A695" s="2">
-        <v>44158</v>
-      </c>
-      <c r="B695" s="3">
-        <v>761.55</v>
-      </c>
-    </row>
-    <row r="696" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A696" s="2">
-        <v>44159</v>
-      </c>
-      <c r="B696" s="3">
-        <v>765.96</v>
-      </c>
-    </row>
-    <row r="697" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A697" s="2">
-        <v>44160</v>
-      </c>
-      <c r="B697" s="3">
-        <v>772.83</v>
-      </c>
-    </row>
-    <row r="698" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A698" s="2">
-        <v>44161</v>
-      </c>
-      <c r="B698" s="3">
-        <v>771.68</v>
-      </c>
-    </row>
-    <row r="699" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A699" s="2">
-        <v>44162</v>
-      </c>
-      <c r="B699" s="3">
-        <v>766</v>
-      </c>
-    </row>
-    <row r="700" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A700" s="2">
-        <v>44163</v>
-      </c>
-      <c r="B700" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="701" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A701" s="2">
-        <v>44164</v>
-      </c>
-      <c r="B701" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="702" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A702" s="2">
-        <v>44165</v>
-      </c>
-      <c r="B702" s="3">
-        <v>766.69</v>
-      </c>
-    </row>
-    <row r="703" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A703" s="2">
-        <v>44166</v>
-      </c>
-      <c r="B703" s="3">
-        <v>767.29</v>
-      </c>
-    </row>
-    <row r="704" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A704" s="2">
-        <v>44167</v>
-      </c>
-      <c r="B704" s="3">
-        <v>760.16</v>
-      </c>
-    </row>
-    <row r="705" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A705" s="2">
-        <v>44168</v>
-      </c>
-      <c r="B705" s="3">
-        <v>755.34</v>
-      </c>
-    </row>
-    <row r="706" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A706" s="2">
-        <v>44169</v>
-      </c>
-      <c r="B706" s="3">
-        <v>752.03</v>
-      </c>
-    </row>
-    <row r="707" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A707" s="2">
-        <v>44170</v>
-      </c>
-      <c r="B707" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="708" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A708" s="2">
-        <v>44171</v>
-      </c>
-      <c r="B708" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="709" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A709" s="2">
-        <v>44172</v>
-      </c>
-      <c r="B709" s="3">
-        <v>747.61</v>
-      </c>
-    </row>
-    <row r="710" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A710" s="2">
-        <v>44173</v>
-      </c>
-      <c r="B710" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="711" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A711" s="2">
-        <v>44174</v>
-      </c>
-      <c r="B711" s="3">
-        <v>744.82</v>
-      </c>
-    </row>
-    <row r="712" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A712" s="2">
-        <v>44175</v>
-      </c>
-      <c r="B712" s="3">
-        <v>739.45</v>
-      </c>
-    </row>
-    <row r="713" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A713" s="2">
-        <v>44176</v>
-      </c>
-      <c r="B713" s="3">
-        <v>738.17</v>
-      </c>
-    </row>
-    <row r="714" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A714" s="2">
-        <v>44177</v>
-      </c>
-      <c r="B714" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="715" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A715" s="2">
-        <v>44178</v>
-      </c>
-      <c r="B715" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="716" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A716" s="2">
-        <v>44179</v>
-      </c>
-      <c r="B716" s="3">
-        <v>733.55</v>
-      </c>
-    </row>
-    <row r="717" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A717" s="2">
-        <v>44180</v>
-      </c>
-      <c r="B717" s="3">
-        <v>731.58</v>
-      </c>
-    </row>
-    <row r="718" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A718" s="2">
-        <v>44181</v>
-      </c>
-      <c r="B718" s="3">
-        <v>734.23</v>
-      </c>
-    </row>
-    <row r="719" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A719" s="2">
-        <v>44182</v>
-      </c>
-      <c r="B719" s="3">
-        <v>735.09</v>
-      </c>
-    </row>
-    <row r="720" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A720" s="2">
-        <v>44183</v>
-      </c>
-      <c r="B720" s="3">
-        <v>723.44</v>
-      </c>
-    </row>
-    <row r="721" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A721" s="2">
-        <v>44184</v>
-      </c>
-      <c r="B721" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="722" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A722" s="2">
-        <v>44185</v>
-      </c>
-      <c r="B722" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="723" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A723" s="2">
-        <v>44186</v>
-      </c>
-      <c r="B723" s="3">
-        <v>723.85</v>
-      </c>
-    </row>
-    <row r="724" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A724" s="2">
-        <v>44187</v>
-      </c>
-      <c r="B724" s="3">
-        <v>730.7</v>
-      </c>
-    </row>
-    <row r="725" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A725" s="2">
-        <v>44188</v>
-      </c>
-      <c r="B725" s="3">
-        <v>728.96</v>
-      </c>
-    </row>
-    <row r="726" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A726" s="2">
-        <v>44189</v>
-      </c>
-      <c r="B726" s="3">
-        <v>716.25</v>
-      </c>
-    </row>
-    <row r="727" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A727" s="2">
-        <v>44190</v>
-      </c>
-      <c r="B727" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="728" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A728" s="2">
-        <v>44191</v>
-      </c>
-      <c r="B728" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="729" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A729" s="2">
-        <v>44192</v>
-      </c>
-      <c r="B729" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="730" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A730" s="2">
-        <v>44193</v>
-      </c>
-      <c r="B730" s="3">
-        <v>710.26</v>
-      </c>
-    </row>
-    <row r="731" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A731" s="2">
-        <v>44194</v>
-      </c>
-      <c r="B731" s="3">
-        <v>710.64</v>
-      </c>
-    </row>
-    <row r="732" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A732" s="2">
-        <v>44195</v>
-      </c>
-      <c r="B732" s="3">
-        <v>711.24</v>
-      </c>
-    </row>
-    <row r="733" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A733" s="2">
-        <v>44196</v>
-      </c>
-      <c r="B733" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="734" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A734" s="2">
-        <v>44197</v>
-      </c>
-      <c r="B734" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="735" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A735" s="2">
-        <v>44198</v>
-      </c>
-      <c r="B735" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="736" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A736" s="2">
-        <v>44199</v>
-      </c>
-      <c r="B736" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="737" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A737" s="2">
-        <v>44200</v>
-      </c>
-      <c r="B737" s="3">
-        <v>710.95</v>
-      </c>
-    </row>
-    <row r="738" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A738" s="2">
-        <v>44201</v>
-      </c>
-      <c r="B738" s="3">
-        <v>702.93</v>
-      </c>
-    </row>
-    <row r="739" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A739" s="2">
-        <v>44202</v>
-      </c>
-      <c r="B739" s="3">
-        <v>702.29</v>
-      </c>
-    </row>
-    <row r="740" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A740" s="2">
-        <v>44203</v>
-      </c>
-      <c r="B740" s="3">
-        <v>696.18</v>
-      </c>
-    </row>
-    <row r="741" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A741" s="2">
-        <v>44204</v>
-      </c>
-      <c r="B741" s="3">
-        <v>709.99</v>
-      </c>
-    </row>
-    <row r="742" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A742" s="2">
-        <v>44205</v>
-      </c>
-      <c r="B742" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="743" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A743" s="2">
-        <v>44206</v>
-      </c>
-      <c r="B743" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="744" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A744" s="2">
-        <v>44207</v>
-      </c>
-      <c r="B744" s="3">
-        <v>713.28</v>
-      </c>
-    </row>
-    <row r="745" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A745" s="2">
-        <v>44208</v>
-      </c>
-      <c r="B745" s="3">
-        <v>718.89</v>
-      </c>
-    </row>
-    <row r="746" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A746" s="2">
-        <v>44209</v>
-      </c>
-      <c r="B746" s="3">
-        <v>725.24</v>
-      </c>
-    </row>
-    <row r="747" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A747" s="2">
-        <v>44210</v>
-      </c>
-      <c r="B747" s="3">
-        <v>739.72</v>
-      </c>
-    </row>
-    <row r="748" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A748" s="2">
-        <v>44211</v>
-      </c>
-      <c r="B748" s="3">
-        <v>735.35</v>
-      </c>
-    </row>
-    <row r="749" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A749" s="2">
-        <v>44212</v>
-      </c>
-      <c r="B749" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="750" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A750" s="2">
-        <v>44213</v>
-      </c>
-      <c r="B750" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="751" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A751" s="2">
-        <v>44214</v>
-      </c>
-      <c r="B751" s="3">
-        <v>735.06</v>
-      </c>
-    </row>
-    <row r="752" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A752" s="2">
-        <v>44215</v>
-      </c>
-      <c r="B752" s="3">
-        <v>736.11</v>
-      </c>
-    </row>
-    <row r="753" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A753" s="2">
-        <v>44216</v>
-      </c>
-      <c r="B753" s="3">
-        <v>733.73</v>
-      </c>
-    </row>
-    <row r="754" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A754" s="2">
-        <v>44217</v>
-      </c>
-      <c r="B754" s="3">
-        <v>730.38</v>
-      </c>
-    </row>
-    <row r="755" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A755" s="2">
-        <v>44218</v>
-      </c>
-      <c r="B755" s="3">
-        <v>715.56</v>
-      </c>
-    </row>
-    <row r="756" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A756" s="2">
-        <v>44219</v>
-      </c>
-      <c r="B756" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="757" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A757" s="2">
-        <v>44220</v>
-      </c>
-      <c r="B757" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="758" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A758" s="2">
-        <v>44221</v>
-      </c>
-      <c r="B758" s="3">
-        <v>724.26</v>
-      </c>
-    </row>
-    <row r="759" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A759" s="2">
-        <v>44222</v>
-      </c>
-      <c r="B759" s="3">
-        <v>731.92</v>
-      </c>
-    </row>
-    <row r="760" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A760" s="2">
-        <v>44223</v>
-      </c>
-      <c r="B760" s="3">
-        <v>731</v>
-      </c>
-    </row>
-    <row r="761" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A761" s="2">
-        <v>44224</v>
-      </c>
-      <c r="B761" s="3">
-        <v>736.88</v>
-      </c>
-    </row>
-    <row r="762" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A762" s="2">
-        <v>44225</v>
-      </c>
-      <c r="B762" s="3">
-        <v>741.4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update automatico via Actualizar 02-05-2021 19-08-46
</commit_message>
<xml_diff>
--- a/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
+++ b/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID CL/IndicadoresEconomicos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="14_{F2753A6D-642C-43B1-9D50-7716AF012233}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{EB69DD7D-6DC7-40C7-A6EB-3567AAC68B32}"/>
+  <xr:revisionPtr revIDLastSave="125" documentId="13_ncr:1_{C8B25996-B8C9-45E8-BF5F-0058EDDB5306}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{B2D90656-DD48-4ECD-BB23-8C8D4EDECED3}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,9 +16,21 @@
     <sheet name="DOLAR_OBS_ADO" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$683</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">DOLAR_OBS_ADO!$A$3:$B$762</definedName>
+    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$762</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -35,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="5">
   <si>
     <t>Tipos de cambio (pesos por dólar)</t>
   </si>
@@ -56,7 +68,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -202,6 +214,21 @@
       <b/>
       <sz val="10"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -504,7 +531,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="42">
+  <cellStyleXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -547,6 +574,14 @@
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -569,7 +604,7 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="42">
+  <cellStyles count="50">
     <cellStyle name="20% - Énfasis1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Énfasis2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Énfasis3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -583,11 +618,17 @@
     <cellStyle name="40% - Énfasis5" xfId="36" builtinId="47" customBuiltin="1"/>
     <cellStyle name="40% - Énfasis6" xfId="40" builtinId="51" customBuiltin="1"/>
     <cellStyle name="60% - Énfasis1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Énfasis1 2" xfId="42" xr:uid="{4385A8D2-651C-4773-80CB-11F47798F1CE}"/>
     <cellStyle name="60% - Énfasis2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Énfasis2 2" xfId="43" xr:uid="{054221C2-13B6-4754-B0B6-C32A4E8A95AD}"/>
     <cellStyle name="60% - Énfasis3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Énfasis3 2" xfId="44" xr:uid="{BB28A6FF-22BE-46E4-B116-00518D401B6E}"/>
     <cellStyle name="60% - Énfasis4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Énfasis4 2" xfId="45" xr:uid="{D1C02AD5-7A4A-4764-935B-FAB4D7D87EE9}"/>
     <cellStyle name="60% - Énfasis5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Énfasis5 2" xfId="46" xr:uid="{9F6E8D91-7C00-42FF-8A7D-91C893DA4AB8}"/>
     <cellStyle name="60% - Énfasis6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="60% - Énfasis6 2" xfId="47" xr:uid="{1DF80BA0-24DE-4DA9-8EE2-A15003600F7C}"/>
     <cellStyle name="Bueno" xfId="6" builtinId="26" customBuiltin="1"/>
     <cellStyle name="Cálculo" xfId="11" builtinId="22" customBuiltin="1"/>
     <cellStyle name="Celda de comprobación" xfId="13" builtinId="23" customBuiltin="1"/>
@@ -603,6 +644,7 @@
     <cellStyle name="Entrada" xfId="9" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Incorrecto" xfId="7" builtinId="27" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
+    <cellStyle name="Neutral 2" xfId="48" xr:uid="{96B4E413-929F-4319-B3D6-5D1EF8AD0E76}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Notas" xfId="15" builtinId="10" customBuiltin="1"/>
     <cellStyle name="Salida" xfId="10" builtinId="21" customBuiltin="1"/>
@@ -611,6 +653,7 @@
     <cellStyle name="Título" xfId="1" builtinId="15" customBuiltin="1"/>
     <cellStyle name="Título 2" xfId="3" builtinId="17" customBuiltin="1"/>
     <cellStyle name="Título 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Título 4" xfId="49" xr:uid="{072D0298-5CC9-445D-BF36-9D06198D96B3}"/>
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -927,19 +970,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B683"/>
+  <dimension ref="A1:B762"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="4" topLeftCell="B671" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="4" topLeftCell="B761" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="B683" sqref="B683"/>
+      <selection pane="bottomRight" activeCell="B762" sqref="B762"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.5703125" customWidth="1"/>
-    <col min="2" max="2" width="15.5703125" customWidth="1"/>
+    <col min="1" max="1" width="12.7109375" customWidth="1"/>
+    <col min="2" max="2" width="14.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -6400,6 +6443,638 @@
       </c>
       <c r="B683" s="3">
         <v>760.9</v>
+      </c>
+    </row>
+    <row r="684" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A684" s="2">
+        <v>44147</v>
+      </c>
+      <c r="B684" s="3">
+        <v>757.42</v>
+      </c>
+    </row>
+    <row r="685" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A685" s="2">
+        <v>44148</v>
+      </c>
+      <c r="B685" s="3">
+        <v>757.43</v>
+      </c>
+    </row>
+    <row r="686" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A686" s="2">
+        <v>44149</v>
+      </c>
+      <c r="B686" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="687" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A687" s="2">
+        <v>44150</v>
+      </c>
+      <c r="B687" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="688" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A688" s="2">
+        <v>44151</v>
+      </c>
+      <c r="B688" s="3">
+        <v>766.7</v>
+      </c>
+    </row>
+    <row r="689" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A689" s="2">
+        <v>44152</v>
+      </c>
+      <c r="B689" s="3">
+        <v>767.86</v>
+      </c>
+    </row>
+    <row r="690" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A690" s="2">
+        <v>44153</v>
+      </c>
+      <c r="B690" s="3">
+        <v>767.05</v>
+      </c>
+    </row>
+    <row r="691" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A691" s="2">
+        <v>44154</v>
+      </c>
+      <c r="B691" s="3">
+        <v>758.1</v>
+      </c>
+    </row>
+    <row r="692" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A692" s="2">
+        <v>44155</v>
+      </c>
+      <c r="B692" s="3">
+        <v>758.62</v>
+      </c>
+    </row>
+    <row r="693" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A693" s="2">
+        <v>44156</v>
+      </c>
+      <c r="B693" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="694" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A694" s="2">
+        <v>44157</v>
+      </c>
+      <c r="B694" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="695" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A695" s="2">
+        <v>44158</v>
+      </c>
+      <c r="B695" s="3">
+        <v>761.55</v>
+      </c>
+    </row>
+    <row r="696" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A696" s="2">
+        <v>44159</v>
+      </c>
+      <c r="B696" s="3">
+        <v>765.96</v>
+      </c>
+    </row>
+    <row r="697" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A697" s="2">
+        <v>44160</v>
+      </c>
+      <c r="B697" s="3">
+        <v>772.83</v>
+      </c>
+    </row>
+    <row r="698" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A698" s="2">
+        <v>44161</v>
+      </c>
+      <c r="B698" s="3">
+        <v>771.68</v>
+      </c>
+    </row>
+    <row r="699" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A699" s="2">
+        <v>44162</v>
+      </c>
+      <c r="B699" s="3">
+        <v>766</v>
+      </c>
+    </row>
+    <row r="700" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A700" s="2">
+        <v>44163</v>
+      </c>
+      <c r="B700" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="701" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A701" s="2">
+        <v>44164</v>
+      </c>
+      <c r="B701" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="702" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A702" s="2">
+        <v>44165</v>
+      </c>
+      <c r="B702" s="3">
+        <v>766.69</v>
+      </c>
+    </row>
+    <row r="703" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A703" s="2">
+        <v>44166</v>
+      </c>
+      <c r="B703" s="3">
+        <v>767.29</v>
+      </c>
+    </row>
+    <row r="704" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A704" s="2">
+        <v>44167</v>
+      </c>
+      <c r="B704" s="3">
+        <v>760.16</v>
+      </c>
+    </row>
+    <row r="705" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A705" s="2">
+        <v>44168</v>
+      </c>
+      <c r="B705" s="3">
+        <v>755.34</v>
+      </c>
+    </row>
+    <row r="706" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A706" s="2">
+        <v>44169</v>
+      </c>
+      <c r="B706" s="3">
+        <v>752.03</v>
+      </c>
+    </row>
+    <row r="707" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A707" s="2">
+        <v>44170</v>
+      </c>
+      <c r="B707" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="708" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A708" s="2">
+        <v>44171</v>
+      </c>
+      <c r="B708" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="709" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A709" s="2">
+        <v>44172</v>
+      </c>
+      <c r="B709" s="3">
+        <v>747.61</v>
+      </c>
+    </row>
+    <row r="710" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A710" s="2">
+        <v>44173</v>
+      </c>
+      <c r="B710" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="711" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A711" s="2">
+        <v>44174</v>
+      </c>
+      <c r="B711" s="3">
+        <v>744.82</v>
+      </c>
+    </row>
+    <row r="712" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A712" s="2">
+        <v>44175</v>
+      </c>
+      <c r="B712" s="3">
+        <v>739.45</v>
+      </c>
+    </row>
+    <row r="713" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A713" s="2">
+        <v>44176</v>
+      </c>
+      <c r="B713" s="3">
+        <v>738.17</v>
+      </c>
+    </row>
+    <row r="714" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A714" s="2">
+        <v>44177</v>
+      </c>
+      <c r="B714" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="715" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A715" s="2">
+        <v>44178</v>
+      </c>
+      <c r="B715" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="716" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A716" s="2">
+        <v>44179</v>
+      </c>
+      <c r="B716" s="3">
+        <v>733.55</v>
+      </c>
+    </row>
+    <row r="717" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A717" s="2">
+        <v>44180</v>
+      </c>
+      <c r="B717" s="3">
+        <v>731.58</v>
+      </c>
+    </row>
+    <row r="718" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A718" s="2">
+        <v>44181</v>
+      </c>
+      <c r="B718" s="3">
+        <v>734.23</v>
+      </c>
+    </row>
+    <row r="719" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A719" s="2">
+        <v>44182</v>
+      </c>
+      <c r="B719" s="3">
+        <v>735.09</v>
+      </c>
+    </row>
+    <row r="720" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A720" s="2">
+        <v>44183</v>
+      </c>
+      <c r="B720" s="3">
+        <v>723.44</v>
+      </c>
+    </row>
+    <row r="721" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A721" s="2">
+        <v>44184</v>
+      </c>
+      <c r="B721" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="722" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A722" s="2">
+        <v>44185</v>
+      </c>
+      <c r="B722" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="723" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A723" s="2">
+        <v>44186</v>
+      </c>
+      <c r="B723" s="3">
+        <v>723.85</v>
+      </c>
+    </row>
+    <row r="724" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A724" s="2">
+        <v>44187</v>
+      </c>
+      <c r="B724" s="3">
+        <v>730.7</v>
+      </c>
+    </row>
+    <row r="725" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A725" s="2">
+        <v>44188</v>
+      </c>
+      <c r="B725" s="3">
+        <v>728.96</v>
+      </c>
+    </row>
+    <row r="726" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A726" s="2">
+        <v>44189</v>
+      </c>
+      <c r="B726" s="3">
+        <v>716.25</v>
+      </c>
+    </row>
+    <row r="727" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A727" s="2">
+        <v>44190</v>
+      </c>
+      <c r="B727" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="728" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A728" s="2">
+        <v>44191</v>
+      </c>
+      <c r="B728" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="729" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A729" s="2">
+        <v>44192</v>
+      </c>
+      <c r="B729" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="730" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A730" s="2">
+        <v>44193</v>
+      </c>
+      <c r="B730" s="3">
+        <v>710.26</v>
+      </c>
+    </row>
+    <row r="731" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A731" s="2">
+        <v>44194</v>
+      </c>
+      <c r="B731" s="3">
+        <v>710.64</v>
+      </c>
+    </row>
+    <row r="732" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A732" s="2">
+        <v>44195</v>
+      </c>
+      <c r="B732" s="3">
+        <v>711.24</v>
+      </c>
+    </row>
+    <row r="733" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A733" s="2">
+        <v>44196</v>
+      </c>
+      <c r="B733" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="734" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A734" s="2">
+        <v>44197</v>
+      </c>
+      <c r="B734" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="735" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A735" s="2">
+        <v>44198</v>
+      </c>
+      <c r="B735" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="736" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A736" s="2">
+        <v>44199</v>
+      </c>
+      <c r="B736" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="737" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A737" s="2">
+        <v>44200</v>
+      </c>
+      <c r="B737" s="3">
+        <v>710.95</v>
+      </c>
+    </row>
+    <row r="738" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A738" s="2">
+        <v>44201</v>
+      </c>
+      <c r="B738" s="3">
+        <v>702.93</v>
+      </c>
+    </row>
+    <row r="739" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A739" s="2">
+        <v>44202</v>
+      </c>
+      <c r="B739" s="3">
+        <v>702.29</v>
+      </c>
+    </row>
+    <row r="740" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A740" s="2">
+        <v>44203</v>
+      </c>
+      <c r="B740" s="3">
+        <v>696.18</v>
+      </c>
+    </row>
+    <row r="741" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A741" s="2">
+        <v>44204</v>
+      </c>
+      <c r="B741" s="3">
+        <v>709.99</v>
+      </c>
+    </row>
+    <row r="742" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A742" s="2">
+        <v>44205</v>
+      </c>
+      <c r="B742" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="743" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A743" s="2">
+        <v>44206</v>
+      </c>
+      <c r="B743" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="744" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A744" s="2">
+        <v>44207</v>
+      </c>
+      <c r="B744" s="3">
+        <v>713.28</v>
+      </c>
+    </row>
+    <row r="745" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A745" s="2">
+        <v>44208</v>
+      </c>
+      <c r="B745" s="3">
+        <v>718.89</v>
+      </c>
+    </row>
+    <row r="746" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A746" s="2">
+        <v>44209</v>
+      </c>
+      <c r="B746" s="3">
+        <v>725.24</v>
+      </c>
+    </row>
+    <row r="747" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A747" s="2">
+        <v>44210</v>
+      </c>
+      <c r="B747" s="3">
+        <v>739.72</v>
+      </c>
+    </row>
+    <row r="748" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A748" s="2">
+        <v>44211</v>
+      </c>
+      <c r="B748" s="3">
+        <v>735.35</v>
+      </c>
+    </row>
+    <row r="749" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A749" s="2">
+        <v>44212</v>
+      </c>
+      <c r="B749" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="750" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A750" s="2">
+        <v>44213</v>
+      </c>
+      <c r="B750" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="751" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A751" s="2">
+        <v>44214</v>
+      </c>
+      <c r="B751" s="3">
+        <v>735.06</v>
+      </c>
+    </row>
+    <row r="752" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A752" s="2">
+        <v>44215</v>
+      </c>
+      <c r="B752" s="3">
+        <v>736.11</v>
+      </c>
+    </row>
+    <row r="753" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A753" s="2">
+        <v>44216</v>
+      </c>
+      <c r="B753" s="3">
+        <v>733.73</v>
+      </c>
+    </row>
+    <row r="754" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A754" s="2">
+        <v>44217</v>
+      </c>
+      <c r="B754" s="3">
+        <v>730.38</v>
+      </c>
+    </row>
+    <row r="755" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A755" s="2">
+        <v>44218</v>
+      </c>
+      <c r="B755" s="3">
+        <v>715.56</v>
+      </c>
+    </row>
+    <row r="756" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A756" s="2">
+        <v>44219</v>
+      </c>
+      <c r="B756" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="757" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A757" s="2">
+        <v>44220</v>
+      </c>
+      <c r="B757" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="758" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A758" s="2">
+        <v>44221</v>
+      </c>
+      <c r="B758" s="3">
+        <v>724.26</v>
+      </c>
+    </row>
+    <row r="759" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A759" s="2">
+        <v>44222</v>
+      </c>
+      <c r="B759" s="3">
+        <v>731.92</v>
+      </c>
+    </row>
+    <row r="760" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A760" s="2">
+        <v>44223</v>
+      </c>
+      <c r="B760" s="3">
+        <v>731</v>
+      </c>
+    </row>
+    <row r="761" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A761" s="2">
+        <v>44224</v>
+      </c>
+      <c r="B761" s="3">
+        <v>736.88</v>
+      </c>
+    </row>
+    <row r="762" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A762" s="2">
+        <v>44225</v>
+      </c>
+      <c r="B762" s="3">
+        <v>741.4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update automatico via Actualizar 02-05-2021 19-12-40
</commit_message>
<xml_diff>
--- a/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
+++ b/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID CL/IndicadoresEconomicos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="125" documentId="13_ncr:1_{C8B25996-B8C9-45E8-BF5F-0058EDDB5306}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{B2D90656-DD48-4ECD-BB23-8C8D4EDECED3}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="14_{F2753A6D-642C-43B1-9D50-7716AF012233}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{EB69DD7D-6DC7-40C7-A6EB-3567AAC68B32}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,21 +16,9 @@
     <sheet name="DOLAR_OBS_ADO" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">DOLAR_OBS_ADO!$A$3:$B$762</definedName>
-    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$762</definedName>
+    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$683</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -47,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="5">
   <si>
     <t>Tipos de cambio (pesos por dólar)</t>
   </si>
@@ -68,7 +56,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="22" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -214,21 +202,6 @@
       <b/>
       <sz val="10"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri Light"/>
-      <family val="2"/>
-      <scheme val="major"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -531,7 +504,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="50">
+  <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -574,14 +547,6 @@
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -604,7 +569,7 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="50">
+  <cellStyles count="42">
     <cellStyle name="20% - Énfasis1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Énfasis2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Énfasis3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -618,17 +583,11 @@
     <cellStyle name="40% - Énfasis5" xfId="36" builtinId="47" customBuiltin="1"/>
     <cellStyle name="40% - Énfasis6" xfId="40" builtinId="51" customBuiltin="1"/>
     <cellStyle name="60% - Énfasis1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% - Énfasis1 2" xfId="42" xr:uid="{4385A8D2-651C-4773-80CB-11F47798F1CE}"/>
     <cellStyle name="60% - Énfasis2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% - Énfasis2 2" xfId="43" xr:uid="{054221C2-13B6-4754-B0B6-C32A4E8A95AD}"/>
     <cellStyle name="60% - Énfasis3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% - Énfasis3 2" xfId="44" xr:uid="{BB28A6FF-22BE-46E4-B116-00518D401B6E}"/>
     <cellStyle name="60% - Énfasis4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% - Énfasis4 2" xfId="45" xr:uid="{D1C02AD5-7A4A-4764-935B-FAB4D7D87EE9}"/>
     <cellStyle name="60% - Énfasis5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% - Énfasis5 2" xfId="46" xr:uid="{9F6E8D91-7C00-42FF-8A7D-91C893DA4AB8}"/>
     <cellStyle name="60% - Énfasis6" xfId="41" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="60% - Énfasis6 2" xfId="47" xr:uid="{1DF80BA0-24DE-4DA9-8EE2-A15003600F7C}"/>
     <cellStyle name="Bueno" xfId="6" builtinId="26" customBuiltin="1"/>
     <cellStyle name="Cálculo" xfId="11" builtinId="22" customBuiltin="1"/>
     <cellStyle name="Celda de comprobación" xfId="13" builtinId="23" customBuiltin="1"/>
@@ -644,7 +603,6 @@
     <cellStyle name="Entrada" xfId="9" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Incorrecto" xfId="7" builtinId="27" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
-    <cellStyle name="Neutral 2" xfId="48" xr:uid="{96B4E413-929F-4319-B3D6-5D1EF8AD0E76}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Notas" xfId="15" builtinId="10" customBuiltin="1"/>
     <cellStyle name="Salida" xfId="10" builtinId="21" customBuiltin="1"/>
@@ -653,7 +611,6 @@
     <cellStyle name="Título" xfId="1" builtinId="15" customBuiltin="1"/>
     <cellStyle name="Título 2" xfId="3" builtinId="17" customBuiltin="1"/>
     <cellStyle name="Título 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Título 4" xfId="49" xr:uid="{072D0298-5CC9-445D-BF36-9D06198D96B3}"/>
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -970,19 +927,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B762"/>
+  <dimension ref="A1:B683"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="4" topLeftCell="B761" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="4" topLeftCell="B671" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="B762" sqref="B762"/>
+      <selection pane="bottomRight" activeCell="B683" sqref="B683"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.7109375" customWidth="1"/>
-    <col min="2" max="2" width="14.42578125" customWidth="1"/>
+    <col min="1" max="1" width="11.5703125" customWidth="1"/>
+    <col min="2" max="2" width="15.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -6443,638 +6400,6 @@
       </c>
       <c r="B683" s="3">
         <v>760.9</v>
-      </c>
-    </row>
-    <row r="684" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A684" s="2">
-        <v>44147</v>
-      </c>
-      <c r="B684" s="3">
-        <v>757.42</v>
-      </c>
-    </row>
-    <row r="685" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A685" s="2">
-        <v>44148</v>
-      </c>
-      <c r="B685" s="3">
-        <v>757.43</v>
-      </c>
-    </row>
-    <row r="686" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A686" s="2">
-        <v>44149</v>
-      </c>
-      <c r="B686" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="687" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A687" s="2">
-        <v>44150</v>
-      </c>
-      <c r="B687" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="688" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A688" s="2">
-        <v>44151</v>
-      </c>
-      <c r="B688" s="3">
-        <v>766.7</v>
-      </c>
-    </row>
-    <row r="689" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A689" s="2">
-        <v>44152</v>
-      </c>
-      <c r="B689" s="3">
-        <v>767.86</v>
-      </c>
-    </row>
-    <row r="690" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A690" s="2">
-        <v>44153</v>
-      </c>
-      <c r="B690" s="3">
-        <v>767.05</v>
-      </c>
-    </row>
-    <row r="691" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A691" s="2">
-        <v>44154</v>
-      </c>
-      <c r="B691" s="3">
-        <v>758.1</v>
-      </c>
-    </row>
-    <row r="692" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A692" s="2">
-        <v>44155</v>
-      </c>
-      <c r="B692" s="3">
-        <v>758.62</v>
-      </c>
-    </row>
-    <row r="693" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A693" s="2">
-        <v>44156</v>
-      </c>
-      <c r="B693" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="694" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A694" s="2">
-        <v>44157</v>
-      </c>
-      <c r="B694" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="695" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A695" s="2">
-        <v>44158</v>
-      </c>
-      <c r="B695" s="3">
-        <v>761.55</v>
-      </c>
-    </row>
-    <row r="696" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A696" s="2">
-        <v>44159</v>
-      </c>
-      <c r="B696" s="3">
-        <v>765.96</v>
-      </c>
-    </row>
-    <row r="697" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A697" s="2">
-        <v>44160</v>
-      </c>
-      <c r="B697" s="3">
-        <v>772.83</v>
-      </c>
-    </row>
-    <row r="698" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A698" s="2">
-        <v>44161</v>
-      </c>
-      <c r="B698" s="3">
-        <v>771.68</v>
-      </c>
-    </row>
-    <row r="699" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A699" s="2">
-        <v>44162</v>
-      </c>
-      <c r="B699" s="3">
-        <v>766</v>
-      </c>
-    </row>
-    <row r="700" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A700" s="2">
-        <v>44163</v>
-      </c>
-      <c r="B700" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="701" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A701" s="2">
-        <v>44164</v>
-      </c>
-      <c r="B701" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="702" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A702" s="2">
-        <v>44165</v>
-      </c>
-      <c r="B702" s="3">
-        <v>766.69</v>
-      </c>
-    </row>
-    <row r="703" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A703" s="2">
-        <v>44166</v>
-      </c>
-      <c r="B703" s="3">
-        <v>767.29</v>
-      </c>
-    </row>
-    <row r="704" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A704" s="2">
-        <v>44167</v>
-      </c>
-      <c r="B704" s="3">
-        <v>760.16</v>
-      </c>
-    </row>
-    <row r="705" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A705" s="2">
-        <v>44168</v>
-      </c>
-      <c r="B705" s="3">
-        <v>755.34</v>
-      </c>
-    </row>
-    <row r="706" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A706" s="2">
-        <v>44169</v>
-      </c>
-      <c r="B706" s="3">
-        <v>752.03</v>
-      </c>
-    </row>
-    <row r="707" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A707" s="2">
-        <v>44170</v>
-      </c>
-      <c r="B707" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="708" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A708" s="2">
-        <v>44171</v>
-      </c>
-      <c r="B708" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="709" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A709" s="2">
-        <v>44172</v>
-      </c>
-      <c r="B709" s="3">
-        <v>747.61</v>
-      </c>
-    </row>
-    <row r="710" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A710" s="2">
-        <v>44173</v>
-      </c>
-      <c r="B710" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="711" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A711" s="2">
-        <v>44174</v>
-      </c>
-      <c r="B711" s="3">
-        <v>744.82</v>
-      </c>
-    </row>
-    <row r="712" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A712" s="2">
-        <v>44175</v>
-      </c>
-      <c r="B712" s="3">
-        <v>739.45</v>
-      </c>
-    </row>
-    <row r="713" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A713" s="2">
-        <v>44176</v>
-      </c>
-      <c r="B713" s="3">
-        <v>738.17</v>
-      </c>
-    </row>
-    <row r="714" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A714" s="2">
-        <v>44177</v>
-      </c>
-      <c r="B714" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="715" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A715" s="2">
-        <v>44178</v>
-      </c>
-      <c r="B715" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="716" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A716" s="2">
-        <v>44179</v>
-      </c>
-      <c r="B716" s="3">
-        <v>733.55</v>
-      </c>
-    </row>
-    <row r="717" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A717" s="2">
-        <v>44180</v>
-      </c>
-      <c r="B717" s="3">
-        <v>731.58</v>
-      </c>
-    </row>
-    <row r="718" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A718" s="2">
-        <v>44181</v>
-      </c>
-      <c r="B718" s="3">
-        <v>734.23</v>
-      </c>
-    </row>
-    <row r="719" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A719" s="2">
-        <v>44182</v>
-      </c>
-      <c r="B719" s="3">
-        <v>735.09</v>
-      </c>
-    </row>
-    <row r="720" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A720" s="2">
-        <v>44183</v>
-      </c>
-      <c r="B720" s="3">
-        <v>723.44</v>
-      </c>
-    </row>
-    <row r="721" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A721" s="2">
-        <v>44184</v>
-      </c>
-      <c r="B721" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="722" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A722" s="2">
-        <v>44185</v>
-      </c>
-      <c r="B722" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="723" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A723" s="2">
-        <v>44186</v>
-      </c>
-      <c r="B723" s="3">
-        <v>723.85</v>
-      </c>
-    </row>
-    <row r="724" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A724" s="2">
-        <v>44187</v>
-      </c>
-      <c r="B724" s="3">
-        <v>730.7</v>
-      </c>
-    </row>
-    <row r="725" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A725" s="2">
-        <v>44188</v>
-      </c>
-      <c r="B725" s="3">
-        <v>728.96</v>
-      </c>
-    </row>
-    <row r="726" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A726" s="2">
-        <v>44189</v>
-      </c>
-      <c r="B726" s="3">
-        <v>716.25</v>
-      </c>
-    </row>
-    <row r="727" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A727" s="2">
-        <v>44190</v>
-      </c>
-      <c r="B727" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="728" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A728" s="2">
-        <v>44191</v>
-      </c>
-      <c r="B728" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="729" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A729" s="2">
-        <v>44192</v>
-      </c>
-      <c r="B729" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="730" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A730" s="2">
-        <v>44193</v>
-      </c>
-      <c r="B730" s="3">
-        <v>710.26</v>
-      </c>
-    </row>
-    <row r="731" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A731" s="2">
-        <v>44194</v>
-      </c>
-      <c r="B731" s="3">
-        <v>710.64</v>
-      </c>
-    </row>
-    <row r="732" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A732" s="2">
-        <v>44195</v>
-      </c>
-      <c r="B732" s="3">
-        <v>711.24</v>
-      </c>
-    </row>
-    <row r="733" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A733" s="2">
-        <v>44196</v>
-      </c>
-      <c r="B733" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="734" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A734" s="2">
-        <v>44197</v>
-      </c>
-      <c r="B734" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="735" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A735" s="2">
-        <v>44198</v>
-      </c>
-      <c r="B735" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="736" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A736" s="2">
-        <v>44199</v>
-      </c>
-      <c r="B736" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="737" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A737" s="2">
-        <v>44200</v>
-      </c>
-      <c r="B737" s="3">
-        <v>710.95</v>
-      </c>
-    </row>
-    <row r="738" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A738" s="2">
-        <v>44201</v>
-      </c>
-      <c r="B738" s="3">
-        <v>702.93</v>
-      </c>
-    </row>
-    <row r="739" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A739" s="2">
-        <v>44202</v>
-      </c>
-      <c r="B739" s="3">
-        <v>702.29</v>
-      </c>
-    </row>
-    <row r="740" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A740" s="2">
-        <v>44203</v>
-      </c>
-      <c r="B740" s="3">
-        <v>696.18</v>
-      </c>
-    </row>
-    <row r="741" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A741" s="2">
-        <v>44204</v>
-      </c>
-      <c r="B741" s="3">
-        <v>709.99</v>
-      </c>
-    </row>
-    <row r="742" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A742" s="2">
-        <v>44205</v>
-      </c>
-      <c r="B742" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="743" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A743" s="2">
-        <v>44206</v>
-      </c>
-      <c r="B743" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="744" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A744" s="2">
-        <v>44207</v>
-      </c>
-      <c r="B744" s="3">
-        <v>713.28</v>
-      </c>
-    </row>
-    <row r="745" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A745" s="2">
-        <v>44208</v>
-      </c>
-      <c r="B745" s="3">
-        <v>718.89</v>
-      </c>
-    </row>
-    <row r="746" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A746" s="2">
-        <v>44209</v>
-      </c>
-      <c r="B746" s="3">
-        <v>725.24</v>
-      </c>
-    </row>
-    <row r="747" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A747" s="2">
-        <v>44210</v>
-      </c>
-      <c r="B747" s="3">
-        <v>739.72</v>
-      </c>
-    </row>
-    <row r="748" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A748" s="2">
-        <v>44211</v>
-      </c>
-      <c r="B748" s="3">
-        <v>735.35</v>
-      </c>
-    </row>
-    <row r="749" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A749" s="2">
-        <v>44212</v>
-      </c>
-      <c r="B749" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="750" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A750" s="2">
-        <v>44213</v>
-      </c>
-      <c r="B750" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="751" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A751" s="2">
-        <v>44214</v>
-      </c>
-      <c r="B751" s="3">
-        <v>735.06</v>
-      </c>
-    </row>
-    <row r="752" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A752" s="2">
-        <v>44215</v>
-      </c>
-      <c r="B752" s="3">
-        <v>736.11</v>
-      </c>
-    </row>
-    <row r="753" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A753" s="2">
-        <v>44216</v>
-      </c>
-      <c r="B753" s="3">
-        <v>733.73</v>
-      </c>
-    </row>
-    <row r="754" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A754" s="2">
-        <v>44217</v>
-      </c>
-      <c r="B754" s="3">
-        <v>730.38</v>
-      </c>
-    </row>
-    <row r="755" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A755" s="2">
-        <v>44218</v>
-      </c>
-      <c r="B755" s="3">
-        <v>715.56</v>
-      </c>
-    </row>
-    <row r="756" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A756" s="2">
-        <v>44219</v>
-      </c>
-      <c r="B756" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="757" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A757" s="2">
-        <v>44220</v>
-      </c>
-      <c r="B757" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="758" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A758" s="2">
-        <v>44221</v>
-      </c>
-      <c r="B758" s="3">
-        <v>724.26</v>
-      </c>
-    </row>
-    <row r="759" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A759" s="2">
-        <v>44222</v>
-      </c>
-      <c r="B759" s="3">
-        <v>731.92</v>
-      </c>
-    </row>
-    <row r="760" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A760" s="2">
-        <v>44223</v>
-      </c>
-      <c r="B760" s="3">
-        <v>731</v>
-      </c>
-    </row>
-    <row r="761" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A761" s="2">
-        <v>44224</v>
-      </c>
-      <c r="B761" s="3">
-        <v>736.88</v>
-      </c>
-    </row>
-    <row r="762" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A762" s="2">
-        <v>44225</v>
-      </c>
-      <c r="B762" s="3">
-        <v>741.4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update automatico via Actualizar 02-06-2021 17-05-31
</commit_message>
<xml_diff>
--- a/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
+++ b/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID CL/IndicadoresEconomicos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="14_{F2753A6D-642C-43B1-9D50-7716AF012233}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{EB69DD7D-6DC7-40C7-A6EB-3567AAC68B32}"/>
+  <xr:revisionPtr revIDLastSave="125" documentId="13_ncr:1_{C8B25996-B8C9-45E8-BF5F-0058EDDB5306}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{B2D90656-DD48-4ECD-BB23-8C8D4EDECED3}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,9 +16,21 @@
     <sheet name="DOLAR_OBS_ADO" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$683</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">DOLAR_OBS_ADO!$A$3:$B$762</definedName>
+    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$762</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -35,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="5">
   <si>
     <t>Tipos de cambio (pesos por dólar)</t>
   </si>
@@ -56,7 +68,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -202,6 +214,21 @@
       <b/>
       <sz val="10"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -504,7 +531,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="42">
+  <cellStyleXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -547,6 +574,14 @@
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -569,7 +604,7 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="42">
+  <cellStyles count="50">
     <cellStyle name="20% - Énfasis1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Énfasis2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Énfasis3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -583,11 +618,17 @@
     <cellStyle name="40% - Énfasis5" xfId="36" builtinId="47" customBuiltin="1"/>
     <cellStyle name="40% - Énfasis6" xfId="40" builtinId="51" customBuiltin="1"/>
     <cellStyle name="60% - Énfasis1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Énfasis1 2" xfId="42" xr:uid="{4385A8D2-651C-4773-80CB-11F47798F1CE}"/>
     <cellStyle name="60% - Énfasis2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Énfasis2 2" xfId="43" xr:uid="{054221C2-13B6-4754-B0B6-C32A4E8A95AD}"/>
     <cellStyle name="60% - Énfasis3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Énfasis3 2" xfId="44" xr:uid="{BB28A6FF-22BE-46E4-B116-00518D401B6E}"/>
     <cellStyle name="60% - Énfasis4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Énfasis4 2" xfId="45" xr:uid="{D1C02AD5-7A4A-4764-935B-FAB4D7D87EE9}"/>
     <cellStyle name="60% - Énfasis5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Énfasis5 2" xfId="46" xr:uid="{9F6E8D91-7C00-42FF-8A7D-91C893DA4AB8}"/>
     <cellStyle name="60% - Énfasis6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="60% - Énfasis6 2" xfId="47" xr:uid="{1DF80BA0-24DE-4DA9-8EE2-A15003600F7C}"/>
     <cellStyle name="Bueno" xfId="6" builtinId="26" customBuiltin="1"/>
     <cellStyle name="Cálculo" xfId="11" builtinId="22" customBuiltin="1"/>
     <cellStyle name="Celda de comprobación" xfId="13" builtinId="23" customBuiltin="1"/>
@@ -603,6 +644,7 @@
     <cellStyle name="Entrada" xfId="9" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Incorrecto" xfId="7" builtinId="27" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
+    <cellStyle name="Neutral 2" xfId="48" xr:uid="{96B4E413-929F-4319-B3D6-5D1EF8AD0E76}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Notas" xfId="15" builtinId="10" customBuiltin="1"/>
     <cellStyle name="Salida" xfId="10" builtinId="21" customBuiltin="1"/>
@@ -611,6 +653,7 @@
     <cellStyle name="Título" xfId="1" builtinId="15" customBuiltin="1"/>
     <cellStyle name="Título 2" xfId="3" builtinId="17" customBuiltin="1"/>
     <cellStyle name="Título 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Título 4" xfId="49" xr:uid="{072D0298-5CC9-445D-BF36-9D06198D96B3}"/>
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -927,19 +970,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B683"/>
+  <dimension ref="A1:B762"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="4" topLeftCell="B671" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="4" topLeftCell="B761" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="B683" sqref="B683"/>
+      <selection pane="bottomRight" activeCell="B762" sqref="B762"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.5703125" customWidth="1"/>
-    <col min="2" max="2" width="15.5703125" customWidth="1"/>
+    <col min="1" max="1" width="12.7109375" customWidth="1"/>
+    <col min="2" max="2" width="14.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -6400,6 +6443,638 @@
       </c>
       <c r="B683" s="3">
         <v>760.9</v>
+      </c>
+    </row>
+    <row r="684" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A684" s="2">
+        <v>44147</v>
+      </c>
+      <c r="B684" s="3">
+        <v>757.42</v>
+      </c>
+    </row>
+    <row r="685" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A685" s="2">
+        <v>44148</v>
+      </c>
+      <c r="B685" s="3">
+        <v>757.43</v>
+      </c>
+    </row>
+    <row r="686" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A686" s="2">
+        <v>44149</v>
+      </c>
+      <c r="B686" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="687" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A687" s="2">
+        <v>44150</v>
+      </c>
+      <c r="B687" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="688" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A688" s="2">
+        <v>44151</v>
+      </c>
+      <c r="B688" s="3">
+        <v>766.7</v>
+      </c>
+    </row>
+    <row r="689" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A689" s="2">
+        <v>44152</v>
+      </c>
+      <c r="B689" s="3">
+        <v>767.86</v>
+      </c>
+    </row>
+    <row r="690" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A690" s="2">
+        <v>44153</v>
+      </c>
+      <c r="B690" s="3">
+        <v>767.05</v>
+      </c>
+    </row>
+    <row r="691" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A691" s="2">
+        <v>44154</v>
+      </c>
+      <c r="B691" s="3">
+        <v>758.1</v>
+      </c>
+    </row>
+    <row r="692" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A692" s="2">
+        <v>44155</v>
+      </c>
+      <c r="B692" s="3">
+        <v>758.62</v>
+      </c>
+    </row>
+    <row r="693" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A693" s="2">
+        <v>44156</v>
+      </c>
+      <c r="B693" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="694" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A694" s="2">
+        <v>44157</v>
+      </c>
+      <c r="B694" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="695" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A695" s="2">
+        <v>44158</v>
+      </c>
+      <c r="B695" s="3">
+        <v>761.55</v>
+      </c>
+    </row>
+    <row r="696" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A696" s="2">
+        <v>44159</v>
+      </c>
+      <c r="B696" s="3">
+        <v>765.96</v>
+      </c>
+    </row>
+    <row r="697" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A697" s="2">
+        <v>44160</v>
+      </c>
+      <c r="B697" s="3">
+        <v>772.83</v>
+      </c>
+    </row>
+    <row r="698" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A698" s="2">
+        <v>44161</v>
+      </c>
+      <c r="B698" s="3">
+        <v>771.68</v>
+      </c>
+    </row>
+    <row r="699" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A699" s="2">
+        <v>44162</v>
+      </c>
+      <c r="B699" s="3">
+        <v>766</v>
+      </c>
+    </row>
+    <row r="700" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A700" s="2">
+        <v>44163</v>
+      </c>
+      <c r="B700" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="701" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A701" s="2">
+        <v>44164</v>
+      </c>
+      <c r="B701" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="702" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A702" s="2">
+        <v>44165</v>
+      </c>
+      <c r="B702" s="3">
+        <v>766.69</v>
+      </c>
+    </row>
+    <row r="703" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A703" s="2">
+        <v>44166</v>
+      </c>
+      <c r="B703" s="3">
+        <v>767.29</v>
+      </c>
+    </row>
+    <row r="704" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A704" s="2">
+        <v>44167</v>
+      </c>
+      <c r="B704" s="3">
+        <v>760.16</v>
+      </c>
+    </row>
+    <row r="705" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A705" s="2">
+        <v>44168</v>
+      </c>
+      <c r="B705" s="3">
+        <v>755.34</v>
+      </c>
+    </row>
+    <row r="706" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A706" s="2">
+        <v>44169</v>
+      </c>
+      <c r="B706" s="3">
+        <v>752.03</v>
+      </c>
+    </row>
+    <row r="707" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A707" s="2">
+        <v>44170</v>
+      </c>
+      <c r="B707" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="708" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A708" s="2">
+        <v>44171</v>
+      </c>
+      <c r="B708" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="709" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A709" s="2">
+        <v>44172</v>
+      </c>
+      <c r="B709" s="3">
+        <v>747.61</v>
+      </c>
+    </row>
+    <row r="710" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A710" s="2">
+        <v>44173</v>
+      </c>
+      <c r="B710" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="711" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A711" s="2">
+        <v>44174</v>
+      </c>
+      <c r="B711" s="3">
+        <v>744.82</v>
+      </c>
+    </row>
+    <row r="712" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A712" s="2">
+        <v>44175</v>
+      </c>
+      <c r="B712" s="3">
+        <v>739.45</v>
+      </c>
+    </row>
+    <row r="713" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A713" s="2">
+        <v>44176</v>
+      </c>
+      <c r="B713" s="3">
+        <v>738.17</v>
+      </c>
+    </row>
+    <row r="714" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A714" s="2">
+        <v>44177</v>
+      </c>
+      <c r="B714" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="715" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A715" s="2">
+        <v>44178</v>
+      </c>
+      <c r="B715" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="716" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A716" s="2">
+        <v>44179</v>
+      </c>
+      <c r="B716" s="3">
+        <v>733.55</v>
+      </c>
+    </row>
+    <row r="717" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A717" s="2">
+        <v>44180</v>
+      </c>
+      <c r="B717" s="3">
+        <v>731.58</v>
+      </c>
+    </row>
+    <row r="718" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A718" s="2">
+        <v>44181</v>
+      </c>
+      <c r="B718" s="3">
+        <v>734.23</v>
+      </c>
+    </row>
+    <row r="719" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A719" s="2">
+        <v>44182</v>
+      </c>
+      <c r="B719" s="3">
+        <v>735.09</v>
+      </c>
+    </row>
+    <row r="720" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A720" s="2">
+        <v>44183</v>
+      </c>
+      <c r="B720" s="3">
+        <v>723.44</v>
+      </c>
+    </row>
+    <row r="721" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A721" s="2">
+        <v>44184</v>
+      </c>
+      <c r="B721" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="722" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A722" s="2">
+        <v>44185</v>
+      </c>
+      <c r="B722" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="723" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A723" s="2">
+        <v>44186</v>
+      </c>
+      <c r="B723" s="3">
+        <v>723.85</v>
+      </c>
+    </row>
+    <row r="724" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A724" s="2">
+        <v>44187</v>
+      </c>
+      <c r="B724" s="3">
+        <v>730.7</v>
+      </c>
+    </row>
+    <row r="725" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A725" s="2">
+        <v>44188</v>
+      </c>
+      <c r="B725" s="3">
+        <v>728.96</v>
+      </c>
+    </row>
+    <row r="726" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A726" s="2">
+        <v>44189</v>
+      </c>
+      <c r="B726" s="3">
+        <v>716.25</v>
+      </c>
+    </row>
+    <row r="727" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A727" s="2">
+        <v>44190</v>
+      </c>
+      <c r="B727" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="728" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A728" s="2">
+        <v>44191</v>
+      </c>
+      <c r="B728" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="729" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A729" s="2">
+        <v>44192</v>
+      </c>
+      <c r="B729" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="730" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A730" s="2">
+        <v>44193</v>
+      </c>
+      <c r="B730" s="3">
+        <v>710.26</v>
+      </c>
+    </row>
+    <row r="731" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A731" s="2">
+        <v>44194</v>
+      </c>
+      <c r="B731" s="3">
+        <v>710.64</v>
+      </c>
+    </row>
+    <row r="732" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A732" s="2">
+        <v>44195</v>
+      </c>
+      <c r="B732" s="3">
+        <v>711.24</v>
+      </c>
+    </row>
+    <row r="733" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A733" s="2">
+        <v>44196</v>
+      </c>
+      <c r="B733" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="734" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A734" s="2">
+        <v>44197</v>
+      </c>
+      <c r="B734" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="735" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A735" s="2">
+        <v>44198</v>
+      </c>
+      <c r="B735" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="736" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A736" s="2">
+        <v>44199</v>
+      </c>
+      <c r="B736" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="737" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A737" s="2">
+        <v>44200</v>
+      </c>
+      <c r="B737" s="3">
+        <v>710.95</v>
+      </c>
+    </row>
+    <row r="738" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A738" s="2">
+        <v>44201</v>
+      </c>
+      <c r="B738" s="3">
+        <v>702.93</v>
+      </c>
+    </row>
+    <row r="739" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A739" s="2">
+        <v>44202</v>
+      </c>
+      <c r="B739" s="3">
+        <v>702.29</v>
+      </c>
+    </row>
+    <row r="740" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A740" s="2">
+        <v>44203</v>
+      </c>
+      <c r="B740" s="3">
+        <v>696.18</v>
+      </c>
+    </row>
+    <row r="741" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A741" s="2">
+        <v>44204</v>
+      </c>
+      <c r="B741" s="3">
+        <v>709.99</v>
+      </c>
+    </row>
+    <row r="742" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A742" s="2">
+        <v>44205</v>
+      </c>
+      <c r="B742" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="743" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A743" s="2">
+        <v>44206</v>
+      </c>
+      <c r="B743" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="744" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A744" s="2">
+        <v>44207</v>
+      </c>
+      <c r="B744" s="3">
+        <v>713.28</v>
+      </c>
+    </row>
+    <row r="745" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A745" s="2">
+        <v>44208</v>
+      </c>
+      <c r="B745" s="3">
+        <v>718.89</v>
+      </c>
+    </row>
+    <row r="746" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A746" s="2">
+        <v>44209</v>
+      </c>
+      <c r="B746" s="3">
+        <v>725.24</v>
+      </c>
+    </row>
+    <row r="747" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A747" s="2">
+        <v>44210</v>
+      </c>
+      <c r="B747" s="3">
+        <v>739.72</v>
+      </c>
+    </row>
+    <row r="748" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A748" s="2">
+        <v>44211</v>
+      </c>
+      <c r="B748" s="3">
+        <v>735.35</v>
+      </c>
+    </row>
+    <row r="749" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A749" s="2">
+        <v>44212</v>
+      </c>
+      <c r="B749" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="750" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A750" s="2">
+        <v>44213</v>
+      </c>
+      <c r="B750" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="751" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A751" s="2">
+        <v>44214</v>
+      </c>
+      <c r="B751" s="3">
+        <v>735.06</v>
+      </c>
+    </row>
+    <row r="752" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A752" s="2">
+        <v>44215</v>
+      </c>
+      <c r="B752" s="3">
+        <v>736.11</v>
+      </c>
+    </row>
+    <row r="753" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A753" s="2">
+        <v>44216</v>
+      </c>
+      <c r="B753" s="3">
+        <v>733.73</v>
+      </c>
+    </row>
+    <row r="754" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A754" s="2">
+        <v>44217</v>
+      </c>
+      <c r="B754" s="3">
+        <v>730.38</v>
+      </c>
+    </row>
+    <row r="755" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A755" s="2">
+        <v>44218</v>
+      </c>
+      <c r="B755" s="3">
+        <v>715.56</v>
+      </c>
+    </row>
+    <row r="756" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A756" s="2">
+        <v>44219</v>
+      </c>
+      <c r="B756" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="757" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A757" s="2">
+        <v>44220</v>
+      </c>
+      <c r="B757" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="758" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A758" s="2">
+        <v>44221</v>
+      </c>
+      <c r="B758" s="3">
+        <v>724.26</v>
+      </c>
+    </row>
+    <row r="759" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A759" s="2">
+        <v>44222</v>
+      </c>
+      <c r="B759" s="3">
+        <v>731.92</v>
+      </c>
+    </row>
+    <row r="760" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A760" s="2">
+        <v>44223</v>
+      </c>
+      <c r="B760" s="3">
+        <v>731</v>
+      </c>
+    </row>
+    <row r="761" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A761" s="2">
+        <v>44224</v>
+      </c>
+      <c r="B761" s="3">
+        <v>736.88</v>
+      </c>
+    </row>
+    <row r="762" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A762" s="2">
+        <v>44225</v>
+      </c>
+      <c r="B762" s="3">
+        <v>741.4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update automatico via Actualizar 02-06-2021 17-08-51
</commit_message>
<xml_diff>
--- a/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
+++ b/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID CL/IndicadoresEconomicos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="125" documentId="13_ncr:1_{C8B25996-B8C9-45E8-BF5F-0058EDDB5306}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{B2D90656-DD48-4ECD-BB23-8C8D4EDECED3}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="14_{F2753A6D-642C-43B1-9D50-7716AF012233}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{EB69DD7D-6DC7-40C7-A6EB-3567AAC68B32}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,21 +16,9 @@
     <sheet name="DOLAR_OBS_ADO" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">DOLAR_OBS_ADO!$A$3:$B$762</definedName>
-    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$762</definedName>
+    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$683</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -47,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="5">
   <si>
     <t>Tipos de cambio (pesos por dólar)</t>
   </si>
@@ -68,7 +56,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="22" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -214,21 +202,6 @@
       <b/>
       <sz val="10"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri Light"/>
-      <family val="2"/>
-      <scheme val="major"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -531,7 +504,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="50">
+  <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -574,14 +547,6 @@
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -604,7 +569,7 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="50">
+  <cellStyles count="42">
     <cellStyle name="20% - Énfasis1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Énfasis2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Énfasis3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -618,17 +583,11 @@
     <cellStyle name="40% - Énfasis5" xfId="36" builtinId="47" customBuiltin="1"/>
     <cellStyle name="40% - Énfasis6" xfId="40" builtinId="51" customBuiltin="1"/>
     <cellStyle name="60% - Énfasis1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% - Énfasis1 2" xfId="42" xr:uid="{4385A8D2-651C-4773-80CB-11F47798F1CE}"/>
     <cellStyle name="60% - Énfasis2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% - Énfasis2 2" xfId="43" xr:uid="{054221C2-13B6-4754-B0B6-C32A4E8A95AD}"/>
     <cellStyle name="60% - Énfasis3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% - Énfasis3 2" xfId="44" xr:uid="{BB28A6FF-22BE-46E4-B116-00518D401B6E}"/>
     <cellStyle name="60% - Énfasis4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% - Énfasis4 2" xfId="45" xr:uid="{D1C02AD5-7A4A-4764-935B-FAB4D7D87EE9}"/>
     <cellStyle name="60% - Énfasis5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% - Énfasis5 2" xfId="46" xr:uid="{9F6E8D91-7C00-42FF-8A7D-91C893DA4AB8}"/>
     <cellStyle name="60% - Énfasis6" xfId="41" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="60% - Énfasis6 2" xfId="47" xr:uid="{1DF80BA0-24DE-4DA9-8EE2-A15003600F7C}"/>
     <cellStyle name="Bueno" xfId="6" builtinId="26" customBuiltin="1"/>
     <cellStyle name="Cálculo" xfId="11" builtinId="22" customBuiltin="1"/>
     <cellStyle name="Celda de comprobación" xfId="13" builtinId="23" customBuiltin="1"/>
@@ -644,7 +603,6 @@
     <cellStyle name="Entrada" xfId="9" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Incorrecto" xfId="7" builtinId="27" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
-    <cellStyle name="Neutral 2" xfId="48" xr:uid="{96B4E413-929F-4319-B3D6-5D1EF8AD0E76}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Notas" xfId="15" builtinId="10" customBuiltin="1"/>
     <cellStyle name="Salida" xfId="10" builtinId="21" customBuiltin="1"/>
@@ -653,7 +611,6 @@
     <cellStyle name="Título" xfId="1" builtinId="15" customBuiltin="1"/>
     <cellStyle name="Título 2" xfId="3" builtinId="17" customBuiltin="1"/>
     <cellStyle name="Título 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Título 4" xfId="49" xr:uid="{072D0298-5CC9-445D-BF36-9D06198D96B3}"/>
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -970,19 +927,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B762"/>
+  <dimension ref="A1:B683"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="4" topLeftCell="B761" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="4" topLeftCell="B671" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="B762" sqref="B762"/>
+      <selection pane="bottomRight" activeCell="B683" sqref="B683"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.7109375" customWidth="1"/>
-    <col min="2" max="2" width="14.42578125" customWidth="1"/>
+    <col min="1" max="1" width="11.5703125" customWidth="1"/>
+    <col min="2" max="2" width="15.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -6443,638 +6400,6 @@
       </c>
       <c r="B683" s="3">
         <v>760.9</v>
-      </c>
-    </row>
-    <row r="684" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A684" s="2">
-        <v>44147</v>
-      </c>
-      <c r="B684" s="3">
-        <v>757.42</v>
-      </c>
-    </row>
-    <row r="685" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A685" s="2">
-        <v>44148</v>
-      </c>
-      <c r="B685" s="3">
-        <v>757.43</v>
-      </c>
-    </row>
-    <row r="686" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A686" s="2">
-        <v>44149</v>
-      </c>
-      <c r="B686" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="687" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A687" s="2">
-        <v>44150</v>
-      </c>
-      <c r="B687" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="688" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A688" s="2">
-        <v>44151</v>
-      </c>
-      <c r="B688" s="3">
-        <v>766.7</v>
-      </c>
-    </row>
-    <row r="689" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A689" s="2">
-        <v>44152</v>
-      </c>
-      <c r="B689" s="3">
-        <v>767.86</v>
-      </c>
-    </row>
-    <row r="690" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A690" s="2">
-        <v>44153</v>
-      </c>
-      <c r="B690" s="3">
-        <v>767.05</v>
-      </c>
-    </row>
-    <row r="691" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A691" s="2">
-        <v>44154</v>
-      </c>
-      <c r="B691" s="3">
-        <v>758.1</v>
-      </c>
-    </row>
-    <row r="692" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A692" s="2">
-        <v>44155</v>
-      </c>
-      <c r="B692" s="3">
-        <v>758.62</v>
-      </c>
-    </row>
-    <row r="693" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A693" s="2">
-        <v>44156</v>
-      </c>
-      <c r="B693" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="694" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A694" s="2">
-        <v>44157</v>
-      </c>
-      <c r="B694" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="695" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A695" s="2">
-        <v>44158</v>
-      </c>
-      <c r="B695" s="3">
-        <v>761.55</v>
-      </c>
-    </row>
-    <row r="696" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A696" s="2">
-        <v>44159</v>
-      </c>
-      <c r="B696" s="3">
-        <v>765.96</v>
-      </c>
-    </row>
-    <row r="697" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A697" s="2">
-        <v>44160</v>
-      </c>
-      <c r="B697" s="3">
-        <v>772.83</v>
-      </c>
-    </row>
-    <row r="698" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A698" s="2">
-        <v>44161</v>
-      </c>
-      <c r="B698" s="3">
-        <v>771.68</v>
-      </c>
-    </row>
-    <row r="699" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A699" s="2">
-        <v>44162</v>
-      </c>
-      <c r="B699" s="3">
-        <v>766</v>
-      </c>
-    </row>
-    <row r="700" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A700" s="2">
-        <v>44163</v>
-      </c>
-      <c r="B700" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="701" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A701" s="2">
-        <v>44164</v>
-      </c>
-      <c r="B701" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="702" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A702" s="2">
-        <v>44165</v>
-      </c>
-      <c r="B702" s="3">
-        <v>766.69</v>
-      </c>
-    </row>
-    <row r="703" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A703" s="2">
-        <v>44166</v>
-      </c>
-      <c r="B703" s="3">
-        <v>767.29</v>
-      </c>
-    </row>
-    <row r="704" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A704" s="2">
-        <v>44167</v>
-      </c>
-      <c r="B704" s="3">
-        <v>760.16</v>
-      </c>
-    </row>
-    <row r="705" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A705" s="2">
-        <v>44168</v>
-      </c>
-      <c r="B705" s="3">
-        <v>755.34</v>
-      </c>
-    </row>
-    <row r="706" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A706" s="2">
-        <v>44169</v>
-      </c>
-      <c r="B706" s="3">
-        <v>752.03</v>
-      </c>
-    </row>
-    <row r="707" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A707" s="2">
-        <v>44170</v>
-      </c>
-      <c r="B707" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="708" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A708" s="2">
-        <v>44171</v>
-      </c>
-      <c r="B708" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="709" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A709" s="2">
-        <v>44172</v>
-      </c>
-      <c r="B709" s="3">
-        <v>747.61</v>
-      </c>
-    </row>
-    <row r="710" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A710" s="2">
-        <v>44173</v>
-      </c>
-      <c r="B710" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="711" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A711" s="2">
-        <v>44174</v>
-      </c>
-      <c r="B711" s="3">
-        <v>744.82</v>
-      </c>
-    </row>
-    <row r="712" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A712" s="2">
-        <v>44175</v>
-      </c>
-      <c r="B712" s="3">
-        <v>739.45</v>
-      </c>
-    </row>
-    <row r="713" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A713" s="2">
-        <v>44176</v>
-      </c>
-      <c r="B713" s="3">
-        <v>738.17</v>
-      </c>
-    </row>
-    <row r="714" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A714" s="2">
-        <v>44177</v>
-      </c>
-      <c r="B714" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="715" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A715" s="2">
-        <v>44178</v>
-      </c>
-      <c r="B715" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="716" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A716" s="2">
-        <v>44179</v>
-      </c>
-      <c r="B716" s="3">
-        <v>733.55</v>
-      </c>
-    </row>
-    <row r="717" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A717" s="2">
-        <v>44180</v>
-      </c>
-      <c r="B717" s="3">
-        <v>731.58</v>
-      </c>
-    </row>
-    <row r="718" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A718" s="2">
-        <v>44181</v>
-      </c>
-      <c r="B718" s="3">
-        <v>734.23</v>
-      </c>
-    </row>
-    <row r="719" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A719" s="2">
-        <v>44182</v>
-      </c>
-      <c r="B719" s="3">
-        <v>735.09</v>
-      </c>
-    </row>
-    <row r="720" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A720" s="2">
-        <v>44183</v>
-      </c>
-      <c r="B720" s="3">
-        <v>723.44</v>
-      </c>
-    </row>
-    <row r="721" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A721" s="2">
-        <v>44184</v>
-      </c>
-      <c r="B721" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="722" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A722" s="2">
-        <v>44185</v>
-      </c>
-      <c r="B722" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="723" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A723" s="2">
-        <v>44186</v>
-      </c>
-      <c r="B723" s="3">
-        <v>723.85</v>
-      </c>
-    </row>
-    <row r="724" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A724" s="2">
-        <v>44187</v>
-      </c>
-      <c r="B724" s="3">
-        <v>730.7</v>
-      </c>
-    </row>
-    <row r="725" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A725" s="2">
-        <v>44188</v>
-      </c>
-      <c r="B725" s="3">
-        <v>728.96</v>
-      </c>
-    </row>
-    <row r="726" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A726" s="2">
-        <v>44189</v>
-      </c>
-      <c r="B726" s="3">
-        <v>716.25</v>
-      </c>
-    </row>
-    <row r="727" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A727" s="2">
-        <v>44190</v>
-      </c>
-      <c r="B727" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="728" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A728" s="2">
-        <v>44191</v>
-      </c>
-      <c r="B728" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="729" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A729" s="2">
-        <v>44192</v>
-      </c>
-      <c r="B729" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="730" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A730" s="2">
-        <v>44193</v>
-      </c>
-      <c r="B730" s="3">
-        <v>710.26</v>
-      </c>
-    </row>
-    <row r="731" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A731" s="2">
-        <v>44194</v>
-      </c>
-      <c r="B731" s="3">
-        <v>710.64</v>
-      </c>
-    </row>
-    <row r="732" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A732" s="2">
-        <v>44195</v>
-      </c>
-      <c r="B732" s="3">
-        <v>711.24</v>
-      </c>
-    </row>
-    <row r="733" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A733" s="2">
-        <v>44196</v>
-      </c>
-      <c r="B733" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="734" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A734" s="2">
-        <v>44197</v>
-      </c>
-      <c r="B734" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="735" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A735" s="2">
-        <v>44198</v>
-      </c>
-      <c r="B735" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="736" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A736" s="2">
-        <v>44199</v>
-      </c>
-      <c r="B736" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="737" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A737" s="2">
-        <v>44200</v>
-      </c>
-      <c r="B737" s="3">
-        <v>710.95</v>
-      </c>
-    </row>
-    <row r="738" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A738" s="2">
-        <v>44201</v>
-      </c>
-      <c r="B738" s="3">
-        <v>702.93</v>
-      </c>
-    </row>
-    <row r="739" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A739" s="2">
-        <v>44202</v>
-      </c>
-      <c r="B739" s="3">
-        <v>702.29</v>
-      </c>
-    </row>
-    <row r="740" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A740" s="2">
-        <v>44203</v>
-      </c>
-      <c r="B740" s="3">
-        <v>696.18</v>
-      </c>
-    </row>
-    <row r="741" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A741" s="2">
-        <v>44204</v>
-      </c>
-      <c r="B741" s="3">
-        <v>709.99</v>
-      </c>
-    </row>
-    <row r="742" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A742" s="2">
-        <v>44205</v>
-      </c>
-      <c r="B742" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="743" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A743" s="2">
-        <v>44206</v>
-      </c>
-      <c r="B743" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="744" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A744" s="2">
-        <v>44207</v>
-      </c>
-      <c r="B744" s="3">
-        <v>713.28</v>
-      </c>
-    </row>
-    <row r="745" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A745" s="2">
-        <v>44208</v>
-      </c>
-      <c r="B745" s="3">
-        <v>718.89</v>
-      </c>
-    </row>
-    <row r="746" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A746" s="2">
-        <v>44209</v>
-      </c>
-      <c r="B746" s="3">
-        <v>725.24</v>
-      </c>
-    </row>
-    <row r="747" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A747" s="2">
-        <v>44210</v>
-      </c>
-      <c r="B747" s="3">
-        <v>739.72</v>
-      </c>
-    </row>
-    <row r="748" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A748" s="2">
-        <v>44211</v>
-      </c>
-      <c r="B748" s="3">
-        <v>735.35</v>
-      </c>
-    </row>
-    <row r="749" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A749" s="2">
-        <v>44212</v>
-      </c>
-      <c r="B749" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="750" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A750" s="2">
-        <v>44213</v>
-      </c>
-      <c r="B750" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="751" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A751" s="2">
-        <v>44214</v>
-      </c>
-      <c r="B751" s="3">
-        <v>735.06</v>
-      </c>
-    </row>
-    <row r="752" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A752" s="2">
-        <v>44215</v>
-      </c>
-      <c r="B752" s="3">
-        <v>736.11</v>
-      </c>
-    </row>
-    <row r="753" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A753" s="2">
-        <v>44216</v>
-      </c>
-      <c r="B753" s="3">
-        <v>733.73</v>
-      </c>
-    </row>
-    <row r="754" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A754" s="2">
-        <v>44217</v>
-      </c>
-      <c r="B754" s="3">
-        <v>730.38</v>
-      </c>
-    </row>
-    <row r="755" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A755" s="2">
-        <v>44218</v>
-      </c>
-      <c r="B755" s="3">
-        <v>715.56</v>
-      </c>
-    </row>
-    <row r="756" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A756" s="2">
-        <v>44219</v>
-      </c>
-      <c r="B756" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="757" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A757" s="2">
-        <v>44220</v>
-      </c>
-      <c r="B757" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="758" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A758" s="2">
-        <v>44221</v>
-      </c>
-      <c r="B758" s="3">
-        <v>724.26</v>
-      </c>
-    </row>
-    <row r="759" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A759" s="2">
-        <v>44222</v>
-      </c>
-      <c r="B759" s="3">
-        <v>731.92</v>
-      </c>
-    </row>
-    <row r="760" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A760" s="2">
-        <v>44223</v>
-      </c>
-      <c r="B760" s="3">
-        <v>731</v>
-      </c>
-    </row>
-    <row r="761" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A761" s="2">
-        <v>44224</v>
-      </c>
-      <c r="B761" s="3">
-        <v>736.88</v>
-      </c>
-    </row>
-    <row r="762" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A762" s="2">
-        <v>44225</v>
-      </c>
-      <c r="B762" s="3">
-        <v>741.4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update automatico via Actualizar 02-06-2021 19-09-47
</commit_message>
<xml_diff>
--- a/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
+++ b/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID CL/IndicadoresEconomicos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="14_{F2753A6D-642C-43B1-9D50-7716AF012233}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{EB69DD7D-6DC7-40C7-A6EB-3567AAC68B32}"/>
+  <xr:revisionPtr revIDLastSave="125" documentId="13_ncr:1_{C8B25996-B8C9-45E8-BF5F-0058EDDB5306}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{B2D90656-DD48-4ECD-BB23-8C8D4EDECED3}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,9 +16,21 @@
     <sheet name="DOLAR_OBS_ADO" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$683</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">DOLAR_OBS_ADO!$A$3:$B$762</definedName>
+    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$762</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -35,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="5">
   <si>
     <t>Tipos de cambio (pesos por dólar)</t>
   </si>
@@ -56,7 +68,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -202,6 +214,21 @@
       <b/>
       <sz val="10"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -504,7 +531,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="42">
+  <cellStyleXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -547,6 +574,14 @@
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -569,7 +604,7 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="42">
+  <cellStyles count="50">
     <cellStyle name="20% - Énfasis1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Énfasis2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Énfasis3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -583,11 +618,17 @@
     <cellStyle name="40% - Énfasis5" xfId="36" builtinId="47" customBuiltin="1"/>
     <cellStyle name="40% - Énfasis6" xfId="40" builtinId="51" customBuiltin="1"/>
     <cellStyle name="60% - Énfasis1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Énfasis1 2" xfId="42" xr:uid="{4385A8D2-651C-4773-80CB-11F47798F1CE}"/>
     <cellStyle name="60% - Énfasis2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Énfasis2 2" xfId="43" xr:uid="{054221C2-13B6-4754-B0B6-C32A4E8A95AD}"/>
     <cellStyle name="60% - Énfasis3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Énfasis3 2" xfId="44" xr:uid="{BB28A6FF-22BE-46E4-B116-00518D401B6E}"/>
     <cellStyle name="60% - Énfasis4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Énfasis4 2" xfId="45" xr:uid="{D1C02AD5-7A4A-4764-935B-FAB4D7D87EE9}"/>
     <cellStyle name="60% - Énfasis5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Énfasis5 2" xfId="46" xr:uid="{9F6E8D91-7C00-42FF-8A7D-91C893DA4AB8}"/>
     <cellStyle name="60% - Énfasis6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="60% - Énfasis6 2" xfId="47" xr:uid="{1DF80BA0-24DE-4DA9-8EE2-A15003600F7C}"/>
     <cellStyle name="Bueno" xfId="6" builtinId="26" customBuiltin="1"/>
     <cellStyle name="Cálculo" xfId="11" builtinId="22" customBuiltin="1"/>
     <cellStyle name="Celda de comprobación" xfId="13" builtinId="23" customBuiltin="1"/>
@@ -603,6 +644,7 @@
     <cellStyle name="Entrada" xfId="9" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Incorrecto" xfId="7" builtinId="27" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
+    <cellStyle name="Neutral 2" xfId="48" xr:uid="{96B4E413-929F-4319-B3D6-5D1EF8AD0E76}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Notas" xfId="15" builtinId="10" customBuiltin="1"/>
     <cellStyle name="Salida" xfId="10" builtinId="21" customBuiltin="1"/>
@@ -611,6 +653,7 @@
     <cellStyle name="Título" xfId="1" builtinId="15" customBuiltin="1"/>
     <cellStyle name="Título 2" xfId="3" builtinId="17" customBuiltin="1"/>
     <cellStyle name="Título 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Título 4" xfId="49" xr:uid="{072D0298-5CC9-445D-BF36-9D06198D96B3}"/>
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -927,19 +970,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B683"/>
+  <dimension ref="A1:B762"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="4" topLeftCell="B671" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="4" topLeftCell="B761" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="B683" sqref="B683"/>
+      <selection pane="bottomRight" activeCell="B762" sqref="B762"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.5703125" customWidth="1"/>
-    <col min="2" max="2" width="15.5703125" customWidth="1"/>
+    <col min="1" max="1" width="12.7109375" customWidth="1"/>
+    <col min="2" max="2" width="14.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -6400,6 +6443,638 @@
       </c>
       <c r="B683" s="3">
         <v>760.9</v>
+      </c>
+    </row>
+    <row r="684" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A684" s="2">
+        <v>44147</v>
+      </c>
+      <c r="B684" s="3">
+        <v>757.42</v>
+      </c>
+    </row>
+    <row r="685" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A685" s="2">
+        <v>44148</v>
+      </c>
+      <c r="B685" s="3">
+        <v>757.43</v>
+      </c>
+    </row>
+    <row r="686" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A686" s="2">
+        <v>44149</v>
+      </c>
+      <c r="B686" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="687" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A687" s="2">
+        <v>44150</v>
+      </c>
+      <c r="B687" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="688" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A688" s="2">
+        <v>44151</v>
+      </c>
+      <c r="B688" s="3">
+        <v>766.7</v>
+      </c>
+    </row>
+    <row r="689" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A689" s="2">
+        <v>44152</v>
+      </c>
+      <c r="B689" s="3">
+        <v>767.86</v>
+      </c>
+    </row>
+    <row r="690" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A690" s="2">
+        <v>44153</v>
+      </c>
+      <c r="B690" s="3">
+        <v>767.05</v>
+      </c>
+    </row>
+    <row r="691" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A691" s="2">
+        <v>44154</v>
+      </c>
+      <c r="B691" s="3">
+        <v>758.1</v>
+      </c>
+    </row>
+    <row r="692" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A692" s="2">
+        <v>44155</v>
+      </c>
+      <c r="B692" s="3">
+        <v>758.62</v>
+      </c>
+    </row>
+    <row r="693" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A693" s="2">
+        <v>44156</v>
+      </c>
+      <c r="B693" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="694" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A694" s="2">
+        <v>44157</v>
+      </c>
+      <c r="B694" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="695" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A695" s="2">
+        <v>44158</v>
+      </c>
+      <c r="B695" s="3">
+        <v>761.55</v>
+      </c>
+    </row>
+    <row r="696" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A696" s="2">
+        <v>44159</v>
+      </c>
+      <c r="B696" s="3">
+        <v>765.96</v>
+      </c>
+    </row>
+    <row r="697" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A697" s="2">
+        <v>44160</v>
+      </c>
+      <c r="B697" s="3">
+        <v>772.83</v>
+      </c>
+    </row>
+    <row r="698" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A698" s="2">
+        <v>44161</v>
+      </c>
+      <c r="B698" s="3">
+        <v>771.68</v>
+      </c>
+    </row>
+    <row r="699" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A699" s="2">
+        <v>44162</v>
+      </c>
+      <c r="B699" s="3">
+        <v>766</v>
+      </c>
+    </row>
+    <row r="700" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A700" s="2">
+        <v>44163</v>
+      </c>
+      <c r="B700" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="701" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A701" s="2">
+        <v>44164</v>
+      </c>
+      <c r="B701" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="702" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A702" s="2">
+        <v>44165</v>
+      </c>
+      <c r="B702" s="3">
+        <v>766.69</v>
+      </c>
+    </row>
+    <row r="703" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A703" s="2">
+        <v>44166</v>
+      </c>
+      <c r="B703" s="3">
+        <v>767.29</v>
+      </c>
+    </row>
+    <row r="704" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A704" s="2">
+        <v>44167</v>
+      </c>
+      <c r="B704" s="3">
+        <v>760.16</v>
+      </c>
+    </row>
+    <row r="705" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A705" s="2">
+        <v>44168</v>
+      </c>
+      <c r="B705" s="3">
+        <v>755.34</v>
+      </c>
+    </row>
+    <row r="706" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A706" s="2">
+        <v>44169</v>
+      </c>
+      <c r="B706" s="3">
+        <v>752.03</v>
+      </c>
+    </row>
+    <row r="707" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A707" s="2">
+        <v>44170</v>
+      </c>
+      <c r="B707" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="708" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A708" s="2">
+        <v>44171</v>
+      </c>
+      <c r="B708" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="709" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A709" s="2">
+        <v>44172</v>
+      </c>
+      <c r="B709" s="3">
+        <v>747.61</v>
+      </c>
+    </row>
+    <row r="710" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A710" s="2">
+        <v>44173</v>
+      </c>
+      <c r="B710" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="711" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A711" s="2">
+        <v>44174</v>
+      </c>
+      <c r="B711" s="3">
+        <v>744.82</v>
+      </c>
+    </row>
+    <row r="712" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A712" s="2">
+        <v>44175</v>
+      </c>
+      <c r="B712" s="3">
+        <v>739.45</v>
+      </c>
+    </row>
+    <row r="713" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A713" s="2">
+        <v>44176</v>
+      </c>
+      <c r="B713" s="3">
+        <v>738.17</v>
+      </c>
+    </row>
+    <row r="714" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A714" s="2">
+        <v>44177</v>
+      </c>
+      <c r="B714" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="715" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A715" s="2">
+        <v>44178</v>
+      </c>
+      <c r="B715" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="716" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A716" s="2">
+        <v>44179</v>
+      </c>
+      <c r="B716" s="3">
+        <v>733.55</v>
+      </c>
+    </row>
+    <row r="717" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A717" s="2">
+        <v>44180</v>
+      </c>
+      <c r="B717" s="3">
+        <v>731.58</v>
+      </c>
+    </row>
+    <row r="718" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A718" s="2">
+        <v>44181</v>
+      </c>
+      <c r="B718" s="3">
+        <v>734.23</v>
+      </c>
+    </row>
+    <row r="719" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A719" s="2">
+        <v>44182</v>
+      </c>
+      <c r="B719" s="3">
+        <v>735.09</v>
+      </c>
+    </row>
+    <row r="720" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A720" s="2">
+        <v>44183</v>
+      </c>
+      <c r="B720" s="3">
+        <v>723.44</v>
+      </c>
+    </row>
+    <row r="721" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A721" s="2">
+        <v>44184</v>
+      </c>
+      <c r="B721" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="722" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A722" s="2">
+        <v>44185</v>
+      </c>
+      <c r="B722" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="723" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A723" s="2">
+        <v>44186</v>
+      </c>
+      <c r="B723" s="3">
+        <v>723.85</v>
+      </c>
+    </row>
+    <row r="724" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A724" s="2">
+        <v>44187</v>
+      </c>
+      <c r="B724" s="3">
+        <v>730.7</v>
+      </c>
+    </row>
+    <row r="725" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A725" s="2">
+        <v>44188</v>
+      </c>
+      <c r="B725" s="3">
+        <v>728.96</v>
+      </c>
+    </row>
+    <row r="726" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A726" s="2">
+        <v>44189</v>
+      </c>
+      <c r="B726" s="3">
+        <v>716.25</v>
+      </c>
+    </row>
+    <row r="727" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A727" s="2">
+        <v>44190</v>
+      </c>
+      <c r="B727" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="728" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A728" s="2">
+        <v>44191</v>
+      </c>
+      <c r="B728" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="729" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A729" s="2">
+        <v>44192</v>
+      </c>
+      <c r="B729" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="730" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A730" s="2">
+        <v>44193</v>
+      </c>
+      <c r="B730" s="3">
+        <v>710.26</v>
+      </c>
+    </row>
+    <row r="731" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A731" s="2">
+        <v>44194</v>
+      </c>
+      <c r="B731" s="3">
+        <v>710.64</v>
+      </c>
+    </row>
+    <row r="732" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A732" s="2">
+        <v>44195</v>
+      </c>
+      <c r="B732" s="3">
+        <v>711.24</v>
+      </c>
+    </row>
+    <row r="733" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A733" s="2">
+        <v>44196</v>
+      </c>
+      <c r="B733" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="734" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A734" s="2">
+        <v>44197</v>
+      </c>
+      <c r="B734" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="735" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A735" s="2">
+        <v>44198</v>
+      </c>
+      <c r="B735" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="736" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A736" s="2">
+        <v>44199</v>
+      </c>
+      <c r="B736" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="737" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A737" s="2">
+        <v>44200</v>
+      </c>
+      <c r="B737" s="3">
+        <v>710.95</v>
+      </c>
+    </row>
+    <row r="738" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A738" s="2">
+        <v>44201</v>
+      </c>
+      <c r="B738" s="3">
+        <v>702.93</v>
+      </c>
+    </row>
+    <row r="739" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A739" s="2">
+        <v>44202</v>
+      </c>
+      <c r="B739" s="3">
+        <v>702.29</v>
+      </c>
+    </row>
+    <row r="740" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A740" s="2">
+        <v>44203</v>
+      </c>
+      <c r="B740" s="3">
+        <v>696.18</v>
+      </c>
+    </row>
+    <row r="741" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A741" s="2">
+        <v>44204</v>
+      </c>
+      <c r="B741" s="3">
+        <v>709.99</v>
+      </c>
+    </row>
+    <row r="742" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A742" s="2">
+        <v>44205</v>
+      </c>
+      <c r="B742" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="743" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A743" s="2">
+        <v>44206</v>
+      </c>
+      <c r="B743" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="744" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A744" s="2">
+        <v>44207</v>
+      </c>
+      <c r="B744" s="3">
+        <v>713.28</v>
+      </c>
+    </row>
+    <row r="745" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A745" s="2">
+        <v>44208</v>
+      </c>
+      <c r="B745" s="3">
+        <v>718.89</v>
+      </c>
+    </row>
+    <row r="746" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A746" s="2">
+        <v>44209</v>
+      </c>
+      <c r="B746" s="3">
+        <v>725.24</v>
+      </c>
+    </row>
+    <row r="747" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A747" s="2">
+        <v>44210</v>
+      </c>
+      <c r="B747" s="3">
+        <v>739.72</v>
+      </c>
+    </row>
+    <row r="748" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A748" s="2">
+        <v>44211</v>
+      </c>
+      <c r="B748" s="3">
+        <v>735.35</v>
+      </c>
+    </row>
+    <row r="749" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A749" s="2">
+        <v>44212</v>
+      </c>
+      <c r="B749" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="750" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A750" s="2">
+        <v>44213</v>
+      </c>
+      <c r="B750" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="751" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A751" s="2">
+        <v>44214</v>
+      </c>
+      <c r="B751" s="3">
+        <v>735.06</v>
+      </c>
+    </row>
+    <row r="752" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A752" s="2">
+        <v>44215</v>
+      </c>
+      <c r="B752" s="3">
+        <v>736.11</v>
+      </c>
+    </row>
+    <row r="753" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A753" s="2">
+        <v>44216</v>
+      </c>
+      <c r="B753" s="3">
+        <v>733.73</v>
+      </c>
+    </row>
+    <row r="754" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A754" s="2">
+        <v>44217</v>
+      </c>
+      <c r="B754" s="3">
+        <v>730.38</v>
+      </c>
+    </row>
+    <row r="755" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A755" s="2">
+        <v>44218</v>
+      </c>
+      <c r="B755" s="3">
+        <v>715.56</v>
+      </c>
+    </row>
+    <row r="756" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A756" s="2">
+        <v>44219</v>
+      </c>
+      <c r="B756" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="757" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A757" s="2">
+        <v>44220</v>
+      </c>
+      <c r="B757" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="758" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A758" s="2">
+        <v>44221</v>
+      </c>
+      <c r="B758" s="3">
+        <v>724.26</v>
+      </c>
+    </row>
+    <row r="759" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A759" s="2">
+        <v>44222</v>
+      </c>
+      <c r="B759" s="3">
+        <v>731.92</v>
+      </c>
+    </row>
+    <row r="760" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A760" s="2">
+        <v>44223</v>
+      </c>
+      <c r="B760" s="3">
+        <v>731</v>
+      </c>
+    </row>
+    <row r="761" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A761" s="2">
+        <v>44224</v>
+      </c>
+      <c r="B761" s="3">
+        <v>736.88</v>
+      </c>
+    </row>
+    <row r="762" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A762" s="2">
+        <v>44225</v>
+      </c>
+      <c r="B762" s="3">
+        <v>741.4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update automatico via Actualizar 02-09-2021 14-26-34
</commit_message>
<xml_diff>
--- a/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
+++ b/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID CL/IndicadoresEconomicos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="125" documentId="13_ncr:1_{C8B25996-B8C9-45E8-BF5F-0058EDDB5306}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{B2D90656-DD48-4ECD-BB23-8C8D4EDECED3}"/>
+  <xr:revisionPtr revIDLastSave="127" documentId="13_ncr:1_{C8B25996-B8C9-45E8-BF5F-0058EDDB5306}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{A474993B-FE85-4F07-B4EB-2AD9898146C3}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,8 +16,8 @@
     <sheet name="DOLAR_OBS_ADO" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">DOLAR_OBS_ADO!$A$3:$B$762</definedName>
-    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$762</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">DOLAR_OBS_ADO!$A$3:$B$773</definedName>
+    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$773</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="5">
   <si>
     <t>Tipos de cambio (pesos por dólar)</t>
   </si>
@@ -970,19 +970,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B762"/>
+  <dimension ref="A1:B773"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="4" topLeftCell="B761" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="4" topLeftCell="B773" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="B762" sqref="B762"/>
+      <selection pane="bottomRight" activeCell="B773" sqref="B773"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.7109375" customWidth="1"/>
-    <col min="2" max="2" width="14.42578125" customWidth="1"/>
+    <col min="1" max="1" width="11.5703125" customWidth="1"/>
+    <col min="2" max="2" width="15.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -7075,6 +7075,94 @@
       </c>
       <c r="B762" s="3">
         <v>741.4</v>
+      </c>
+    </row>
+    <row r="763" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A763" s="2">
+        <v>44226</v>
+      </c>
+      <c r="B763" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="764" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A764" s="2">
+        <v>44227</v>
+      </c>
+      <c r="B764" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="765" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A765" s="2">
+        <v>44228</v>
+      </c>
+      <c r="B765" s="3">
+        <v>734.62</v>
+      </c>
+    </row>
+    <row r="766" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A766" s="2">
+        <v>44229</v>
+      </c>
+      <c r="B766" s="3">
+        <v>731.66</v>
+      </c>
+    </row>
+    <row r="767" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A767" s="2">
+        <v>44230</v>
+      </c>
+      <c r="B767" s="3">
+        <v>734.86</v>
+      </c>
+    </row>
+    <row r="768" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A768" s="2">
+        <v>44231</v>
+      </c>
+      <c r="B768" s="3">
+        <v>730.53</v>
+      </c>
+    </row>
+    <row r="769" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A769" s="2">
+        <v>44232</v>
+      </c>
+      <c r="B769" s="3">
+        <v>737.23</v>
+      </c>
+    </row>
+    <row r="770" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A770" s="2">
+        <v>44233</v>
+      </c>
+      <c r="B770" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="771" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A771" s="2">
+        <v>44234</v>
+      </c>
+      <c r="B771" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="772" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A772" s="2">
+        <v>44235</v>
+      </c>
+      <c r="B772" s="3">
+        <v>736.65</v>
+      </c>
+    </row>
+    <row r="773" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A773" s="2">
+        <v>44236</v>
+      </c>
+      <c r="B773" s="3">
+        <v>735.07</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update automatico via Actualizar 02-12-2021 17-09-32
</commit_message>
<xml_diff>
--- a/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
+++ b/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID CL/IndicadoresEconomicos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="127" documentId="13_ncr:1_{C8B25996-B8C9-45E8-BF5F-0058EDDB5306}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{A474993B-FE85-4F07-B4EB-2AD9898146C3}"/>
+  <xr:revisionPtr revIDLastSave="133" documentId="13_ncr:1_{C8B25996-B8C9-45E8-BF5F-0058EDDB5306}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{C6386B95-CF3D-489A-AAD0-F799B1385F99}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,8 +16,8 @@
     <sheet name="DOLAR_OBS_ADO" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">DOLAR_OBS_ADO!$A$3:$B$773</definedName>
-    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$773</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">DOLAR_OBS_ADO!$A$3:$B$776</definedName>
+    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$776</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -970,13 +970,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B773"/>
+  <dimension ref="A1:B776"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="4" topLeftCell="B773" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="4" topLeftCell="B775" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="B773" sqref="B773"/>
+      <selection pane="bottomRight" activeCell="A776" sqref="A776"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7165,6 +7165,30 @@
         <v>735.07</v>
       </c>
     </row>
+    <row r="774" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A774" s="2">
+        <v>44237</v>
+      </c>
+      <c r="B774" s="3">
+        <v>733.13</v>
+      </c>
+    </row>
+    <row r="775" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A775" s="2">
+        <v>44238</v>
+      </c>
+      <c r="B775" s="3">
+        <v>728.9</v>
+      </c>
+    </row>
+    <row r="776" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A776" s="2">
+        <v>44239</v>
+      </c>
+      <c r="B776" s="3">
+        <v>722.52</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:B1"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 02-13-2021 17-10-18
</commit_message>
<xml_diff>
--- a/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
+++ b/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID CL/IndicadoresEconomicos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="133" documentId="13_ncr:1_{C8B25996-B8C9-45E8-BF5F-0058EDDB5306}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{C6386B95-CF3D-489A-AAD0-F799B1385F99}"/>
+  <xr:revisionPtr revIDLastSave="135" documentId="13_ncr:1_{C8B25996-B8C9-45E8-BF5F-0058EDDB5306}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{469D6382-657A-43E8-B559-7E31541C2B00}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,8 +16,8 @@
     <sheet name="DOLAR_OBS_ADO" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">DOLAR_OBS_ADO!$A$3:$B$776</definedName>
-    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$776</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">DOLAR_OBS_ADO!$A$3:$B$779</definedName>
+    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$779</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="5">
   <si>
     <t>Tipos de cambio (pesos por dólar)</t>
   </si>
@@ -970,13 +970,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B776"/>
+  <dimension ref="A1:B779"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="4" topLeftCell="B775" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="4" topLeftCell="B779" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="A776" sqref="A776"/>
+      <selection pane="bottomRight" activeCell="A779" sqref="A779"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7189,6 +7189,30 @@
         <v>722.52</v>
       </c>
     </row>
+    <row r="777" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A777" s="2">
+        <v>44240</v>
+      </c>
+      <c r="B777" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="778" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A778" s="2">
+        <v>44241</v>
+      </c>
+      <c r="B778" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="779" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A779" s="2">
+        <v>44242</v>
+      </c>
+      <c r="B779" s="3">
+        <v>724.39</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:B1"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 02-16-2021 17-16-51
</commit_message>
<xml_diff>
--- a/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
+++ b/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID CL/IndicadoresEconomicos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="135" documentId="13_ncr:1_{C8B25996-B8C9-45E8-BF5F-0058EDDB5306}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{469D6382-657A-43E8-B559-7E31541C2B00}"/>
+  <xr:revisionPtr revIDLastSave="142" documentId="13_ncr:1_{C8B25996-B8C9-45E8-BF5F-0058EDDB5306}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{789F24B9-3952-4D25-B1E0-F42CE54DA0A7}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,8 +16,8 @@
     <sheet name="DOLAR_OBS_ADO" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">DOLAR_OBS_ADO!$A$3:$B$779</definedName>
-    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$779</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">DOLAR_OBS_ADO!$A$3:$B$780</definedName>
+    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$780</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -970,13 +970,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B779"/>
+  <dimension ref="A1:B780"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="4" topLeftCell="B779" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="A779" sqref="A779"/>
+      <selection pane="bottomRight" activeCell="B783" sqref="B783"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7213,6 +7213,14 @@
         <v>724.39</v>
       </c>
     </row>
+    <row r="780" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A780" s="2">
+        <v>44243</v>
+      </c>
+      <c r="B780" s="3">
+        <v>718.45</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:B1"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 02-17-2021 17-09-01
</commit_message>
<xml_diff>
--- a/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
+++ b/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID CL/IndicadoresEconomicos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="142" documentId="13_ncr:1_{C8B25996-B8C9-45E8-BF5F-0058EDDB5306}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{789F24B9-3952-4D25-B1E0-F42CE54DA0A7}"/>
+  <xr:revisionPtr revIDLastSave="144" documentId="13_ncr:1_{C8B25996-B8C9-45E8-BF5F-0058EDDB5306}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{AC187E75-6B3B-47CB-A5FB-77A2ED6C250F}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,8 +16,8 @@
     <sheet name="DOLAR_OBS_ADO" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">DOLAR_OBS_ADO!$A$3:$B$780</definedName>
-    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$780</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">DOLAR_OBS_ADO!$A$3:$B$781</definedName>
+    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$781</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -970,13 +970,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B780"/>
+  <dimension ref="A1:B781"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="4" topLeftCell="B779" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="B783" sqref="B783"/>
+      <selection pane="bottomRight" activeCell="A781" sqref="A781"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7221,6 +7221,14 @@
         <v>718.45</v>
       </c>
     </row>
+    <row r="781" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A781" s="2">
+        <v>44244</v>
+      </c>
+      <c r="B781" s="3">
+        <v>717.38</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:B1"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 02-18-2021 17-10-53
</commit_message>
<xml_diff>
--- a/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
+++ b/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID CL/IndicadoresEconomicos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="144" documentId="13_ncr:1_{C8B25996-B8C9-45E8-BF5F-0058EDDB5306}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{AC187E75-6B3B-47CB-A5FB-77A2ED6C250F}"/>
+  <xr:revisionPtr revIDLastSave="146" documentId="13_ncr:1_{C8B25996-B8C9-45E8-BF5F-0058EDDB5306}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{96714D36-995B-4215-9ADF-63D4AE748806}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,8 +16,8 @@
     <sheet name="DOLAR_OBS_ADO" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">DOLAR_OBS_ADO!$A$3:$B$781</definedName>
-    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$781</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">DOLAR_OBS_ADO!$A$3:$B$782</definedName>
+    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$782</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -970,13 +970,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B781"/>
+  <dimension ref="A1:B782"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="4" topLeftCell="B779" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="A781" sqref="A781"/>
+      <selection pane="bottomRight" activeCell="A785" sqref="A785"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7229,6 +7229,14 @@
         <v>717.38</v>
       </c>
     </row>
+    <row r="782" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A782" s="2">
+        <v>44245</v>
+      </c>
+      <c r="B782" s="3">
+        <v>719.78</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:B1"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 02-19-2021 17-07-54
</commit_message>
<xml_diff>
--- a/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
+++ b/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID CL/IndicadoresEconomicos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="146" documentId="13_ncr:1_{C8B25996-B8C9-45E8-BF5F-0058EDDB5306}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{96714D36-995B-4215-9ADF-63D4AE748806}"/>
+  <xr:revisionPtr revIDLastSave="147" documentId="13_ncr:1_{C8B25996-B8C9-45E8-BF5F-0058EDDB5306}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{30380F17-5A95-4542-AF41-1E19E9CB599F}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,8 +16,8 @@
     <sheet name="DOLAR_OBS_ADO" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">DOLAR_OBS_ADO!$A$3:$B$782</definedName>
-    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$782</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">DOLAR_OBS_ADO!$A$3:$B$783</definedName>
+    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$783</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -970,13 +970,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B782"/>
+  <dimension ref="A1:B783"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="4" topLeftCell="B779" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="4" topLeftCell="B783" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="A785" sqref="A785"/>
+      <selection pane="bottomRight" activeCell="A783" sqref="A783"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7237,6 +7237,14 @@
         <v>719.78</v>
       </c>
     </row>
+    <row r="783" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A783" s="2">
+        <v>44246</v>
+      </c>
+      <c r="B783" s="3">
+        <v>712.14</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:B1"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 02-20-2021 17-16-05
</commit_message>
<xml_diff>
--- a/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
+++ b/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID CL/IndicadoresEconomicos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="147" documentId="13_ncr:1_{C8B25996-B8C9-45E8-BF5F-0058EDDB5306}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{30380F17-5A95-4542-AF41-1E19E9CB599F}"/>
+  <xr:revisionPtr revIDLastSave="149" documentId="13_ncr:1_{C8B25996-B8C9-45E8-BF5F-0058EDDB5306}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{F461C022-91A8-4947-AF65-9786E51882E4}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,8 +16,8 @@
     <sheet name="DOLAR_OBS_ADO" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">DOLAR_OBS_ADO!$A$3:$B$783</definedName>
-    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$783</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">DOLAR_OBS_ADO!$A$3:$B$786</definedName>
+    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$786</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="5">
   <si>
     <t>Tipos de cambio (pesos por dólar)</t>
   </si>
@@ -970,7 +970,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B783"/>
+  <dimension ref="A1:B786"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="4" topLeftCell="B783" activePane="bottomRight" state="frozen"/>
@@ -7245,6 +7245,30 @@
         <v>712.14</v>
       </c>
     </row>
+    <row r="784" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A784" s="2">
+        <v>44247</v>
+      </c>
+      <c r="B784" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="785" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A785" s="2">
+        <v>44248</v>
+      </c>
+      <c r="B785" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="786" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A786" s="2">
+        <v>44249</v>
+      </c>
+      <c r="B786" s="3">
+        <v>707.12</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:B1"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 02-23-2021 17-07-09
</commit_message>
<xml_diff>
--- a/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
+++ b/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID CL/IndicadoresEconomicos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="149" documentId="13_ncr:1_{C8B25996-B8C9-45E8-BF5F-0058EDDB5306}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{F461C022-91A8-4947-AF65-9786E51882E4}"/>
+  <xr:revisionPtr revIDLastSave="153" documentId="13_ncr:1_{C8B25996-B8C9-45E8-BF5F-0058EDDB5306}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{CE2D74FD-6415-4A84-BD9E-410EF1D53394}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,8 +16,8 @@
     <sheet name="DOLAR_OBS_ADO" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">DOLAR_OBS_ADO!$A$3:$B$786</definedName>
-    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$786</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">DOLAR_OBS_ADO!$A$3:$B$787</definedName>
+    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$787</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -970,19 +970,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B786"/>
+  <dimension ref="A1:B787"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="4" topLeftCell="B783" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="A783" sqref="A783"/>
+      <selection pane="bottomRight" activeCell="A786" sqref="A786"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.5703125" customWidth="1"/>
-    <col min="2" max="2" width="15.5703125" customWidth="1"/>
+    <col min="1" max="1" width="12.7109375" customWidth="1"/>
+    <col min="2" max="2" width="14.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -7267,6 +7267,14 @@
       </c>
       <c r="B786" s="3">
         <v>707.12</v>
+      </c>
+    </row>
+    <row r="787" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A787" s="2">
+        <v>44250</v>
+      </c>
+      <c r="B787" s="3">
+        <v>709.65</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update automatico via Actualizar 02-24-2021 17-13-34
</commit_message>
<xml_diff>
--- a/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
+++ b/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID CL/IndicadoresEconomicos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="153" documentId="13_ncr:1_{C8B25996-B8C9-45E8-BF5F-0058EDDB5306}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{CE2D74FD-6415-4A84-BD9E-410EF1D53394}"/>
+  <xr:revisionPtr revIDLastSave="155" documentId="13_ncr:1_{C8B25996-B8C9-45E8-BF5F-0058EDDB5306}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{230C6260-27EC-438E-932D-D0C2D57F63B8}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,8 +16,8 @@
     <sheet name="DOLAR_OBS_ADO" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">DOLAR_OBS_ADO!$A$3:$B$787</definedName>
-    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$787</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">DOLAR_OBS_ADO!$A$3:$B$788</definedName>
+    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$788</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -970,19 +970,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B787"/>
+  <dimension ref="A1:B788"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="4" topLeftCell="B783" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="4" topLeftCell="B788" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="A786" sqref="A786"/>
+      <selection pane="bottomRight" activeCell="A788" sqref="A788"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.7109375" customWidth="1"/>
-    <col min="2" max="2" width="14.42578125" customWidth="1"/>
+    <col min="1" max="1" width="11.5703125" customWidth="1"/>
+    <col min="2" max="2" width="15.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -7275,6 +7275,14 @@
       </c>
       <c r="B787" s="3">
         <v>709.65</v>
+      </c>
+    </row>
+    <row r="788" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A788" s="2">
+        <v>44251</v>
+      </c>
+      <c r="B788" s="3">
+        <v>706.76</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update automatico via Actualizar 02-25-2021 17-11-50
</commit_message>
<xml_diff>
--- a/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
+++ b/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID CL/IndicadoresEconomicos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="155" documentId="13_ncr:1_{C8B25996-B8C9-45E8-BF5F-0058EDDB5306}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{230C6260-27EC-438E-932D-D0C2D57F63B8}"/>
+  <xr:revisionPtr revIDLastSave="157" documentId="13_ncr:1_{C8B25996-B8C9-45E8-BF5F-0058EDDB5306}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{F489840F-0311-40EB-9E6D-67A713D54B9C}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,8 +16,8 @@
     <sheet name="DOLAR_OBS_ADO" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">DOLAR_OBS_ADO!$A$3:$B$788</definedName>
-    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$788</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">DOLAR_OBS_ADO!$A$3:$B$789</definedName>
+    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$789</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -970,13 +970,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B788"/>
+  <dimension ref="A1:B789"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="4" topLeftCell="B788" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="A788" sqref="A788"/>
+      <selection pane="bottomRight" activeCell="A789" sqref="A789"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7285,6 +7285,14 @@
         <v>706.76</v>
       </c>
     </row>
+    <row r="789" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A789" s="2">
+        <v>44252</v>
+      </c>
+      <c r="B789" s="3">
+        <v>703.65</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:B1"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 02-26-2021 17-12-42
</commit_message>
<xml_diff>
--- a/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
+++ b/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID CL/IndicadoresEconomicos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="157" documentId="13_ncr:1_{C8B25996-B8C9-45E8-BF5F-0058EDDB5306}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{F489840F-0311-40EB-9E6D-67A713D54B9C}"/>
+  <xr:revisionPtr revIDLastSave="159" documentId="13_ncr:1_{C8B25996-B8C9-45E8-BF5F-0058EDDB5306}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{F763AE46-F6E5-498D-95F6-8204B6060C75}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,8 +16,8 @@
     <sheet name="DOLAR_OBS_ADO" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">DOLAR_OBS_ADO!$A$3:$B$789</definedName>
-    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$789</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">DOLAR_OBS_ADO!$A$3:$B$790</definedName>
+    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$790</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -970,13 +970,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B789"/>
+  <dimension ref="A1:B790"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="4" topLeftCell="B788" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="A789" sqref="A789"/>
+      <selection pane="bottomRight" activeCell="A790" sqref="A790"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7293,6 +7293,14 @@
         <v>703.65</v>
       </c>
     </row>
+    <row r="790" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A790" s="2">
+        <v>44253</v>
+      </c>
+      <c r="B790" s="3">
+        <v>708.04</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:B1"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 02-27-2021 17-13-45
</commit_message>
<xml_diff>
--- a/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
+++ b/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID CL/IndicadoresEconomicos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="159" documentId="13_ncr:1_{C8B25996-B8C9-45E8-BF5F-0058EDDB5306}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{F763AE46-F6E5-498D-95F6-8204B6060C75}"/>
+  <xr:revisionPtr revIDLastSave="162" documentId="13_ncr:1_{C8B25996-B8C9-45E8-BF5F-0058EDDB5306}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{084010D3-04DD-4CF5-92E1-923C32F3A936}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,8 +16,8 @@
     <sheet name="DOLAR_OBS_ADO" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">DOLAR_OBS_ADO!$A$3:$B$790</definedName>
-    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$790</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">DOLAR_OBS_ADO!$A$3:$B$793</definedName>
+    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$793</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="5">
   <si>
     <t>Tipos de cambio (pesos por dólar)</t>
   </si>
@@ -970,19 +970,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B790"/>
+  <dimension ref="A1:B793"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="4" topLeftCell="B788" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="4" topLeftCell="B793" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="A790" sqref="A790"/>
+      <selection pane="bottomRight" activeCell="A793" sqref="A793"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.5703125" customWidth="1"/>
-    <col min="2" max="2" width="15.5703125" customWidth="1"/>
+    <col min="1" max="1" width="12.7109375" customWidth="1"/>
+    <col min="2" max="2" width="14.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -7299,6 +7299,30 @@
       </c>
       <c r="B790" s="3">
         <v>708.04</v>
+      </c>
+    </row>
+    <row r="791" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A791" s="2">
+        <v>44254</v>
+      </c>
+      <c r="B791" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="792" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A792" s="2">
+        <v>44255</v>
+      </c>
+      <c r="B792" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="793" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A793" s="2">
+        <v>44256</v>
+      </c>
+      <c r="B793" s="3">
+        <v>719.91</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update automatico via Actualizar 03-02-2021 17-09-19
</commit_message>
<xml_diff>
--- a/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
+++ b/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID CL/IndicadoresEconomicos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="162" documentId="13_ncr:1_{C8B25996-B8C9-45E8-BF5F-0058EDDB5306}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{084010D3-04DD-4CF5-92E1-923C32F3A936}"/>
+  <xr:revisionPtr revIDLastSave="164" documentId="13_ncr:1_{C8B25996-B8C9-45E8-BF5F-0058EDDB5306}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{C8C0CC13-59B4-496D-85BA-66A020527D0B}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,8 +16,8 @@
     <sheet name="DOLAR_OBS_ADO" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">DOLAR_OBS_ADO!$A$3:$B$793</definedName>
-    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$793</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">DOLAR_OBS_ADO!$A$3:$B$794</definedName>
+    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$794</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -970,19 +970,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B793"/>
+  <dimension ref="A1:B794"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="4" topLeftCell="B793" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="4" topLeftCell="B794" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="A793" sqref="A793"/>
+      <selection pane="bottomRight" activeCell="A794" sqref="A794"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.7109375" customWidth="1"/>
-    <col min="2" max="2" width="14.42578125" customWidth="1"/>
+    <col min="1" max="1" width="11.5703125" customWidth="1"/>
+    <col min="2" max="2" width="15.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -7323,6 +7323,14 @@
       </c>
       <c r="B793" s="3">
         <v>719.91</v>
+      </c>
+    </row>
+    <row r="794" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A794" s="2">
+        <v>44257</v>
+      </c>
+      <c r="B794" s="3">
+        <v>721.2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update automatico via Actualizar 03-03-2021 17-06-14
</commit_message>
<xml_diff>
--- a/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
+++ b/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID CL/IndicadoresEconomicos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="164" documentId="13_ncr:1_{C8B25996-B8C9-45E8-BF5F-0058EDDB5306}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{C8C0CC13-59B4-496D-85BA-66A020527D0B}"/>
+  <xr:revisionPtr revIDLastSave="166" documentId="13_ncr:1_{C8B25996-B8C9-45E8-BF5F-0058EDDB5306}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{E35DFD50-87BB-4F2D-9644-E749154125A9}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,8 +16,8 @@
     <sheet name="DOLAR_OBS_ADO" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">DOLAR_OBS_ADO!$A$3:$B$794</definedName>
-    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$794</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">DOLAR_OBS_ADO!$A$3:$B$795</definedName>
+    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$795</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -970,13 +970,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B794"/>
+  <dimension ref="A1:B795"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="4" topLeftCell="B794" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="4" topLeftCell="B795" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="A794" sqref="A794"/>
+      <selection pane="bottomRight" activeCell="A795" sqref="A795"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7333,6 +7333,14 @@
         <v>721.2</v>
       </c>
     </row>
+    <row r="795" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A795" s="2">
+        <v>44258</v>
+      </c>
+      <c r="B795" s="3">
+        <v>726.74</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:B1"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 03-05-2021 14-29-16
</commit_message>
<xml_diff>
--- a/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
+++ b/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID CL/IndicadoresEconomicos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="166" documentId="13_ncr:1_{C8B25996-B8C9-45E8-BF5F-0058EDDB5306}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{E35DFD50-87BB-4F2D-9644-E749154125A9}"/>
+  <xr:revisionPtr revIDLastSave="170" documentId="13_ncr:1_{C8B25996-B8C9-45E8-BF5F-0058EDDB5306}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{4E4707FD-0C5E-4FAA-87FF-28E9503276F5}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,8 +16,8 @@
     <sheet name="DOLAR_OBS_ADO" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">DOLAR_OBS_ADO!$A$3:$B$795</definedName>
-    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$795</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">DOLAR_OBS_ADO!$A$3:$B$797</definedName>
+    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$797</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -970,13 +970,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B795"/>
+  <dimension ref="A1:B797"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="4" topLeftCell="B795" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="4" topLeftCell="B796" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="A795" sqref="A795"/>
+      <selection pane="bottomRight" activeCell="A797" sqref="A797"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7341,6 +7341,22 @@
         <v>726.74</v>
       </c>
     </row>
+    <row r="796" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A796" s="2">
+        <v>44259</v>
+      </c>
+      <c r="B796" s="3">
+        <v>731.3</v>
+      </c>
+    </row>
+    <row r="797" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A797" s="2">
+        <v>44260</v>
+      </c>
+      <c r="B797" s="3">
+        <v>729.15</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:B1"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 03-08-2021 13-53-03
</commit_message>
<xml_diff>
--- a/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
+++ b/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID CL/IndicadoresEconomicos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="170" documentId="13_ncr:1_{C8B25996-B8C9-45E8-BF5F-0058EDDB5306}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{4E4707FD-0C5E-4FAA-87FF-28E9503276F5}"/>
+  <xr:revisionPtr revIDLastSave="173" documentId="13_ncr:1_{C8B25996-B8C9-45E8-BF5F-0058EDDB5306}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{F79C77D9-6D75-4DD3-877A-34F0C5E9753B}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,8 +16,8 @@
     <sheet name="DOLAR_OBS_ADO" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">DOLAR_OBS_ADO!$A$3:$B$797</definedName>
-    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$797</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">DOLAR_OBS_ADO!$A$3:$B$800</definedName>
+    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$800</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="5">
   <si>
     <t>Tipos de cambio (pesos por dólar)</t>
   </si>
@@ -970,13 +970,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B797"/>
+  <dimension ref="A1:B800"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="4" topLeftCell="B796" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="4" topLeftCell="B800" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="A797" sqref="A797"/>
+      <selection pane="bottomRight" activeCell="A800" sqref="A800"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7357,6 +7357,30 @@
         <v>729.15</v>
       </c>
     </row>
+    <row r="798" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A798" s="2">
+        <v>44261</v>
+      </c>
+      <c r="B798" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="799" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A799" s="2">
+        <v>44262</v>
+      </c>
+      <c r="B799" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="800" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A800" s="2">
+        <v>44263</v>
+      </c>
+      <c r="B800" s="3">
+        <v>733.11</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:B1"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 03-09-2021 17-11-06
</commit_message>
<xml_diff>
--- a/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
+++ b/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID CL/IndicadoresEconomicos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="173" documentId="13_ncr:1_{C8B25996-B8C9-45E8-BF5F-0058EDDB5306}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{F79C77D9-6D75-4DD3-877A-34F0C5E9753B}"/>
+  <xr:revisionPtr revIDLastSave="175" documentId="13_ncr:1_{C8B25996-B8C9-45E8-BF5F-0058EDDB5306}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{24FB1B98-4941-4011-B0BC-814FADBD3206}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,8 +16,8 @@
     <sheet name="DOLAR_OBS_ADO" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">DOLAR_OBS_ADO!$A$3:$B$800</definedName>
-    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$800</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">DOLAR_OBS_ADO!$A$3:$B$801</definedName>
+    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$801</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -970,13 +970,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B800"/>
+  <dimension ref="A1:B801"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="4" topLeftCell="B800" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="4" topLeftCell="B801" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="A800" sqref="A800"/>
+      <selection pane="bottomRight" activeCell="A801" sqref="A801"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7381,6 +7381,14 @@
         <v>733.11</v>
       </c>
     </row>
+    <row r="801" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A801" s="2">
+        <v>44264</v>
+      </c>
+      <c r="B801" s="3">
+        <v>738.46</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:B1"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 03-10-2021 17-13-57
</commit_message>
<xml_diff>
--- a/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
+++ b/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID CL/IndicadoresEconomicos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="175" documentId="13_ncr:1_{C8B25996-B8C9-45E8-BF5F-0058EDDB5306}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{24FB1B98-4941-4011-B0BC-814FADBD3206}"/>
+  <xr:revisionPtr revIDLastSave="177" documentId="13_ncr:1_{C8B25996-B8C9-45E8-BF5F-0058EDDB5306}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{79EBD17A-34D4-4F59-9A0E-7C02DB146578}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,8 +16,8 @@
     <sheet name="DOLAR_OBS_ADO" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">DOLAR_OBS_ADO!$A$3:$B$801</definedName>
-    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$801</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">DOLAR_OBS_ADO!$A$3:$B$802</definedName>
+    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$802</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -970,13 +970,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B801"/>
+  <dimension ref="A1:B802"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="4" topLeftCell="B801" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="A801" sqref="A801"/>
+      <selection pane="bottomRight" activeCell="A802" sqref="A802"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7389,6 +7389,14 @@
         <v>738.46</v>
       </c>
     </row>
+    <row r="802" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A802" s="2">
+        <v>44265</v>
+      </c>
+      <c r="B802" s="3">
+        <v>733.42</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:B1"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 03-11-2021 17-13-16
</commit_message>
<xml_diff>
--- a/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
+++ b/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID CL/IndicadoresEconomicos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="177" documentId="13_ncr:1_{C8B25996-B8C9-45E8-BF5F-0058EDDB5306}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{79EBD17A-34D4-4F59-9A0E-7C02DB146578}"/>
+  <xr:revisionPtr revIDLastSave="179" documentId="13_ncr:1_{C8B25996-B8C9-45E8-BF5F-0058EDDB5306}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{A06FA27E-C1AF-475C-8B90-EA65BD50E9FF}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,8 +16,8 @@
     <sheet name="DOLAR_OBS_ADO" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">DOLAR_OBS_ADO!$A$3:$B$802</definedName>
-    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$802</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">DOLAR_OBS_ADO!$A$3:$B$803</definedName>
+    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$803</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -970,13 +970,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B802"/>
+  <dimension ref="A1:B803"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="4" topLeftCell="B801" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="4" topLeftCell="B803" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="A802" sqref="A802"/>
+      <selection pane="bottomRight" activeCell="A803" sqref="A803"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7397,6 +7397,14 @@
         <v>733.42</v>
       </c>
     </row>
+    <row r="803" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A803" s="2">
+        <v>44266</v>
+      </c>
+      <c r="B803" s="3">
+        <v>728.89</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:B1"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 03-12-2021 17-11-34
</commit_message>
<xml_diff>
--- a/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
+++ b/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID CL/IndicadoresEconomicos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="179" documentId="13_ncr:1_{C8B25996-B8C9-45E8-BF5F-0058EDDB5306}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{A06FA27E-C1AF-475C-8B90-EA65BD50E9FF}"/>
+  <xr:revisionPtr revIDLastSave="183" documentId="13_ncr:1_{C8B25996-B8C9-45E8-BF5F-0058EDDB5306}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{3F294C30-9160-4EE6-81FE-2648F4E5F9A2}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,8 +16,8 @@
     <sheet name="DOLAR_OBS_ADO" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">DOLAR_OBS_ADO!$A$3:$B$803</definedName>
-    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$803</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">DOLAR_OBS_ADO!$A$3:$B$804</definedName>
+    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$804</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -970,13 +970,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B803"/>
+  <dimension ref="A1:B804"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="4" topLeftCell="B803" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="4" topLeftCell="B804" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="A803" sqref="A803"/>
+      <selection pane="bottomRight" activeCell="A804" sqref="A804"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7405,6 +7405,14 @@
         <v>728.89</v>
       </c>
     </row>
+    <row r="804" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A804" s="2">
+        <v>44267</v>
+      </c>
+      <c r="B804" s="3">
+        <v>718.4</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:B1"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 03-13-2021 17-07-46
</commit_message>
<xml_diff>
--- a/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
+++ b/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID CL/IndicadoresEconomicos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="183" documentId="13_ncr:1_{C8B25996-B8C9-45E8-BF5F-0058EDDB5306}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{3F294C30-9160-4EE6-81FE-2648F4E5F9A2}"/>
+  <xr:revisionPtr revIDLastSave="185" documentId="13_ncr:1_{C8B25996-B8C9-45E8-BF5F-0058EDDB5306}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{7390FFDE-1CA9-49FC-8C13-275998B1906C}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,8 +16,8 @@
     <sheet name="DOLAR_OBS_ADO" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">DOLAR_OBS_ADO!$A$3:$B$804</definedName>
-    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$804</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">DOLAR_OBS_ADO!$A$3:$B$807</definedName>
+    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$807</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="5">
   <si>
     <t>Tipos de cambio (pesos por dólar)</t>
   </si>
@@ -970,13 +970,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B804"/>
+  <dimension ref="A1:B807"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="4" topLeftCell="B804" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="4" topLeftCell="B807" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="A804" sqref="A804"/>
+      <selection pane="bottomRight" activeCell="A807" sqref="A807"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7413,6 +7413,30 @@
         <v>718.4</v>
       </c>
     </row>
+    <row r="805" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A805" s="2">
+        <v>44268</v>
+      </c>
+      <c r="B805" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="806" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A806" s="2">
+        <v>44269</v>
+      </c>
+      <c r="B806" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="807" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A807" s="2">
+        <v>44270</v>
+      </c>
+      <c r="B807" s="3">
+        <v>718.37</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:B1"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 03-16-2021 17-05-42
</commit_message>
<xml_diff>
--- a/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
+++ b/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID CL/IndicadoresEconomicos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="185" documentId="13_ncr:1_{C8B25996-B8C9-45E8-BF5F-0058EDDB5306}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{7390FFDE-1CA9-49FC-8C13-275998B1906C}"/>
+  <xr:revisionPtr revIDLastSave="187" documentId="13_ncr:1_{C8B25996-B8C9-45E8-BF5F-0058EDDB5306}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{62629EC3-5F23-4685-A6F9-6950EB0CCCB4}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,8 +16,8 @@
     <sheet name="DOLAR_OBS_ADO" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">DOLAR_OBS_ADO!$A$3:$B$807</definedName>
-    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$807</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">DOLAR_OBS_ADO!$A$3:$B$808</definedName>
+    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$808</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -970,13 +970,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B807"/>
+  <dimension ref="A1:B808"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="4" topLeftCell="B807" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="4" topLeftCell="B808" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="A807" sqref="A807"/>
+      <selection pane="bottomRight" activeCell="A808" sqref="A808"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7437,6 +7437,14 @@
         <v>718.37</v>
       </c>
     </row>
+    <row r="808" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A808" s="2">
+        <v>44271</v>
+      </c>
+      <c r="B808" s="3">
+        <v>721.49</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:B1"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 03-17-2021 17-13-26
</commit_message>
<xml_diff>
--- a/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
+++ b/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID CL/IndicadoresEconomicos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="187" documentId="13_ncr:1_{C8B25996-B8C9-45E8-BF5F-0058EDDB5306}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{62629EC3-5F23-4685-A6F9-6950EB0CCCB4}"/>
+  <xr:revisionPtr revIDLastSave="189" documentId="13_ncr:1_{C8B25996-B8C9-45E8-BF5F-0058EDDB5306}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{D4160A2F-1ED2-4845-8873-67792B850100}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,8 +16,8 @@
     <sheet name="DOLAR_OBS_ADO" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">DOLAR_OBS_ADO!$A$3:$B$808</definedName>
-    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$808</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">DOLAR_OBS_ADO!$A$3:$B$809</definedName>
+    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$809</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -970,13 +970,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B808"/>
+  <dimension ref="A1:B809"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="4" topLeftCell="B808" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="4" topLeftCell="B809" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="A808" sqref="A808"/>
+      <selection pane="bottomRight" activeCell="A809" sqref="A809"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7445,6 +7445,14 @@
         <v>721.49</v>
       </c>
     </row>
+    <row r="809" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A809" s="2">
+        <v>44272</v>
+      </c>
+      <c r="B809" s="3">
+        <v>723.47</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:B1"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 03-18-2021 17-11-58
</commit_message>
<xml_diff>
--- a/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
+++ b/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID CL/IndicadoresEconomicos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="189" documentId="13_ncr:1_{C8B25996-B8C9-45E8-BF5F-0058EDDB5306}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{D4160A2F-1ED2-4845-8873-67792B850100}"/>
+  <xr:revisionPtr revIDLastSave="191" documentId="13_ncr:1_{C8B25996-B8C9-45E8-BF5F-0058EDDB5306}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{0F09D77A-A574-4EBA-87E1-1CEDCE4448A9}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,8 +16,8 @@
     <sheet name="DOLAR_OBS_ADO" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">DOLAR_OBS_ADO!$A$3:$B$809</definedName>
-    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$809</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">DOLAR_OBS_ADO!$A$3:$B$810</definedName>
+    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$810</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -970,13 +970,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B809"/>
+  <dimension ref="A1:B810"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="4" topLeftCell="B809" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="A809" sqref="A809"/>
+      <selection pane="bottomRight" activeCell="A810" sqref="A810"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7453,6 +7453,14 @@
         <v>723.47</v>
       </c>
     </row>
+    <row r="810" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A810" s="2">
+        <v>44273</v>
+      </c>
+      <c r="B810" s="3">
+        <v>730.93</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:B1"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 03-19-2021 17-06-30
</commit_message>
<xml_diff>
--- a/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
+++ b/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID CL/IndicadoresEconomicos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="191" documentId="13_ncr:1_{C8B25996-B8C9-45E8-BF5F-0058EDDB5306}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{0F09D77A-A574-4EBA-87E1-1CEDCE4448A9}"/>
+  <xr:revisionPtr revIDLastSave="195" documentId="13_ncr:1_{C8B25996-B8C9-45E8-BF5F-0058EDDB5306}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{21617188-2AC0-45AD-98C3-E82C15309D88}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,8 +16,8 @@
     <sheet name="DOLAR_OBS_ADO" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">DOLAR_OBS_ADO!$A$3:$B$810</definedName>
-    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$810</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">DOLAR_OBS_ADO!$A$3:$B$811</definedName>
+    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$811</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -970,13 +970,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B810"/>
+  <dimension ref="A1:B811"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="4" topLeftCell="B809" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="4" topLeftCell="B811" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="A810" sqref="A810"/>
+      <selection pane="bottomRight" activeCell="A811" sqref="A811"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7461,6 +7461,14 @@
         <v>730.93</v>
       </c>
     </row>
+    <row r="811" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A811" s="2">
+        <v>44274</v>
+      </c>
+      <c r="B811" s="3">
+        <v>724.59</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:B1"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 03-20-2021 17-14-30
</commit_message>
<xml_diff>
--- a/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
+++ b/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID CL/IndicadoresEconomicos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="195" documentId="13_ncr:1_{C8B25996-B8C9-45E8-BF5F-0058EDDB5306}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{21617188-2AC0-45AD-98C3-E82C15309D88}"/>
+  <xr:revisionPtr revIDLastSave="197" documentId="13_ncr:1_{C8B25996-B8C9-45E8-BF5F-0058EDDB5306}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{B6D620BF-CC0B-4ACF-A7CC-154B36A671F8}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,8 +16,8 @@
     <sheet name="DOLAR_OBS_ADO" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">DOLAR_OBS_ADO!$A$3:$B$811</definedName>
-    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$811</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">DOLAR_OBS_ADO!$A$3:$B$814</definedName>
+    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$814</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="5">
   <si>
     <t>Tipos de cambio (pesos por dólar)</t>
   </si>
@@ -970,13 +970,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B811"/>
+  <dimension ref="A1:B814"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="4" topLeftCell="B811" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="4" topLeftCell="B814" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="A811" sqref="A811"/>
+      <selection pane="bottomRight" activeCell="A814" sqref="A814"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7469,6 +7469,30 @@
         <v>724.59</v>
       </c>
     </row>
+    <row r="812" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A812" s="2">
+        <v>44275</v>
+      </c>
+      <c r="B812" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="813" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A813" s="2">
+        <v>44276</v>
+      </c>
+      <c r="B813" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="814" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A814" s="2">
+        <v>44277</v>
+      </c>
+      <c r="B814" s="3">
+        <v>717.96</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:B1"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 03-23-2021 17-14-58
</commit_message>
<xml_diff>
--- a/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
+++ b/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID CL/IndicadoresEconomicos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="197" documentId="13_ncr:1_{C8B25996-B8C9-45E8-BF5F-0058EDDB5306}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{B6D620BF-CC0B-4ACF-A7CC-154B36A671F8}"/>
+  <xr:revisionPtr revIDLastSave="199" documentId="13_ncr:1_{C8B25996-B8C9-45E8-BF5F-0058EDDB5306}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{9A125C0B-46A7-46DB-B8D5-0242492CD926}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,8 +16,8 @@
     <sheet name="DOLAR_OBS_ADO" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">DOLAR_OBS_ADO!$A$3:$B$814</definedName>
-    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$814</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">DOLAR_OBS_ADO!$A$3:$B$815</definedName>
+    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$815</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -970,13 +970,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B814"/>
+  <dimension ref="A1:B815"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="4" topLeftCell="B814" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="4" topLeftCell="B815" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="A814" sqref="A814"/>
+      <selection pane="bottomRight" activeCell="A815" sqref="A815"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7493,6 +7493,14 @@
         <v>717.96</v>
       </c>
     </row>
+    <row r="815" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A815" s="2">
+        <v>44278</v>
+      </c>
+      <c r="B815" s="3">
+        <v>716.46</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:B1"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 03-24-2021 17-06-53
</commit_message>
<xml_diff>
--- a/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
+++ b/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID CL/IndicadoresEconomicos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="199" documentId="13_ncr:1_{C8B25996-B8C9-45E8-BF5F-0058EDDB5306}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{9A125C0B-46A7-46DB-B8D5-0242492CD926}"/>
+  <xr:revisionPtr revIDLastSave="201" documentId="13_ncr:1_{C8B25996-B8C9-45E8-BF5F-0058EDDB5306}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{BEFD48D5-B7C5-4A2D-BC29-B705CE3359A7}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="90" yWindow="810" windowWidth="17115" windowHeight="10110" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DOLAR_OBS_ADO" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">DOLAR_OBS_ADO!$A$3:$B$815</definedName>
-    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$815</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">DOLAR_OBS_ADO!$A$3:$B$816</definedName>
+    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$816</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -970,13 +970,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B815"/>
+  <dimension ref="A1:B816"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="4" topLeftCell="B815" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="4" topLeftCell="B816" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="A815" sqref="A815"/>
+      <selection pane="bottomRight" activeCell="A816" sqref="A816"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7501,6 +7501,14 @@
         <v>716.46</v>
       </c>
     </row>
+    <row r="816" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A816" s="2">
+        <v>44279</v>
+      </c>
+      <c r="B816" s="3">
+        <v>720.62</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:B1"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 03-25-2021 17-13-21
</commit_message>
<xml_diff>
--- a/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
+++ b/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID CL/IndicadoresEconomicos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="201" documentId="13_ncr:1_{C8B25996-B8C9-45E8-BF5F-0058EDDB5306}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{BEFD48D5-B7C5-4A2D-BC29-B705CE3359A7}"/>
+  <xr:revisionPtr revIDLastSave="203" documentId="13_ncr:1_{C8B25996-B8C9-45E8-BF5F-0058EDDB5306}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{CA50F994-AEFF-4A39-9C99-1E3C1F2083BF}"/>
   <bookViews>
-    <workbookView xWindow="90" yWindow="810" windowWidth="17115" windowHeight="10110" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="780" windowWidth="16980" windowHeight="10110" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DOLAR_OBS_ADO" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">DOLAR_OBS_ADO!$A$3:$B$816</definedName>
-    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$816</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">DOLAR_OBS_ADO!$A$3:$B$817</definedName>
+    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$817</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -970,13 +970,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B816"/>
+  <dimension ref="A1:B817"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="4" topLeftCell="B816" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="4" topLeftCell="B817" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="A816" sqref="A816"/>
+      <selection pane="bottomRight" activeCell="A817" sqref="A817"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7509,6 +7509,14 @@
         <v>720.62</v>
       </c>
     </row>
+    <row r="817" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A817" s="2">
+        <v>44280</v>
+      </c>
+      <c r="B817" s="3">
+        <v>723.35</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:B1"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 03-26-2021 17-08-42
</commit_message>
<xml_diff>
--- a/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
+++ b/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID CL/IndicadoresEconomicos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="203" documentId="13_ncr:1_{C8B25996-B8C9-45E8-BF5F-0058EDDB5306}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{CA50F994-AEFF-4A39-9C99-1E3C1F2083BF}"/>
+  <xr:revisionPtr revIDLastSave="205" documentId="13_ncr:1_{C8B25996-B8C9-45E8-BF5F-0058EDDB5306}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{E1E00439-3A23-44EF-A460-4E6F513DB400}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="780" windowWidth="16980" windowHeight="10110" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="810" windowWidth="16890" windowHeight="10110" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DOLAR_OBS_ADO" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">DOLAR_OBS_ADO!$A$3:$B$817</definedName>
-    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$817</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">DOLAR_OBS_ADO!$A$3:$B$818</definedName>
+    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$818</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -970,13 +970,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B817"/>
+  <dimension ref="A1:B818"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="4" topLeftCell="B817" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="4" topLeftCell="B818" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="A817" sqref="A817"/>
+      <selection pane="bottomRight" activeCell="A818" sqref="A818"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7517,6 +7517,14 @@
         <v>723.35</v>
       </c>
     </row>
+    <row r="818" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A818" s="2">
+        <v>44281</v>
+      </c>
+      <c r="B818" s="3">
+        <v>730.82</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:B1"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 03-27-2021 17-12-56
</commit_message>
<xml_diff>
--- a/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
+++ b/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID CL/IndicadoresEconomicos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="205" documentId="13_ncr:1_{C8B25996-B8C9-45E8-BF5F-0058EDDB5306}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{E1E00439-3A23-44EF-A460-4E6F513DB400}"/>
+  <xr:revisionPtr revIDLastSave="207" documentId="13_ncr:1_{C8B25996-B8C9-45E8-BF5F-0058EDDB5306}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{DAF7DACB-ECFE-4E34-83AC-D5E799DA3F93}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="810" windowWidth="16890" windowHeight="10110" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="60" yWindow="780" windowWidth="16905" windowHeight="10110" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DOLAR_OBS_ADO" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">DOLAR_OBS_ADO!$A$3:$B$818</definedName>
-    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$818</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">DOLAR_OBS_ADO!$A$3:$B$821</definedName>
+    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$821</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="5">
   <si>
     <t>Tipos de cambio (pesos por dólar)</t>
   </si>
@@ -970,13 +970,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B818"/>
+  <dimension ref="A1:B821"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="4" topLeftCell="B818" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="4" topLeftCell="B821" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="A818" sqref="A818"/>
+      <selection pane="bottomRight" activeCell="A821" sqref="A821"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7525,6 +7525,30 @@
         <v>730.82</v>
       </c>
     </row>
+    <row r="819" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A819" s="2">
+        <v>44282</v>
+      </c>
+      <c r="B819" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="820" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A820" s="2">
+        <v>44283</v>
+      </c>
+      <c r="B820" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="821" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A821" s="2">
+        <v>44284</v>
+      </c>
+      <c r="B821" s="3">
+        <v>729.5</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:B1"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 03-30-2021 17-11-15
</commit_message>
<xml_diff>
--- a/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
+++ b/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID CL/IndicadoresEconomicos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="207" documentId="13_ncr:1_{C8B25996-B8C9-45E8-BF5F-0058EDDB5306}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{DAF7DACB-ECFE-4E34-83AC-D5E799DA3F93}"/>
+  <xr:revisionPtr revIDLastSave="209" documentId="13_ncr:1_{C8B25996-B8C9-45E8-BF5F-0058EDDB5306}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{A21E3F42-FBF7-43BA-BAC5-ADEA9FE83365}"/>
   <bookViews>
-    <workbookView xWindow="60" yWindow="780" windowWidth="16905" windowHeight="10110" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15" yWindow="780" windowWidth="17025" windowHeight="10110" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DOLAR_OBS_ADO" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">DOLAR_OBS_ADO!$A$3:$B$821</definedName>
-    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$821</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">DOLAR_OBS_ADO!$A$3:$B$822</definedName>
+    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$822</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -970,13 +970,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B821"/>
+  <dimension ref="A1:B822"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="4" topLeftCell="B821" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="4" topLeftCell="B822" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="A821" sqref="A821"/>
+      <selection pane="bottomRight" activeCell="A822" sqref="A822"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7549,6 +7549,14 @@
         <v>729.5</v>
       </c>
     </row>
+    <row r="822" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A822" s="2">
+        <v>44285</v>
+      </c>
+      <c r="B822" s="3">
+        <v>736.17</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:B1"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 03-31-2021 17-09-56
</commit_message>
<xml_diff>
--- a/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
+++ b/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID CL/IndicadoresEconomicos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="209" documentId="13_ncr:1_{C8B25996-B8C9-45E8-BF5F-0058EDDB5306}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{A21E3F42-FBF7-43BA-BAC5-ADEA9FE83365}"/>
+  <xr:revisionPtr revIDLastSave="211" documentId="13_ncr:1_{C8B25996-B8C9-45E8-BF5F-0058EDDB5306}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{54893F93-7078-4FE9-AC26-87C429055EF7}"/>
   <bookViews>
-    <workbookView xWindow="15" yWindow="780" windowWidth="17025" windowHeight="10110" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30" yWindow="810" windowWidth="16950" windowHeight="10110" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DOLAR_OBS_ADO" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">DOLAR_OBS_ADO!$A$3:$B$822</definedName>
-    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$822</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">DOLAR_OBS_ADO!$A$3:$B$823</definedName>
+    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$823</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -970,13 +970,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B822"/>
+  <dimension ref="A1:B823"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="4" topLeftCell="B822" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="4" topLeftCell="B823" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="A822" sqref="A822"/>
+      <selection pane="bottomRight" activeCell="A823" sqref="A823"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7557,6 +7557,14 @@
         <v>736.17</v>
       </c>
     </row>
+    <row r="823" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A823" s="2">
+        <v>44286</v>
+      </c>
+      <c r="B823" s="3">
+        <v>732.11</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:B1"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 04-01-2021 17-10-53
</commit_message>
<xml_diff>
--- a/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
+++ b/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID CL/IndicadoresEconomicos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="211" documentId="13_ncr:1_{C8B25996-B8C9-45E8-BF5F-0058EDDB5306}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{54893F93-7078-4FE9-AC26-87C429055EF7}"/>
+  <xr:revisionPtr revIDLastSave="213" documentId="13_ncr:1_{C8B25996-B8C9-45E8-BF5F-0058EDDB5306}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{438B320A-1BB2-4FE9-984A-FE5C311A9BB4}"/>
   <bookViews>
-    <workbookView xWindow="30" yWindow="810" windowWidth="16950" windowHeight="10110" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15" yWindow="735" windowWidth="16920" windowHeight="10110" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DOLAR_OBS_ADO" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">DOLAR_OBS_ADO!$A$3:$B$823</definedName>
-    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$823</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">DOLAR_OBS_ADO!$A$3:$B$824</definedName>
+    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$824</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -970,13 +970,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B823"/>
+  <dimension ref="A1:B824"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="4" topLeftCell="B823" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="4" topLeftCell="B824" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="A823" sqref="A823"/>
+      <selection pane="bottomRight" activeCell="A824" sqref="A824"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7565,6 +7565,14 @@
         <v>732.11</v>
       </c>
     </row>
+    <row r="824" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A824" s="2">
+        <v>44287</v>
+      </c>
+      <c r="B824" s="3">
+        <v>721.82</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:B1"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 04-02-2021 17-08-37
</commit_message>
<xml_diff>
--- a/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
+++ b/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID CL/IndicadoresEconomicos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="213" documentId="13_ncr:1_{C8B25996-B8C9-45E8-BF5F-0058EDDB5306}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{438B320A-1BB2-4FE9-984A-FE5C311A9BB4}"/>
+  <xr:revisionPtr revIDLastSave="215" documentId="13_ncr:1_{C8B25996-B8C9-45E8-BF5F-0058EDDB5306}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{25DDECC2-863B-4FA9-8766-F6F83C3F06F4}"/>
   <bookViews>
-    <workbookView xWindow="15" yWindow="735" windowWidth="16920" windowHeight="10110" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DOLAR_OBS_ADO" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">DOLAR_OBS_ADO!$A$3:$B$824</definedName>
-    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$824</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">DOLAR_OBS_ADO!$A$3:$B$828</definedName>
+    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$828</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="5">
   <si>
     <t>Tipos de cambio (pesos por dólar)</t>
   </si>
@@ -970,13 +970,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B824"/>
+  <dimension ref="A1:B828"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="4" topLeftCell="B824" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="4" topLeftCell="B828" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="A824" sqref="A824"/>
+      <selection pane="bottomRight" activeCell="A828" sqref="A828"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7573,6 +7573,38 @@
         <v>721.82</v>
       </c>
     </row>
+    <row r="825" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A825" s="2">
+        <v>44288</v>
+      </c>
+      <c r="B825" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="826" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A826" s="2">
+        <v>44289</v>
+      </c>
+      <c r="B826" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="827" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A827" s="2">
+        <v>44290</v>
+      </c>
+      <c r="B827" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="828" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A828" s="2">
+        <v>44291</v>
+      </c>
+      <c r="B828" s="3">
+        <v>717.12</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:B1"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 04-08-2021 15-54-39
</commit_message>
<xml_diff>
--- a/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
+++ b/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID CL/IndicadoresEconomicos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="215" documentId="13_ncr:1_{C8B25996-B8C9-45E8-BF5F-0058EDDB5306}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{25DDECC2-863B-4FA9-8766-F6F83C3F06F4}"/>
+  <xr:revisionPtr revIDLastSave="220" documentId="13_ncr:1_{C8B25996-B8C9-45E8-BF5F-0058EDDB5306}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{CF7AE17D-8D6D-4C96-95BB-46E813D2AF1C}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,8 +16,8 @@
     <sheet name="DOLAR_OBS_ADO" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">DOLAR_OBS_ADO!$A$3:$B$828</definedName>
-    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$828</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">DOLAR_OBS_ADO!$A$3:$B$831</definedName>
+    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$831</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -970,13 +970,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B828"/>
+  <dimension ref="A1:B831"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="4" topLeftCell="B828" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="4" topLeftCell="B831" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="A828" sqref="A828"/>
+      <selection pane="bottomRight" activeCell="A831" sqref="A831"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7605,6 +7605,30 @@
         <v>717.12</v>
       </c>
     </row>
+    <row r="829" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A829" s="2">
+        <v>44292</v>
+      </c>
+      <c r="B829" s="3">
+        <v>717.9</v>
+      </c>
+    </row>
+    <row r="830" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A830" s="2">
+        <v>44293</v>
+      </c>
+      <c r="B830" s="3">
+        <v>718.17</v>
+      </c>
+    </row>
+    <row r="831" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A831" s="2">
+        <v>44294</v>
+      </c>
+      <c r="B831" s="3">
+        <v>714.21</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:B1"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 04-14-2021 20-49-35
</commit_message>
<xml_diff>
--- a/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
+++ b/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID CL/IndicadoresEconomicos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="220" documentId="13_ncr:1_{C8B25996-B8C9-45E8-BF5F-0058EDDB5306}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{CF7AE17D-8D6D-4C96-95BB-46E813D2AF1C}"/>
+  <xr:revisionPtr revIDLastSave="228" documentId="13_ncr:1_{C8B25996-B8C9-45E8-BF5F-0058EDDB5306}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{F74660F3-5A1B-4423-95AF-6684CAB52A85}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,8 +16,8 @@
     <sheet name="DOLAR_OBS_ADO" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">DOLAR_OBS_ADO!$A$3:$B$831</definedName>
-    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$831</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">DOLAR_OBS_ADO!$A$3:$B$837</definedName>
+    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$837</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
-  <connection id="1" xr16:uid="{00000000-0015-0000-FFFF-FFFF00000000}" odcFile="D:\reyes.rodriguezucv@gmail.com\OneDrive\Proyectos\Data intelligence\Covid-19\Chile\DOLAR_OBS_ADO.iqy" name="DOLAR_OBS_ADO" type="4" refreshedVersion="6" background="1" saveData="1">
+  <connection id="1" xr16:uid="{00000000-0015-0000-FFFF-FFFF00000000}" odcFile="D:\reyes.rodriguezucv@gmail.com\OneDrive\Proyectos\Data intelligence\Covid-19\Chile\DOLAR_OBS_ADO.iqy" name="DOLAR_OBS_ADO" type="4" refreshedVersion="7" background="1" saveData="1">
     <webPr consecutive="1" xl2000="1" url="http://si3.bcentral.cl/SieteIQY/secure/carga_series_excel.aspx" post="fechaInicio=[&quot;añoInicial&quot;,&quot;Año inicial&quot;]&amp;fechaFin=[&quot;añoFinal&quot;,&quot;Año final&quot;]&amp;param=b2EwLjM3MW1sSUxHbUJIWSZSdi5fRXYkMmQtOHImMVh3S2ZrWSYuUFo3MWRMckIwY0UtWiQtVmRPNSZ6VyQkRlJINFYuMGcgUmMgeFJMT2dOIChkR2JfWiBId24gR8OzX0pYKSZ3dUpKUSNBa1lWUUtMMmd5Z19VRW9tUjNyOHRjZmtnU3hOdHJUSk4wNsOzcVVnIE4zN0ouZmNYVA==" htmlTables="1" htmlFormat="all"/>
     <parameters count="2">
       <parameter name="añoInicial" prompt="Año inicial"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="5">
   <si>
     <t>Tipos de cambio (pesos por dólar)</t>
   </si>
@@ -970,13 +970,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B831"/>
+  <dimension ref="A1:B837"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="4" topLeftCell="B831" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="4" topLeftCell="B837" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="A831" sqref="A831"/>
+      <selection pane="bottomRight" activeCell="A837" sqref="A837"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7629,6 +7629,54 @@
         <v>714.21</v>
       </c>
     </row>
+    <row r="832" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A832" s="2">
+        <v>44295</v>
+      </c>
+      <c r="B832" s="3">
+        <v>708.09</v>
+      </c>
+    </row>
+    <row r="833" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A833" s="2">
+        <v>44296</v>
+      </c>
+      <c r="B833" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="834" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A834" s="2">
+        <v>44297</v>
+      </c>
+      <c r="B834" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="835" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A835" s="2">
+        <v>44298</v>
+      </c>
+      <c r="B835" s="3">
+        <v>711.23</v>
+      </c>
+    </row>
+    <row r="836" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A836" s="2">
+        <v>44299</v>
+      </c>
+      <c r="B836" s="3">
+        <v>709.51</v>
+      </c>
+    </row>
+    <row r="837" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A837" s="2">
+        <v>44300</v>
+      </c>
+      <c r="B837" s="3">
+        <v>708.71</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:B1"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 04-15-2021 17-07-11
</commit_message>
<xml_diff>
--- a/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
+++ b/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID CL/IndicadoresEconomicos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="228" documentId="13_ncr:1_{C8B25996-B8C9-45E8-BF5F-0058EDDB5306}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{F74660F3-5A1B-4423-95AF-6684CAB52A85}"/>
+  <xr:revisionPtr revIDLastSave="230" documentId="13_ncr:1_{C8B25996-B8C9-45E8-BF5F-0058EDDB5306}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{A9B7367A-F547-48CC-A3B8-2A5359CBED15}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,8 +16,8 @@
     <sheet name="DOLAR_OBS_ADO" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">DOLAR_OBS_ADO!$A$3:$B$837</definedName>
-    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$837</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">DOLAR_OBS_ADO!$A$3:$B$838</definedName>
+    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$838</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -970,13 +970,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B837"/>
+  <dimension ref="A1:B838"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="4" topLeftCell="B837" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="4" topLeftCell="B838" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="A837" sqref="A837"/>
+      <selection pane="bottomRight" activeCell="A838" sqref="A838"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7677,6 +7677,14 @@
         <v>708.71</v>
       </c>
     </row>
+    <row r="838" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A838" s="2">
+        <v>44301</v>
+      </c>
+      <c r="B838" s="3">
+        <v>707.25</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:B1"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 04-16-2021 17-06-23
</commit_message>
<xml_diff>
--- a/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
+++ b/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID CL/IndicadoresEconomicos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="230" documentId="13_ncr:1_{C8B25996-B8C9-45E8-BF5F-0058EDDB5306}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{A9B7367A-F547-48CC-A3B8-2A5359CBED15}"/>
+  <xr:revisionPtr revIDLastSave="232" documentId="13_ncr:1_{C8B25996-B8C9-45E8-BF5F-0058EDDB5306}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{4E74BFC3-53D9-4457-AFFB-8F108A8B450F}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,8 +16,8 @@
     <sheet name="DOLAR_OBS_ADO" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">DOLAR_OBS_ADO!$A$3:$B$838</definedName>
-    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$838</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">DOLAR_OBS_ADO!$A$3:$B$839</definedName>
+    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$839</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -970,13 +970,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B838"/>
+  <dimension ref="A1:B839"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="4" topLeftCell="B838" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="4" topLeftCell="B839" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="A838" sqref="A838"/>
+      <selection pane="bottomRight" activeCell="A839" sqref="A839"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7685,6 +7685,14 @@
         <v>707.25</v>
       </c>
     </row>
+    <row r="839" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A839" s="2">
+        <v>44302</v>
+      </c>
+      <c r="B839" s="3">
+        <v>701.98</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:B1"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 04-17-2021 17-15-13
</commit_message>
<xml_diff>
--- a/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
+++ b/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID CL/IndicadoresEconomicos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="232" documentId="13_ncr:1_{C8B25996-B8C9-45E8-BF5F-0058EDDB5306}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{4E74BFC3-53D9-4457-AFFB-8F108A8B450F}"/>
+  <xr:revisionPtr revIDLastSave="234" documentId="13_ncr:1_{C8B25996-B8C9-45E8-BF5F-0058EDDB5306}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{346A1D8C-4DA4-4061-9CFE-117F703026B7}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,8 +16,8 @@
     <sheet name="DOLAR_OBS_ADO" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">DOLAR_OBS_ADO!$A$3:$B$839</definedName>
-    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$839</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">DOLAR_OBS_ADO!$A$3:$B$842</definedName>
+    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$842</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="5">
   <si>
     <t>Tipos de cambio (pesos por dólar)</t>
   </si>
@@ -970,13 +970,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B839"/>
+  <dimension ref="A1:B842"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="4" topLeftCell="B839" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="4" topLeftCell="B842" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="A839" sqref="A839"/>
+      <selection pane="bottomRight" activeCell="A842" sqref="A842"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7693,6 +7693,30 @@
         <v>701.98</v>
       </c>
     </row>
+    <row r="840" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A840" s="2">
+        <v>44303</v>
+      </c>
+      <c r="B840" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="841" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A841" s="2">
+        <v>44304</v>
+      </c>
+      <c r="B841" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="842" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A842" s="2">
+        <v>44305</v>
+      </c>
+      <c r="B842" s="3">
+        <v>701.55</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:B1"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 04-20-2021 17-09-46
</commit_message>
<xml_diff>
--- a/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
+++ b/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID CL/IndicadoresEconomicos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="234" documentId="13_ncr:1_{C8B25996-B8C9-45E8-BF5F-0058EDDB5306}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{346A1D8C-4DA4-4061-9CFE-117F703026B7}"/>
+  <xr:revisionPtr revIDLastSave="236" documentId="13_ncr:1_{C8B25996-B8C9-45E8-BF5F-0058EDDB5306}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{A1A9D894-0ED1-4497-8C4E-0D0197998E7A}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,8 +16,8 @@
     <sheet name="DOLAR_OBS_ADO" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">DOLAR_OBS_ADO!$A$3:$B$842</definedName>
-    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$842</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">DOLAR_OBS_ADO!$A$3:$B$843</definedName>
+    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$843</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -970,13 +970,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B842"/>
+  <dimension ref="A1:B843"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="4" topLeftCell="B842" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="4" topLeftCell="B843" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="A842" sqref="A842"/>
+      <selection pane="bottomRight" activeCell="A843" sqref="A843"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7717,6 +7717,14 @@
         <v>701.55</v>
       </c>
     </row>
+    <row r="843" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A843" s="2">
+        <v>44306</v>
+      </c>
+      <c r="B843" s="3">
+        <v>700.96</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:B1"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 04-21-2021 17-13-56
</commit_message>
<xml_diff>
--- a/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
+++ b/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID CL/IndicadoresEconomicos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="236" documentId="13_ncr:1_{C8B25996-B8C9-45E8-BF5F-0058EDDB5306}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{A1A9D894-0ED1-4497-8C4E-0D0197998E7A}"/>
+  <xr:revisionPtr revIDLastSave="238" documentId="13_ncr:1_{C8B25996-B8C9-45E8-BF5F-0058EDDB5306}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{4E8366BB-33BB-4E8A-8417-552FE0243CF1}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,8 +16,8 @@
     <sheet name="DOLAR_OBS_ADO" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">DOLAR_OBS_ADO!$A$3:$B$843</definedName>
-    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$843</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">DOLAR_OBS_ADO!$A$3:$B$844</definedName>
+    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$844</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -970,13 +970,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B843"/>
+  <dimension ref="A1:B844"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="4" topLeftCell="B843" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="4" topLeftCell="B844" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="A843" sqref="A843"/>
+      <selection pane="bottomRight" activeCell="A844" sqref="A844"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7725,6 +7725,14 @@
         <v>700.96</v>
       </c>
     </row>
+    <row r="844" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A844" s="2">
+        <v>44307</v>
+      </c>
+      <c r="B844" s="3">
+        <v>697.19</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:B1"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 04-22-2021 17-07-02
</commit_message>
<xml_diff>
--- a/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
+++ b/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID CL/IndicadoresEconomicos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="238" documentId="13_ncr:1_{C8B25996-B8C9-45E8-BF5F-0058EDDB5306}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{4E8366BB-33BB-4E8A-8417-552FE0243CF1}"/>
+  <xr:revisionPtr revIDLastSave="240" documentId="13_ncr:1_{C8B25996-B8C9-45E8-BF5F-0058EDDB5306}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{6E8D19DB-A3EF-488C-A456-8334BDAAD0EA}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,8 +16,8 @@
     <sheet name="DOLAR_OBS_ADO" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">DOLAR_OBS_ADO!$A$3:$B$844</definedName>
-    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$844</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">DOLAR_OBS_ADO!$A$3:$B$845</definedName>
+    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$845</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -970,13 +970,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B844"/>
+  <dimension ref="A1:B845"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="4" topLeftCell="B844" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="4" topLeftCell="B845" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="A844" sqref="A844"/>
+      <selection pane="bottomRight" activeCell="A845" sqref="A845"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7733,6 +7733,14 @@
         <v>697.19</v>
       </c>
     </row>
+    <row r="845" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A845" s="2">
+        <v>44308</v>
+      </c>
+      <c r="B845" s="3">
+        <v>696.8</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:B1"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 04-23-2021 17-09-05
</commit_message>
<xml_diff>
--- a/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
+++ b/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID CL/IndicadoresEconomicos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="240" documentId="13_ncr:1_{C8B25996-B8C9-45E8-BF5F-0058EDDB5306}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{6E8D19DB-A3EF-488C-A456-8334BDAAD0EA}"/>
+  <xr:revisionPtr revIDLastSave="242" documentId="13_ncr:1_{C8B25996-B8C9-45E8-BF5F-0058EDDB5306}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{235B0AFF-B072-44F2-B68A-2500B50A5B9A}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,8 +16,8 @@
     <sheet name="DOLAR_OBS_ADO" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">DOLAR_OBS_ADO!$A$3:$B$845</definedName>
-    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$845</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">DOLAR_OBS_ADO!$A$3:$B$846</definedName>
+    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$846</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -970,13 +970,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B845"/>
+  <dimension ref="A1:B846"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="4" topLeftCell="B845" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="4" topLeftCell="B846" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="A845" sqref="A845"/>
+      <selection pane="bottomRight" activeCell="A846" sqref="A846"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7741,6 +7741,14 @@
         <v>696.8</v>
       </c>
     </row>
+    <row r="846" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A846" s="2">
+        <v>44309</v>
+      </c>
+      <c r="B846" s="3">
+        <v>705.41</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:B1"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 04-24-2021 17-14-48
</commit_message>
<xml_diff>
--- a/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
+++ b/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID CL/IndicadoresEconomicos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="242" documentId="13_ncr:1_{C8B25996-B8C9-45E8-BF5F-0058EDDB5306}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{235B0AFF-B072-44F2-B68A-2500B50A5B9A}"/>
+  <xr:revisionPtr revIDLastSave="246" documentId="13_ncr:1_{C8B25996-B8C9-45E8-BF5F-0058EDDB5306}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{425C3755-5DD8-48B9-BE88-D7AF1F06952B}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,8 +16,8 @@
     <sheet name="DOLAR_OBS_ADO" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">DOLAR_OBS_ADO!$A$3:$B$846</definedName>
-    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$846</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">DOLAR_OBS_ADO!$A$3:$B$849</definedName>
+    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$849</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="5">
   <si>
     <t>Tipos de cambio (pesos por dólar)</t>
   </si>
@@ -970,13 +970,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B846"/>
+  <dimension ref="A1:B849"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="4" topLeftCell="B846" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="4" topLeftCell="B849" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="A846" sqref="A846"/>
+      <selection pane="bottomRight" activeCell="A849" sqref="A849"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7749,6 +7749,30 @@
         <v>705.41</v>
       </c>
     </row>
+    <row r="847" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A847" s="2">
+        <v>44310</v>
+      </c>
+      <c r="B847" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="848" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A848" s="2">
+        <v>44311</v>
+      </c>
+      <c r="B848" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="849" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A849" s="2">
+        <v>44312</v>
+      </c>
+      <c r="B849" s="3">
+        <v>712.54</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:B1"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 04-27-2021 17-14-55
</commit_message>
<xml_diff>
--- a/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
+++ b/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID CL/IndicadoresEconomicos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="246" documentId="13_ncr:1_{C8B25996-B8C9-45E8-BF5F-0058EDDB5306}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{425C3755-5DD8-48B9-BE88-D7AF1F06952B}"/>
+  <xr:revisionPtr revIDLastSave="248" documentId="13_ncr:1_{C8B25996-B8C9-45E8-BF5F-0058EDDB5306}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{998CD77B-8F97-4172-A4E2-01A20D9E98FB}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,8 +16,8 @@
     <sheet name="DOLAR_OBS_ADO" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">DOLAR_OBS_ADO!$A$3:$B$849</definedName>
-    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$849</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">DOLAR_OBS_ADO!$A$3:$B$850</definedName>
+    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$850</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -970,13 +970,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B849"/>
+  <dimension ref="A1:B850"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="4" topLeftCell="B849" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="4" topLeftCell="B850" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="A849" sqref="A849"/>
+      <selection pane="bottomRight" activeCell="A850" sqref="A850"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7773,6 +7773,14 @@
         <v>712.54</v>
       </c>
     </row>
+    <row r="850" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A850" s="2">
+        <v>44313</v>
+      </c>
+      <c r="B850" s="3">
+        <v>707.05</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:B1"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 04-28-2021 17-14-39
</commit_message>
<xml_diff>
--- a/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
+++ b/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID CL/IndicadoresEconomicos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="248" documentId="13_ncr:1_{C8B25996-B8C9-45E8-BF5F-0058EDDB5306}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{998CD77B-8F97-4172-A4E2-01A20D9E98FB}"/>
+  <xr:revisionPtr revIDLastSave="250" documentId="13_ncr:1_{C8B25996-B8C9-45E8-BF5F-0058EDDB5306}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{7F6968EB-A847-4A39-B791-2BB95A6D7F0B}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,8 +16,8 @@
     <sheet name="DOLAR_OBS_ADO" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">DOLAR_OBS_ADO!$A$3:$B$850</definedName>
-    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$850</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">DOLAR_OBS_ADO!$A$3:$B$851</definedName>
+    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$851</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -970,13 +970,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B850"/>
+  <dimension ref="A1:B851"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="4" topLeftCell="B850" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="4" topLeftCell="B851" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="A850" sqref="A850"/>
+      <selection pane="bottomRight" activeCell="A851" sqref="A851"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7781,6 +7781,14 @@
         <v>707.05</v>
       </c>
     </row>
+    <row r="851" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A851" s="2">
+        <v>44314</v>
+      </c>
+      <c r="B851" s="3">
+        <v>702.02</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:B1"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 04-29-2021 17-11-10
</commit_message>
<xml_diff>
--- a/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
+++ b/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID CL/IndicadoresEconomicos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="250" documentId="13_ncr:1_{C8B25996-B8C9-45E8-BF5F-0058EDDB5306}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{7F6968EB-A847-4A39-B791-2BB95A6D7F0B}"/>
+  <xr:revisionPtr revIDLastSave="252" documentId="13_ncr:1_{C8B25996-B8C9-45E8-BF5F-0058EDDB5306}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{2C989CD4-3F68-4FA2-AD66-9E96406B51B7}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,8 +16,8 @@
     <sheet name="DOLAR_OBS_ADO" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">DOLAR_OBS_ADO!$A$3:$B$851</definedName>
-    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$851</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">DOLAR_OBS_ADO!$A$3:$B$852</definedName>
+    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$852</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -970,13 +970,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B851"/>
+  <dimension ref="A1:B852"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="4" topLeftCell="B851" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="4" topLeftCell="B852" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="A851" sqref="A851"/>
+      <selection pane="bottomRight" activeCell="A852" sqref="A852"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7789,6 +7789,14 @@
         <v>702.02</v>
       </c>
     </row>
+    <row r="852" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A852" s="2">
+        <v>44315</v>
+      </c>
+      <c r="B852" s="3">
+        <v>700.15</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:B1"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 04-30-2021 17-10-05
</commit_message>
<xml_diff>
--- a/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
+++ b/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID CL/IndicadoresEconomicos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="252" documentId="13_ncr:1_{C8B25996-B8C9-45E8-BF5F-0058EDDB5306}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{2C989CD4-3F68-4FA2-AD66-9E96406B51B7}"/>
+  <xr:revisionPtr revIDLastSave="256" documentId="13_ncr:1_{C8B25996-B8C9-45E8-BF5F-0058EDDB5306}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{15317501-D7C9-49C7-A4B2-9AA4F00BB426}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,8 +16,8 @@
     <sheet name="DOLAR_OBS_ADO" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">DOLAR_OBS_ADO!$A$3:$B$852</definedName>
-    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$852</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">DOLAR_OBS_ADO!$A$3:$B$853</definedName>
+    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$853</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -970,13 +970,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B852"/>
+  <dimension ref="A1:B853"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="4" topLeftCell="B852" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="4" topLeftCell="B853" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="A852" sqref="A852"/>
+      <selection pane="bottomRight" activeCell="A853" sqref="A853"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7797,6 +7797,14 @@
         <v>700.15</v>
       </c>
     </row>
+    <row r="853" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A853" s="2">
+        <v>44316</v>
+      </c>
+      <c r="B853" s="3">
+        <v>705.09</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:B1"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 05-01-2021 17-08-20
</commit_message>
<xml_diff>
--- a/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
+++ b/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID CL/IndicadoresEconomicos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="256" documentId="13_ncr:1_{C8B25996-B8C9-45E8-BF5F-0058EDDB5306}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{15317501-D7C9-49C7-A4B2-9AA4F00BB426}"/>
+  <xr:revisionPtr revIDLastSave="260" documentId="13_ncr:1_{C8B25996-B8C9-45E8-BF5F-0058EDDB5306}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{312A2F9A-834F-4938-B660-A729B1704250}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,8 +16,8 @@
     <sheet name="DOLAR_OBS_ADO" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">DOLAR_OBS_ADO!$A$3:$B$853</definedName>
-    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$853</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">DOLAR_OBS_ADO!$A$3:$B$856</definedName>
+    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$856</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="5">
   <si>
     <t>Tipos de cambio (pesos por dólar)</t>
   </si>
@@ -970,13 +970,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B853"/>
+  <dimension ref="A1:B856"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="4" topLeftCell="B853" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="4" topLeftCell="B856" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="A853" sqref="A853"/>
+      <selection pane="bottomRight" activeCell="A856" sqref="A856"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7805,6 +7805,30 @@
         <v>705.09</v>
       </c>
     </row>
+    <row r="854" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A854" s="2">
+        <v>44317</v>
+      </c>
+      <c r="B854" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="855" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A855" s="2">
+        <v>44318</v>
+      </c>
+      <c r="B855" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="856" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A856" s="2">
+        <v>44319</v>
+      </c>
+      <c r="B856" s="3">
+        <v>711.06</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:B1"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 05-04-2021 17-15-32
</commit_message>
<xml_diff>
--- a/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
+++ b/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID CL/IndicadoresEconomicos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="260" documentId="13_ncr:1_{C8B25996-B8C9-45E8-BF5F-0058EDDB5306}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{312A2F9A-834F-4938-B660-A729B1704250}"/>
+  <xr:revisionPtr revIDLastSave="262" documentId="13_ncr:1_{C8B25996-B8C9-45E8-BF5F-0058EDDB5306}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{0C941B95-A53E-41BC-93D4-DD9080035F49}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,10 +16,10 @@
     <sheet name="DOLAR_OBS_ADO" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">DOLAR_OBS_ADO!$A$3:$B$856</definedName>
-    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$856</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">DOLAR_OBS_ADO!$A$3:$B$857</definedName>
+    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$857</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" iterate="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -970,13 +970,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B856"/>
+  <dimension ref="A1:B857"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="4" topLeftCell="B856" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="4" topLeftCell="B857" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="A856" sqref="A856"/>
+      <selection pane="bottomRight" activeCell="A857" sqref="A857"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7829,6 +7829,14 @@
         <v>711.06</v>
       </c>
     </row>
+    <row r="857" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A857" s="2">
+        <v>44320</v>
+      </c>
+      <c r="B857" s="3">
+        <v>706.29</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:B1"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 05-05-2021 17-16-57
</commit_message>
<xml_diff>
--- a/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
+++ b/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID CL/IndicadoresEconomicos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="262" documentId="13_ncr:1_{C8B25996-B8C9-45E8-BF5F-0058EDDB5306}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{0C941B95-A53E-41BC-93D4-DD9080035F49}"/>
+  <xr:revisionPtr revIDLastSave="266" documentId="13_ncr:1_{C8B25996-B8C9-45E8-BF5F-0058EDDB5306}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{1EB97B61-0D19-458C-A650-BFDAD08BDC36}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,8 +16,8 @@
     <sheet name="DOLAR_OBS_ADO" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">DOLAR_OBS_ADO!$A$3:$B$857</definedName>
-    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$857</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">DOLAR_OBS_ADO!$A$3:$B$858</definedName>
+    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$858</definedName>
   </definedNames>
   <calcPr calcId="191029" iterate="1"/>
   <extLst>
@@ -970,13 +970,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B857"/>
+  <dimension ref="A1:B858"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="4" topLeftCell="B857" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="4" topLeftCell="B858" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="A857" sqref="A857"/>
+      <selection pane="bottomRight" activeCell="A858" sqref="A858"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7837,6 +7837,14 @@
         <v>706.29</v>
       </c>
     </row>
+    <row r="858" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A858" s="2">
+        <v>44321</v>
+      </c>
+      <c r="B858" s="3">
+        <v>705.25</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:B1"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 05-06-2021 17-06-57
</commit_message>
<xml_diff>
--- a/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
+++ b/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID CL/IndicadoresEconomicos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="266" documentId="13_ncr:1_{C8B25996-B8C9-45E8-BF5F-0058EDDB5306}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{1EB97B61-0D19-458C-A650-BFDAD08BDC36}"/>
+  <xr:revisionPtr revIDLastSave="268" documentId="13_ncr:1_{C8B25996-B8C9-45E8-BF5F-0058EDDB5306}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{F4D92471-B344-4FA7-8BDF-28FCC1E54B5F}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,8 +16,8 @@
     <sheet name="DOLAR_OBS_ADO" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">DOLAR_OBS_ADO!$A$3:$B$858</definedName>
-    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$858</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">DOLAR_OBS_ADO!$A$3:$B$859</definedName>
+    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$859</definedName>
   </definedNames>
   <calcPr calcId="191029" iterate="1"/>
   <extLst>
@@ -970,13 +970,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B858"/>
+  <dimension ref="A1:B859"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="4" topLeftCell="B858" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="4" topLeftCell="B859" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="A858" sqref="A858"/>
+      <selection pane="bottomRight" activeCell="A859" sqref="A859"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7845,6 +7845,14 @@
         <v>705.25</v>
       </c>
     </row>
+    <row r="859" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A859" s="2">
+        <v>44322</v>
+      </c>
+      <c r="B859" s="3">
+        <v>703.09</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:B1"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 05-07-2021 17-12-16
</commit_message>
<xml_diff>
--- a/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
+++ b/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID CL/IndicadoresEconomicos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="268" documentId="13_ncr:1_{C8B25996-B8C9-45E8-BF5F-0058EDDB5306}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{F4D92471-B344-4FA7-8BDF-28FCC1E54B5F}"/>
+  <xr:revisionPtr revIDLastSave="270" documentId="13_ncr:1_{C8B25996-B8C9-45E8-BF5F-0058EDDB5306}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{AB5F0852-6A38-40DD-B7C2-E6485A78573A}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,8 +16,8 @@
     <sheet name="DOLAR_OBS_ADO" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">DOLAR_OBS_ADO!$A$3:$B$859</definedName>
-    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$859</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">DOLAR_OBS_ADO!$A$3:$B$860</definedName>
+    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$860</definedName>
   </definedNames>
   <calcPr calcId="191029" iterate="1"/>
   <extLst>
@@ -970,13 +970,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B859"/>
+  <dimension ref="A1:B860"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="4" topLeftCell="B859" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="4" topLeftCell="B860" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="A859" sqref="A859"/>
+      <selection pane="bottomRight" activeCell="A860" sqref="A860"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7853,6 +7853,14 @@
         <v>703.09</v>
       </c>
     </row>
+    <row r="860" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A860" s="2">
+        <v>44323</v>
+      </c>
+      <c r="B860" s="3">
+        <v>701.27</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:B1"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 05-08-2021 17-12-54
</commit_message>
<xml_diff>
--- a/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
+++ b/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID CL/IndicadoresEconomicos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="270" documentId="13_ncr:1_{C8B25996-B8C9-45E8-BF5F-0058EDDB5306}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{AB5F0852-6A38-40DD-B7C2-E6485A78573A}"/>
+  <xr:revisionPtr revIDLastSave="272" documentId="13_ncr:1_{C8B25996-B8C9-45E8-BF5F-0058EDDB5306}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{C0079648-D401-4433-9008-F525B8A43B88}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,8 +16,8 @@
     <sheet name="DOLAR_OBS_ADO" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">DOLAR_OBS_ADO!$A$3:$B$860</definedName>
-    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$860</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">DOLAR_OBS_ADO!$A$3:$B$863</definedName>
+    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$863</definedName>
   </definedNames>
   <calcPr calcId="191029" iterate="1"/>
   <extLst>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="5">
   <si>
     <t>Tipos de cambio (pesos por dólar)</t>
   </si>
@@ -970,13 +970,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B860"/>
+  <dimension ref="A1:B863"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="4" topLeftCell="B860" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="4" topLeftCell="B863" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="A860" sqref="A860"/>
+      <selection pane="bottomRight" activeCell="A863" sqref="A863"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7861,6 +7861,30 @@
         <v>701.27</v>
       </c>
     </row>
+    <row r="861" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A861" s="2">
+        <v>44324</v>
+      </c>
+      <c r="B861" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="862" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A862" s="2">
+        <v>44325</v>
+      </c>
+      <c r="B862" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="863" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A863" s="2">
+        <v>44326</v>
+      </c>
+      <c r="B863" s="3">
+        <v>694.47</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:B1"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 05-11-2021 17-13-42
</commit_message>
<xml_diff>
--- a/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
+++ b/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID CL/IndicadoresEconomicos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="272" documentId="13_ncr:1_{C8B25996-B8C9-45E8-BF5F-0058EDDB5306}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{C0079648-D401-4433-9008-F525B8A43B88}"/>
+  <xr:revisionPtr revIDLastSave="274" documentId="13_ncr:1_{C8B25996-B8C9-45E8-BF5F-0058EDDB5306}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{704E1046-6BB2-4E66-A6A8-9FF9932629E2}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,8 +16,8 @@
     <sheet name="DOLAR_OBS_ADO" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">DOLAR_OBS_ADO!$A$3:$B$863</definedName>
-    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$863</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">DOLAR_OBS_ADO!$A$3:$B$864</definedName>
+    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$864</definedName>
   </definedNames>
   <calcPr calcId="191029" iterate="1"/>
   <extLst>
@@ -970,13 +970,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B863"/>
+  <dimension ref="A1:B864"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="4" topLeftCell="B863" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="4" topLeftCell="B864" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="A863" sqref="A863"/>
+      <selection pane="bottomRight" activeCell="A864" sqref="A864"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7885,6 +7885,14 @@
         <v>694.47</v>
       </c>
     </row>
+    <row r="864" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A864" s="2">
+        <v>44327</v>
+      </c>
+      <c r="B864" s="3">
+        <v>693.74</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:B1"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 05-12-2021 17-12-09
</commit_message>
<xml_diff>
--- a/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
+++ b/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID CL/IndicadoresEconomicos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="274" documentId="13_ncr:1_{C8B25996-B8C9-45E8-BF5F-0058EDDB5306}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{704E1046-6BB2-4E66-A6A8-9FF9932629E2}"/>
+  <xr:revisionPtr revIDLastSave="276" documentId="13_ncr:1_{C8B25996-B8C9-45E8-BF5F-0058EDDB5306}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{7F9961F4-3145-4C55-9A60-F88F61FD53FE}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,8 +16,8 @@
     <sheet name="DOLAR_OBS_ADO" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">DOLAR_OBS_ADO!$A$3:$B$864</definedName>
-    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$864</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">DOLAR_OBS_ADO!$A$3:$B$865</definedName>
+    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$865</definedName>
   </definedNames>
   <calcPr calcId="191029" iterate="1"/>
   <extLst>
@@ -970,13 +970,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B864"/>
+  <dimension ref="A1:B865"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="4" topLeftCell="B864" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="4" topLeftCell="B865" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="A864" sqref="A864"/>
+      <selection pane="bottomRight" activeCell="A865" sqref="A865"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7893,6 +7893,14 @@
         <v>693.74</v>
       </c>
     </row>
+    <row r="865" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A865" s="2">
+        <v>44328</v>
+      </c>
+      <c r="B865" s="3">
+        <v>700.04</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:B1"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 05-13-2021 17-08-04
</commit_message>
<xml_diff>
--- a/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
+++ b/datacovidChile/IndicadoresEconomicos/DOLAR_OBS_ADO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID CL/IndicadoresEconomicos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="276" documentId="13_ncr:1_{C8B25996-B8C9-45E8-BF5F-0058EDDB5306}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{7F9961F4-3145-4C55-9A60-F88F61FD53FE}"/>
+  <xr:revisionPtr revIDLastSave="278" documentId="13_ncr:1_{C8B25996-B8C9-45E8-BF5F-0058EDDB5306}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{CA6F82BC-F7AF-4384-8CE4-B781A949CF4B}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,8 +16,8 @@
     <sheet name="DOLAR_OBS_ADO" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">DOLAR_OBS_ADO!$A$3:$B$865</definedName>
-    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$865</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">DOLAR_OBS_ADO!$A$3:$B$866</definedName>
+    <definedName name="DOLAR_OBS_ADO" localSheetId="0">DOLAR_OBS_ADO!$A$1:$B$866</definedName>
   </definedNames>
   <calcPr calcId="191029" iterate="1"/>
   <extLst>
@@ -970,13 +970,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B865"/>
+  <dimension ref="A1:B866"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="4" topLeftCell="B865" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="4" topLeftCell="B866" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="A865" sqref="A865"/>
+      <selection pane="bottomRight" activeCell="A866" sqref="A866"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7901,6 +7901,14 @@
         <v>700.04</v>
       </c>
     </row>
+    <row r="866" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A866" s="2">
+        <v>44329</v>
+      </c>
+      <c r="B866" s="3">
+        <v>707.19</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:B1"/>

</xml_diff>